<commit_message>
Tweaks to V0.2 schematic and layout from notes.
</commit_message>
<xml_diff>
--- a/Electronic Design/Core 64 Pin Usage Mapping.xlsx
+++ b/Electronic Design/Core 64 Pin Usage Mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ageppert/OneDrive/00_MBP2011-Documents/Electronics/Core 64 Interactive Badge/Core-64-Interactive-Core-Memory-Badge/Electronic Design/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1c02d23ac1278198/00_MBP2011-Documents/Electronics/Core 64 Interactive Badge/Core-64-Interactive-Core-Memory-Badge/Electronic Design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="114_{C854064A-3C16-0445-B75C-033646BE2CC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="114_{C854064A-3C16-0445-B75C-033646BE2CC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E534EED7-6A1A-8943-A8CC-679BDFB4185B}"/>
   <bookViews>
-    <workbookView xWindow="-51200" yWindow="-10340" windowWidth="51200" windowHeight="28340" activeTab="2" xr2:uid="{A4752792-CA31-B046-B883-84F8D68A57EC}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19600" activeTab="2" xr2:uid="{A4752792-CA31-B046-B883-84F8D68A57EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Reference Pinouts" sheetId="3" r:id="rId1"/>
@@ -1001,6 +1001,61 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>308428</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>99785</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>81643</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>90715</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Straight Connector 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{03B08599-0987-A34B-8D01-D5FCC0E48B33}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10078357" y="4726214"/>
+          <a:ext cx="290286" cy="390072"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1698,8 +1753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7B47D1C-78B7-5A42-A348-9E367CC3D141}">
   <dimension ref="A1:P50"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A14" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2475,7 +2530,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CBC2977-27CE-C64F-BE79-A69FB2535F84}">
   <dimension ref="A1:Z53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="U27" sqref="U27"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Teensy LC and 3.2 updates
</commit_message>
<xml_diff>
--- a/Electronic Design/Core 64 Pin Usage Mapping.xlsx
+++ b/Electronic Design/Core 64 Pin Usage Mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1c02d23ac1278198/00_MBP2011-Documents/Electronics/Core 64 Interactive Badge/Core-64-Interactive-Core-Memory-Badge/Electronic Design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="114_{C854064A-3C16-0445-B75C-033646BE2CC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E534EED7-6A1A-8943-A8CC-679BDFB4185B}"/>
+  <xr:revisionPtr revIDLastSave="74" documentId="114_{C854064A-3C16-0445-B75C-033646BE2CC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C8F2BB7A-3D4B-894A-AEF0-0799CF73EA1D}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19600" activeTab="2" xr2:uid="{A4752792-CA31-B046-B883-84F8D68A57EC}"/>
+    <workbookView xWindow="-35200" yWindow="-10340" windowWidth="35200" windowHeight="28340" activeTab="2" xr2:uid="{A4752792-CA31-B046-B883-84F8D68A57EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Reference Pinouts" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="138">
   <si>
     <t>Custom</t>
   </si>
@@ -235,9 +235,6 @@
     <t>3.3V Regulated VOUT to AREF and low power stuff</t>
   </si>
   <si>
-    <t>Pull high to avoid acceptable programming</t>
-  </si>
-  <si>
     <t>VUSB</t>
   </si>
   <si>
@@ -388,42 +385,6 @@
     <t>(Or use 2x 16 GPIO I2C expander http://ww1.microchip.com/downloads/en/DeviceDoc/20090C.pdf)</t>
   </si>
   <si>
-    <t>Matrix Drive 1 - Q1P (XB0-3)</t>
-  </si>
-  <si>
-    <t>Matrix Drive 2 - Q1N (XB0-3)</t>
-  </si>
-  <si>
-    <t>Matrix Drive 3 - Q2P (XB4-7)</t>
-  </si>
-  <si>
-    <t>Matrix Drive 4 - Q2N (XB4-7)</t>
-  </si>
-  <si>
-    <t>Matrix Drive 5 - Q3P (XT0,4)</t>
-  </si>
-  <si>
-    <t>Matrix Drive 9 - Q5P (XT2,6)</t>
-  </si>
-  <si>
-    <t>Matrix Drive 10 - Q5N (XT2,6)</t>
-  </si>
-  <si>
-    <t>Matrix Drive 8 - Q4N (XT1,5)</t>
-  </si>
-  <si>
-    <t>Matrix Drive 7 - Q4P (XT1,5)</t>
-  </si>
-  <si>
-    <t>Matrix Drive 6 - Q3N (XT0,4)</t>
-  </si>
-  <si>
-    <t>Matrix Drive 11 - Q6P (XT3,7)</t>
-  </si>
-  <si>
-    <t>Matrix Drive 12 - Q6N (XT3,7)</t>
-  </si>
-  <si>
     <t>https://forum.pjrc.com/threads/55568-Teensy-3-2-3-5-pin-compatibility</t>
   </si>
   <si>
@@ -431,13 +392,70 @@
   </si>
   <si>
     <t>https://docs.google.com/spreadsheets/d/1LSi0c17iqtvpKuNSYksMG306_FpWdJcniSRR6aGNNYQ/edit#gid=1683806103</t>
+  </si>
+  <si>
+    <t>Custom 1</t>
+  </si>
+  <si>
+    <t>Custom 2</t>
+  </si>
+  <si>
+    <t>TEENSY_GND</t>
+  </si>
+  <si>
+    <t>TEENSY_VUSB to Core 64 Power Switch</t>
+  </si>
+  <si>
+    <t>supplied from TEENSY_3V3</t>
+  </si>
+  <si>
+    <t>TEENSY_3V3 from Teensy 3.3V aka 3V3_100mA</t>
+  </si>
+  <si>
+    <t>TEENSY_VIN from +VSW</t>
+  </si>
+  <si>
+    <t>OLED Debug</t>
+  </si>
+  <si>
+    <t>IO Expanders 27 of 32 (Core drive, enable, sense/reset, digital halls)</t>
+  </si>
+  <si>
+    <t>Custom 3</t>
+  </si>
+  <si>
+    <t>Custom 4</t>
+  </si>
+  <si>
+    <t>Custom 5</t>
+  </si>
+  <si>
+    <t>I2C Hall Sensors</t>
+  </si>
+  <si>
+    <t>SAO 1,2,3</t>
+  </si>
+  <si>
+    <t>Expansion Header</t>
+  </si>
+  <si>
+    <t>Heartbeat LED - Built-in - user configurable</t>
+  </si>
+  <si>
+    <t>Pull high to avoid accidental programming</t>
+  </si>
+  <si>
+    <t>LED Array - bit-banged</t>
+  </si>
+  <si>
+    <t>VBAT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -511,8 +529,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -540,6 +565,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA845F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -637,7 +668,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -708,6 +739,13 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -715,6 +753,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFA845F2"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1363,8 +1406,8 @@
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>72571</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>3147786</xdr:colOff>
       <xdr:row>54</xdr:row>
       <xdr:rowOff>47267</xdr:rowOff>
     </xdr:to>
@@ -1719,24 +1762,24 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="23" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="23" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -1753,8 +1796,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7B47D1C-78B7-5A42-A348-9E367CC3D141}">
   <dimension ref="A1:P50"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1779,12 +1822,12 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H2" s="19" t="s">
         <v>60</v>
@@ -1883,7 +1926,7 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B6" s="15" t="s">
         <v>26</v>
@@ -1911,7 +1954,7 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F7" s="15">
         <v>2</v>
@@ -1944,7 +1987,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B8" s="15" t="s">
         <v>26</v>
@@ -1978,12 +2021,12 @@
         <v>26</v>
       </c>
       <c r="P8" s="16" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B9" s="15" t="s">
         <v>26</v>
@@ -2011,12 +2054,12 @@
         <v>19</v>
       </c>
       <c r="P9" s="20" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F10" s="15">
         <v>5</v>
@@ -2041,12 +2084,12 @@
         <v>2</v>
       </c>
       <c r="P10" s="20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C11" s="15" t="s">
         <v>2</v>
@@ -2082,7 +2125,7 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E12" s="15" t="s">
         <v>17</v>
@@ -2115,7 +2158,7 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E13" s="15" t="s">
         <v>16</v>
@@ -2143,12 +2186,12 @@
         <v>26</v>
       </c>
       <c r="P13" s="20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C14" s="15" t="s">
         <v>2</v>
@@ -2179,12 +2222,12 @@
         <v>26</v>
       </c>
       <c r="P14" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C15" s="15" t="s">
         <v>2</v>
@@ -2215,12 +2258,12 @@
         <v>26</v>
       </c>
       <c r="P15" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D16" s="15" t="s">
         <v>23</v>
@@ -2242,12 +2285,12 @@
         <v>36</v>
       </c>
       <c r="P16" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" s="16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D17" s="15" t="s">
         <v>24</v>
@@ -2269,7 +2312,7 @@
         <v>54</v>
       </c>
       <c r="P17" s="16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
@@ -2334,7 +2377,7 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F21" s="15" t="s">
         <v>51</v>
@@ -2358,7 +2401,7 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>66</v>
+        <v>135</v>
       </c>
       <c r="F22" s="15" t="s">
         <v>51</v>
@@ -2368,11 +2411,11 @@
       </c>
       <c r="H22" s="7"/>
       <c r="I22" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J22" s="7"/>
       <c r="P22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -2508,12 +2551,12 @@
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -2528,10 +2571,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CBC2977-27CE-C64F-BE79-A69FB2535F84}">
-  <dimension ref="A1:Z53"/>
+  <dimension ref="A1:AC53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="U27" sqref="U27"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2551,18 +2594,21 @@
     <col min="13" max="13" width="6.6640625" style="15" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="5.6640625" style="15" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="10.83203125" style="15"/>
-    <col min="16" max="16" width="29.5" customWidth="1"/>
-    <col min="19" max="20" width="10.83203125" style="15"/>
+    <col min="16" max="16" width="57" customWidth="1"/>
+    <col min="17" max="17" width="12.1640625" customWidth="1"/>
+    <col min="18" max="18" width="14" customWidth="1"/>
+    <col min="20" max="20" width="17.33203125" customWidth="1"/>
+    <col min="22" max="23" width="10.83203125" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G2" s="8"/>
       <c r="H2" s="24" t="s">
@@ -2570,7 +2616,7 @@
       </c>
       <c r="I2" s="8"/>
     </row>
-    <row r="3" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -2614,12 +2660,24 @@
         <v>1</v>
       </c>
       <c r="P3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>52</v>
+        <v>119</v>
+      </c>
+      <c r="Q3" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="R3" t="s">
+        <v>128</v>
+      </c>
+      <c r="S3" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="T3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A4" s="30" t="s">
+        <v>121</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>4</v>
@@ -2628,24 +2686,22 @@
         <v>48</v>
       </c>
       <c r="J4" s="7"/>
-      <c r="P4" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="S4" s="29" t="s">
-        <v>108</v>
-      </c>
-      <c r="T4" s="29"/>
-      <c r="U4" s="29"/>
-      <c r="V4" s="29"/>
+      <c r="P4" s="30" t="s">
+        <v>125</v>
+      </c>
+      <c r="V4" s="29" t="s">
+        <v>107</v>
+      </c>
       <c r="W4" s="29"/>
       <c r="X4" s="29"/>
       <c r="Y4" s="29"/>
-      <c r="Z4" s="26"/>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A5" s="16" t="s">
-        <v>61</v>
-      </c>
+      <c r="Z4" s="29"/>
+      <c r="AA4" s="29"/>
+      <c r="AB4" s="29"/>
+      <c r="AC4" s="26"/>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A5" s="16"/>
       <c r="B5" s="15" t="s">
         <v>26</v>
       </c>
@@ -2666,22 +2722,20 @@
         <v>4</v>
       </c>
       <c r="J5" s="7"/>
-      <c r="P5" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="S5" s="25"/>
-      <c r="T5" s="25"/>
-      <c r="U5" s="26"/>
-      <c r="V5" s="26"/>
-      <c r="W5" s="26"/>
+      <c r="P5" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="V5" s="25"/>
+      <c r="W5" s="25"/>
       <c r="X5" s="26"/>
       <c r="Y5" s="26"/>
       <c r="Z5" s="26"/>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A6" s="16" t="s">
-        <v>117</v>
-      </c>
+      <c r="AA5" s="26"/>
+      <c r="AB5" s="26"/>
+      <c r="AC5" s="26"/>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A6" s="16"/>
       <c r="B6" s="15" t="s">
         <v>26</v>
       </c>
@@ -2702,22 +2756,20 @@
         <v>49</v>
       </c>
       <c r="J6" s="7"/>
-      <c r="P6" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="S6" s="25"/>
-      <c r="T6" s="25"/>
-      <c r="U6" s="26"/>
-      <c r="V6" s="26"/>
-      <c r="W6" s="26"/>
+      <c r="P6" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="V6" s="25"/>
+      <c r="W6" s="25"/>
       <c r="X6" s="26"/>
       <c r="Y6" s="26"/>
       <c r="Z6" s="26"/>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A7" s="16" t="s">
-        <v>118</v>
-      </c>
+      <c r="AA6" s="26"/>
+      <c r="AB6" s="26"/>
+      <c r="AC6" s="26"/>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A7" s="16"/>
       <c r="F7" s="15">
         <v>2</v>
       </c>
@@ -2734,38 +2786,25 @@
       <c r="K7" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="L7" s="15" t="s">
-        <v>39</v>
-      </c>
       <c r="N7" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="O7" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="P7" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="S7" s="25">
+      <c r="P7" s="20"/>
+      <c r="V7" s="25">
         <v>9</v>
       </c>
-      <c r="T7" s="25"/>
-      <c r="U7" s="26" t="s">
-        <v>101</v>
-      </c>
-      <c r="V7" s="26"/>
-      <c r="W7" s="26"/>
-      <c r="X7" s="26"/>
+      <c r="W7" s="25"/>
+      <c r="X7" s="26" t="s">
+        <v>100</v>
+      </c>
       <c r="Y7" s="26"/>
       <c r="Z7" s="26"/>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A8" s="16" t="s">
-        <v>119</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>26</v>
-      </c>
+      <c r="AA7" s="26"/>
+      <c r="AB7" s="26"/>
+      <c r="AC7" s="26"/>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A8" s="16"/>
       <c r="C8" s="15" t="s">
         <v>2</v>
       </c>
@@ -2785,36 +2824,23 @@
       <c r="K8" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="L8" s="15" t="s">
-        <v>40</v>
-      </c>
       <c r="N8" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="O8" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="P8" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="S8" s="25"/>
-      <c r="T8" s="25"/>
-      <c r="U8" s="26" t="s">
-        <v>102</v>
-      </c>
-      <c r="V8" s="26"/>
-      <c r="W8" s="26"/>
-      <c r="X8" s="26"/>
+      <c r="P8" s="16"/>
+      <c r="V8" s="25"/>
+      <c r="W8" s="25"/>
+      <c r="X8" s="26" t="s">
+        <v>101</v>
+      </c>
       <c r="Y8" s="26"/>
       <c r="Z8" s="26"/>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A9" s="16" t="s">
-        <v>120</v>
-      </c>
-      <c r="B9" s="15" t="s">
-        <v>26</v>
-      </c>
+      <c r="AA8" s="26"/>
+      <c r="AB8" s="26"/>
+      <c r="AC8" s="26"/>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A9" s="16"/>
       <c r="C9" s="15" t="s">
         <v>2</v>
       </c>
@@ -2837,23 +2863,25 @@
       <c r="M9" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="P9" s="20" t="s">
-        <v>85</v>
-      </c>
-      <c r="S9" s="25"/>
-      <c r="T9" s="25"/>
-      <c r="U9" s="26" t="s">
-        <v>103</v>
-      </c>
-      <c r="V9" s="26"/>
-      <c r="W9" s="26"/>
-      <c r="X9" s="26"/>
+      <c r="N9" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="P9" s="20"/>
+      <c r="V9" s="25"/>
+      <c r="W9" s="25"/>
+      <c r="X9" s="26" t="s">
+        <v>102</v>
+      </c>
       <c r="Y9" s="26"/>
       <c r="Z9" s="26"/>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A10" s="16" t="s">
-        <v>121</v>
+      <c r="AA9" s="26"/>
+      <c r="AB9" s="26"/>
+      <c r="AC9" s="26"/>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A10" s="16"/>
+      <c r="C10" s="15" t="s">
+        <v>2</v>
       </c>
       <c r="F10" s="15">
         <v>5</v>
@@ -2877,24 +2905,20 @@
       <c r="N10" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="P10" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="S10" s="25"/>
-      <c r="T10" s="25"/>
-      <c r="U10" s="26" t="s">
-        <v>104</v>
-      </c>
-      <c r="V10" s="26"/>
-      <c r="W10" s="26"/>
-      <c r="X10" s="26"/>
+      <c r="P10" s="20"/>
+      <c r="V10" s="25"/>
+      <c r="W10" s="25"/>
+      <c r="X10" s="26" t="s">
+        <v>103</v>
+      </c>
       <c r="Y10" s="26"/>
       <c r="Z10" s="26"/>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A11" s="16" t="s">
-        <v>126</v>
-      </c>
+      <c r="AA10" s="26"/>
+      <c r="AB10" s="26"/>
+      <c r="AC10" s="26"/>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A11" s="16"/>
       <c r="C11" s="15" t="s">
         <v>2</v>
       </c>
@@ -2917,34 +2941,44 @@
       <c r="K11" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="L11" s="15" t="s">
+      <c r="L11" s="31" t="s">
         <v>45</v>
       </c>
       <c r="O11" s="15" t="s">
         <v>26</v>
       </c>
       <c r="P11" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="S11" s="25">
+        <v>127</v>
+      </c>
+      <c r="Q11" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="R11" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="S11" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="T11" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="V11" s="25">
         <v>2</v>
       </c>
-      <c r="T11" s="25">
+      <c r="W11" s="25">
         <v>2</v>
       </c>
-      <c r="U11" s="26" t="s">
-        <v>111</v>
-      </c>
-      <c r="V11" s="26"/>
-      <c r="W11" s="26"/>
-      <c r="X11" s="26"/>
+      <c r="X11" s="26" t="s">
+        <v>110</v>
+      </c>
       <c r="Y11" s="26"/>
       <c r="Z11" s="26"/>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A12" s="16" t="s">
-        <v>125</v>
-      </c>
+      <c r="AA11" s="26"/>
+      <c r="AB11" s="26"/>
+      <c r="AC11" s="26"/>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A12" s="16"/>
       <c r="E12" s="15" t="s">
         <v>17</v>
       </c>
@@ -2964,30 +2998,40 @@
       <c r="K12" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="L12" s="15" t="s">
+      <c r="L12" s="31" t="s">
         <v>44</v>
       </c>
       <c r="O12" s="15" t="s">
         <v>26</v>
       </c>
       <c r="P12" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="S12" s="25"/>
-      <c r="T12" s="25"/>
-      <c r="U12" s="26" t="s">
-        <v>113</v>
-      </c>
-      <c r="V12" s="26"/>
-      <c r="W12" s="26"/>
-      <c r="X12" s="26"/>
+        <v>127</v>
+      </c>
+      <c r="Q12" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="R12" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="S12" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="T12" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="V12" s="25"/>
+      <c r="W12" s="25"/>
+      <c r="X12" s="26" t="s">
+        <v>112</v>
+      </c>
       <c r="Y12" s="26"/>
       <c r="Z12" s="26"/>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A13" s="16" t="s">
-        <v>124</v>
-      </c>
+      <c r="AA12" s="26"/>
+      <c r="AB12" s="26"/>
+      <c r="AC12" s="26"/>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A13" s="16"/>
       <c r="E13" s="15" t="s">
         <v>16</v>
       </c>
@@ -3007,32 +3051,33 @@
       <c r="K13" s="15" t="s">
         <v>33</v>
       </c>
+      <c r="L13" s="32" t="s">
+        <v>39</v>
+      </c>
       <c r="N13" s="15" t="s">
         <v>2</v>
       </c>
       <c r="O13" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="P13" s="20" t="s">
-        <v>84</v>
-      </c>
-      <c r="S13" s="25">
+      <c r="P13" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="V13" s="25">
         <v>8</v>
       </c>
-      <c r="T13" s="25"/>
-      <c r="U13" s="26" t="s">
-        <v>105</v>
-      </c>
-      <c r="V13" s="26"/>
-      <c r="W13" s="26"/>
-      <c r="X13" s="26"/>
+      <c r="W13" s="25"/>
+      <c r="X13" s="26" t="s">
+        <v>104</v>
+      </c>
       <c r="Y13" s="26"/>
       <c r="Z13" s="26"/>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A14" s="16" t="s">
-        <v>122</v>
-      </c>
+      <c r="AA13" s="26"/>
+      <c r="AB13" s="26"/>
+      <c r="AC13" s="26"/>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A14" s="16"/>
       <c r="C14" s="15" t="s">
         <v>2</v>
       </c>
@@ -3055,30 +3100,29 @@
       <c r="K14" s="15" t="s">
         <v>34</v>
       </c>
+      <c r="L14" s="32" t="s">
+        <v>40</v>
+      </c>
       <c r="N14" s="15" t="s">
         <v>2</v>
       </c>
       <c r="O14" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="P14" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="S14" s="25"/>
-      <c r="T14" s="25"/>
-      <c r="U14" s="26" t="s">
-        <v>115</v>
-      </c>
-      <c r="V14" s="26"/>
-      <c r="W14" s="26"/>
-      <c r="X14" s="26"/>
+      <c r="P14" s="16"/>
+      <c r="V14" s="25"/>
+      <c r="W14" s="25"/>
+      <c r="X14" s="26" t="s">
+        <v>114</v>
+      </c>
       <c r="Y14" s="26"/>
       <c r="Z14" s="26"/>
-    </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A15" s="16" t="s">
-        <v>123</v>
-      </c>
+      <c r="AA14" s="26"/>
+      <c r="AB14" s="26"/>
+      <c r="AC14" s="26"/>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A15" s="16"/>
       <c r="C15" s="15" t="s">
         <v>2</v>
       </c>
@@ -3107,24 +3151,20 @@
       <c r="O15" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="P15" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="S15" s="25"/>
-      <c r="T15" s="25"/>
-      <c r="U15" s="27" t="s">
-        <v>116</v>
-      </c>
-      <c r="V15" s="26"/>
-      <c r="W15" s="26"/>
-      <c r="X15" s="26"/>
+      <c r="P15" s="16"/>
+      <c r="V15" s="25"/>
+      <c r="W15" s="25"/>
+      <c r="X15" s="27" t="s">
+        <v>115</v>
+      </c>
       <c r="Y15" s="26"/>
       <c r="Z15" s="26"/>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A16" s="16" t="s">
-        <v>127</v>
-      </c>
+      <c r="AA15" s="26"/>
+      <c r="AB15" s="26"/>
+      <c r="AC15" s="26"/>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A16" s="16"/>
       <c r="D16" s="15" t="s">
         <v>23</v>
       </c>
@@ -3144,28 +3184,24 @@
       <c r="K16" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="P16" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="S16" s="25">
+      <c r="P16" s="16"/>
+      <c r="V16" s="25">
         <v>2</v>
       </c>
-      <c r="T16" s="25">
+      <c r="W16" s="25">
         <v>2</v>
       </c>
-      <c r="U16" s="26" t="s">
-        <v>107</v>
-      </c>
-      <c r="V16" s="26"/>
-      <c r="W16" s="26"/>
-      <c r="X16" s="26"/>
+      <c r="X16" s="26" t="s">
+        <v>106</v>
+      </c>
       <c r="Y16" s="26"/>
       <c r="Z16" s="26"/>
-    </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A17" s="16" t="s">
-        <v>128</v>
-      </c>
+      <c r="AA16" s="26"/>
+      <c r="AB16" s="26"/>
+      <c r="AC16" s="26"/>
+    </row>
+    <row r="17" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A17" s="16"/>
       <c r="D17" s="15" t="s">
         <v>24</v>
       </c>
@@ -3185,25 +3221,25 @@
       <c r="M17" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="P17" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="S17" s="25">
+      <c r="P17" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="V17" s="25">
         <v>2</v>
       </c>
-      <c r="T17" s="25">
+      <c r="W17" s="25">
         <v>2</v>
       </c>
-      <c r="U17" s="26" t="s">
-        <v>114</v>
-      </c>
-      <c r="V17" s="26"/>
-      <c r="W17" s="26"/>
-      <c r="X17" s="26"/>
+      <c r="X17" s="26" t="s">
+        <v>113</v>
+      </c>
       <c r="Y17" s="26"/>
       <c r="Z17" s="26"/>
-    </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA17" s="26"/>
+      <c r="AB17" s="26"/>
+      <c r="AC17" s="26"/>
+    </row>
+    <row r="18" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>51</v>
       </c>
@@ -3218,30 +3254,30 @@
       <c r="P18" t="s">
         <v>51</v>
       </c>
-      <c r="S18" s="25">
+      <c r="V18" s="25">
         <v>1</v>
       </c>
-      <c r="T18" s="25">
+      <c r="W18" s="25">
         <v>1</v>
       </c>
-      <c r="U18" s="26" t="s">
-        <v>106</v>
-      </c>
-      <c r="V18" s="26"/>
-      <c r="W18" s="26"/>
-      <c r="X18" s="26"/>
+      <c r="X18" s="26" t="s">
+        <v>105</v>
+      </c>
       <c r="Y18" s="26"/>
       <c r="Z18" s="26"/>
-    </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA18" s="26"/>
+      <c r="AB18" s="26"/>
+      <c r="AC18" s="26"/>
+    </row>
+    <row r="19" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="F19" s="15">
         <v>17</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>18</v>
+        <v>137</v>
       </c>
       <c r="I19" s="4" t="s">
         <v>10</v>
@@ -3250,24 +3286,24 @@
         <v>51</v>
       </c>
       <c r="P19" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="S19" s="25">
+        <v>123</v>
+      </c>
+      <c r="V19" s="25">
         <v>1</v>
       </c>
-      <c r="T19" s="25">
+      <c r="W19" s="25">
         <v>1</v>
       </c>
-      <c r="U19" s="26" t="s">
-        <v>110</v>
-      </c>
-      <c r="V19" s="26"/>
-      <c r="W19" s="26"/>
-      <c r="X19" s="26"/>
+      <c r="X19" s="26" t="s">
+        <v>109</v>
+      </c>
       <c r="Y19" s="26"/>
       <c r="Z19" s="26"/>
-    </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA19" s="26"/>
+      <c r="AB19" s="26"/>
+      <c r="AC19" s="26"/>
+    </row>
+    <row r="20" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>62</v>
       </c>
@@ -3290,24 +3326,24 @@
       <c r="P20" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="S20" s="25">
+      <c r="V20" s="25">
         <v>1</v>
       </c>
-      <c r="T20" s="25">
+      <c r="W20" s="25">
         <v>1</v>
       </c>
-      <c r="U20" s="26" t="s">
-        <v>112</v>
-      </c>
-      <c r="V20" s="26"/>
-      <c r="W20" s="26"/>
-      <c r="X20" s="26"/>
+      <c r="X20" s="26" t="s">
+        <v>111</v>
+      </c>
       <c r="Y20" s="26"/>
       <c r="Z20" s="26"/>
-    </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>69</v>
+      <c r="AA20" s="26"/>
+      <c r="AB20" s="26"/>
+      <c r="AC20" s="26"/>
+    </row>
+    <row r="21" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A21" s="30" t="s">
+        <v>121</v>
       </c>
       <c r="F21" s="15" t="s">
         <v>51</v>
@@ -3325,21 +3361,19 @@
       <c r="K21" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="P21" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="S21" s="25"/>
-      <c r="T21" s="25"/>
-      <c r="U21" s="26"/>
-      <c r="V21" s="26"/>
-      <c r="W21" s="26"/>
+      <c r="P21" s="16"/>
+      <c r="V21" s="25"/>
+      <c r="W21" s="25"/>
       <c r="X21" s="26"/>
       <c r="Y21" s="26"/>
       <c r="Z21" s="26"/>
-    </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA21" s="26"/>
+      <c r="AB21" s="26"/>
+      <c r="AC21" s="26"/>
+    </row>
+    <row r="22" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>66</v>
+        <v>135</v>
       </c>
       <c r="F22" s="15" t="s">
         <v>51</v>
@@ -3349,24 +3383,24 @@
       </c>
       <c r="H22" s="7"/>
       <c r="I22" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J22" s="7"/>
-      <c r="P22" t="s">
-        <v>68</v>
-      </c>
-      <c r="S22" s="25"/>
-      <c r="T22" s="25"/>
-      <c r="U22" s="26"/>
-      <c r="V22" s="26"/>
-      <c r="W22" s="26"/>
+      <c r="P22" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="V22" s="25"/>
+      <c r="W22" s="25"/>
       <c r="X22" s="26"/>
       <c r="Y22" s="26"/>
       <c r="Z22" s="26"/>
-    </row>
-    <row r="23" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AA22" s="26"/>
+      <c r="AB22" s="26"/>
+      <c r="AC22" s="26"/>
+    </row>
+    <row r="23" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F23" s="15">
         <v>26</v>
@@ -3380,82 +3414,82 @@
       <c r="P23" t="s">
         <v>51</v>
       </c>
-      <c r="S23" s="25">
-        <f>SUM(S7:S22)</f>
+      <c r="V23" s="25">
+        <f>SUM(V7:V22)</f>
         <v>26</v>
       </c>
-      <c r="T23" s="28">
-        <f>SUM(T7:T22)</f>
+      <c r="W23" s="28">
+        <f>SUM(W7:W22)</f>
         <v>9</v>
       </c>
-      <c r="U23" s="26" t="s">
-        <v>109</v>
-      </c>
-      <c r="V23" s="26"/>
-      <c r="W23" s="26"/>
-      <c r="X23" s="26"/>
+      <c r="X23" s="26" t="s">
+        <v>108</v>
+      </c>
       <c r="Y23" s="26"/>
       <c r="Z23" s="26"/>
-    </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="S24" s="25"/>
-      <c r="T24" s="25"/>
-      <c r="U24" s="26"/>
-      <c r="V24" s="26"/>
-      <c r="W24" s="26"/>
+      <c r="AA23" s="26"/>
+      <c r="AB23" s="26"/>
+      <c r="AC23" s="26"/>
+    </row>
+    <row r="24" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="V24" s="25"/>
+      <c r="W24" s="25"/>
       <c r="X24" s="26"/>
       <c r="Y24" s="26"/>
       <c r="Z24" s="26"/>
-    </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA24" s="26"/>
+      <c r="AB24" s="26"/>
+      <c r="AC24" s="26"/>
+    </row>
+    <row r="25" spans="1:29" x14ac:dyDescent="0.2">
       <c r="H25" s="10"/>
-      <c r="S25" s="25"/>
-      <c r="T25" s="25"/>
-      <c r="U25" s="26"/>
-      <c r="V25" s="26"/>
-      <c r="W25" s="26"/>
+      <c r="V25" s="25"/>
+      <c r="W25" s="25"/>
       <c r="X25" s="26"/>
       <c r="Y25" s="26"/>
       <c r="Z25" s="26"/>
-    </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA25" s="26"/>
+      <c r="AB25" s="26"/>
+      <c r="AC25" s="26"/>
+    </row>
+    <row r="26" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A26" s="10"/>
       <c r="G26" s="10"/>
-      <c r="S26" s="25"/>
-      <c r="T26" s="25"/>
-      <c r="U26" s="26"/>
-      <c r="V26" s="26"/>
-      <c r="W26" s="26"/>
+      <c r="V26" s="25"/>
+      <c r="W26" s="25"/>
       <c r="X26" s="26"/>
       <c r="Y26" s="26"/>
       <c r="Z26" s="26"/>
-    </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA26" s="26"/>
+      <c r="AB26" s="26"/>
+      <c r="AC26" s="26"/>
+    </row>
+    <row r="27" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A27" s="11"/>
       <c r="G27" s="11"/>
       <c r="H27" s="11"/>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A28" s="11"/>
       <c r="G28" s="11"/>
       <c r="H28" s="11"/>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A29" s="11"/>
       <c r="G29" s="11"/>
       <c r="H29" s="11"/>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A30" s="11"/>
       <c r="G30" s="11"/>
       <c r="H30" s="11"/>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A31" s="11"/>
       <c r="G31" s="11"/>
       <c r="H31" s="11"/>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A32" s="11"/>
       <c r="G32" s="11"/>
       <c r="H32" s="11"/>
@@ -3537,33 +3571,34 @@
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="S4:Y4"/>
+    <mergeCell ref="V4:AB4"/>
   </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{CF74EE04-8972-D048-A403-865EBF5C5826}"/>
   </hyperlinks>

</xml_diff>

<commit_message>
Pin usage updates for Teensy
</commit_message>
<xml_diff>
--- a/Electronic Design/Core 64 Pin Usage Mapping.xlsx
+++ b/Electronic Design/Core 64 Pin Usage Mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1c02d23ac1278198/00_MBP2011-Documents/Electronics/Core 64 Interactive Badge/Core-64-Interactive-Core-Memory-Badge/Electronic Design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="74" documentId="114_{C854064A-3C16-0445-B75C-033646BE2CC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C8F2BB7A-3D4B-894A-AEF0-0799CF73EA1D}"/>
+  <xr:revisionPtr revIDLastSave="293" documentId="114_{C854064A-3C16-0445-B75C-033646BE2CC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{48C22F0B-A1D8-4E4E-971A-18946189BD53}"/>
   <bookViews>
-    <workbookView xWindow="-35200" yWindow="-10340" windowWidth="35200" windowHeight="28340" activeTab="2" xr2:uid="{A4752792-CA31-B046-B883-84F8D68A57EC}"/>
+    <workbookView xWindow="-33020" yWindow="-10340" windowWidth="32480" windowHeight="28340" activeTab="2" xr2:uid="{A4752792-CA31-B046-B883-84F8D68A57EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Reference Pinouts" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="146">
   <si>
     <t>Custom</t>
   </si>
@@ -337,54 +337,6 @@
     <t>Teensy 3.2 Pinout Assignments for v0.3 Core 64 Badge</t>
   </si>
   <si>
-    <t>Core array matrix transistors 20+1=21 including Enable</t>
-  </si>
-  <si>
-    <t>3X using 3-to-8 decoder yields 24 outputs from 9 pins.</t>
-  </si>
-  <si>
-    <t>#22 and #23 could be used for a future active stylus</t>
-  </si>
-  <si>
-    <t>#24 available</t>
-  </si>
-  <si>
-    <t>Expand hall and reed to be 8 hall sensors.</t>
-  </si>
-  <si>
-    <t>LED Array</t>
-  </si>
-  <si>
-    <t>OLED (i2C)</t>
-  </si>
-  <si>
-    <t>v0.3 and beyond planning</t>
-  </si>
-  <si>
-    <t>TOTAL PINS NEED</t>
-  </si>
-  <si>
-    <t>Analog battery voltage</t>
-  </si>
-  <si>
-    <t>Int. capable, Sense (maybe 2 sense for CW and CCW discrimination?)</t>
-  </si>
-  <si>
-    <t>Heartbeat built-in LED</t>
-  </si>
-  <si>
-    <t>(or use CD4021B  https://www.arduino.cc/en/tutorial/ShiftIn)</t>
-  </si>
-  <si>
-    <t>SAO #1 (i2C, GND, 3.3V, and 2 GPIOS each)</t>
-  </si>
-  <si>
-    <t>(Or use CD4021B  https://www.arduino.cc/en/tutorial/ShiftIn)</t>
-  </si>
-  <si>
-    <t>(Or use 2x 16 GPIO I2C expander http://ww1.microchip.com/downloads/en/DeviceDoc/20090C.pdf)</t>
-  </si>
-  <si>
     <t>https://forum.pjrc.com/threads/55568-Teensy-3-2-3-5-pin-compatibility</t>
   </si>
   <si>
@@ -406,9 +358,6 @@
     <t>TEENSY_VUSB to Core 64 Power Switch</t>
   </si>
   <si>
-    <t>supplied from TEENSY_3V3</t>
-  </si>
-  <si>
     <t>TEENSY_3V3 from Teensy 3.3V aka 3V3_100mA</t>
   </si>
   <si>
@@ -449,6 +398,81 @@
   </si>
   <si>
     <t>VBAT</t>
+  </si>
+  <si>
+    <t>Teensy LC Pinout Assignments for v0.3 Core 64 Badge</t>
+  </si>
+  <si>
+    <t>DOUT</t>
+  </si>
+  <si>
+    <t>DIN</t>
+  </si>
+  <si>
+    <t>CS</t>
+  </si>
+  <si>
+    <t>CAN</t>
+  </si>
+  <si>
+    <t>SCK</t>
+  </si>
+  <si>
+    <t>Connect back to TEENSY_3V3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Battery Voltage (1/2) monitor </t>
+  </si>
+  <si>
+    <t>3.3V (250mA)</t>
+  </si>
+  <si>
+    <t>A12</t>
+  </si>
+  <si>
+    <t>A13</t>
+  </si>
+  <si>
+    <t>26/A14/DAC</t>
+  </si>
+  <si>
+    <t>AGND</t>
+  </si>
+  <si>
+    <t>If needed, pull PRG</t>
+  </si>
+  <si>
+    <t>HIGH with 10K on</t>
+  </si>
+  <si>
+    <t>TEENSY board.</t>
+  </si>
+  <si>
+    <t>Try not to use any of these</t>
+  </si>
+  <si>
+    <t>to avoid the need to populate</t>
+  </si>
+  <si>
+    <t>this end row header on the PCB.</t>
+  </si>
+  <si>
+    <t>SAO Port 3, GPIO 1</t>
+  </si>
+  <si>
+    <t>SAO Port 3, GPIO 2</t>
+  </si>
+  <si>
+    <t>SAO Port 2, GPIO 1 (TX)</t>
+  </si>
+  <si>
+    <t>SAO Port 2, GPIO 2 (RX)</t>
+  </si>
+  <si>
+    <t>SAO Port 1, GPIO 2 (RX)</t>
+  </si>
+  <si>
+    <t>SAO Port 1, GPIO 1 (TX)</t>
   </si>
 </sst>
 </file>
@@ -537,7 +561,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -570,12 +594,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA845F2"/>
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -663,12 +693,49 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -728,22 +795,77 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1109,62 +1231,14 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="AutoShape 5" descr="Image result for teensy lc backside">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A6EE199-8F91-D644-8506-F7CAEB1EBA6B}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="6299200" y="3924300"/>
-          <a:ext cx="304800" cy="304800"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>7</xdr:col>
       <xdr:colOff>66222</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>117928</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>1569357</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>9074</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1217,23 +1291,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>54430</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>172357</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>1302658</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>8165</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>47210</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>81643</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>3628</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>68037</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Picture 7">
+        <xdr:cNvPr id="9" name="Picture 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{725F2268-9C4C-354E-B6CE-41DE42F581BA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C41C1AE-FB4D-514C-B0E0-3869D4B102A5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1255,9 +1329,9 @@
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="6350001" y="5061857"/>
-          <a:ext cx="2795852" cy="1306286"/>
+        <a:xfrm rot="5400000">
+          <a:off x="21368657" y="4694466"/>
+          <a:ext cx="4962072" cy="5800270"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1278,23 +1352,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>235858</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>84365</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>183243</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>143328</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>943428</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>169637</xdr:rowOff>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>226223</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Picture 8">
+        <xdr:cNvPr id="10" name="Picture 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C41C1AE-FB4D-514C-B0E0-3869D4B102A5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5779CE2B-EB33-DC42-84AB-69BC07B6C2D4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1316,9 +1390,9 @@
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
-        <a:xfrm rot="5400000">
-          <a:off x="696686" y="4249966"/>
-          <a:ext cx="4874986" cy="5796641"/>
+        <a:xfrm>
+          <a:off x="26929443" y="5248728"/>
+          <a:ext cx="5821480" cy="4885872"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1339,23 +1413,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>907143</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>117928</xdr:rowOff>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>290285</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>99786</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>166939</xdr:rowOff>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>112486</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>21867</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="10" name="Picture 9">
+        <xdr:cNvPr id="11" name="Picture 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5779CE2B-EB33-DC42-84AB-69BC07B6C2D4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3C87351-5E34-0747-B93E-26AEF1F70F3D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1378,8 +1452,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="5996214" y="6141357"/>
-          <a:ext cx="3202215" cy="2643439"/>
+          <a:off x="32814985" y="5092700"/>
+          <a:ext cx="6426201" cy="6155967"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1400,23 +1474,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>99785</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1203035</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>94188</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>3147786</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>47267</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1578429</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>21777</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="11" name="Picture 10">
+        <xdr:cNvPr id="12" name="Picture 11" descr="5 Ⅵ ">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3C87351-5E34-0747-B93E-26AEF1F70F3D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{033BB512-8439-5E41-9892-D31C46B89151}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1425,7 +1499,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1438,9 +1512,9 @@
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="9198428" y="4816929"/>
-          <a:ext cx="6422572" cy="6043481"/>
+        <a:xfrm rot="5400000">
+          <a:off x="5598887" y="1197436"/>
+          <a:ext cx="2975589" cy="1581894"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1457,6 +1531,282 @@
         </a:extLst>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>1282700</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>431346</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>16102</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13" descr="ad &#10;Analog Pms &#10;2 &#10;A &#10;Program &#10;Touch Sense &#10;GND &#10;Serial PO 心 &#10;OND &#10;0 【 IISOn n01 &#10;I IXI IOSIN n01 &#10;ki 0 &#10;EXE IS) &#10;【 XI IOSI'B' &#10;DISCA &#10;C Ports &#10;Md &#10;SPI PO 心 ">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{250009D9-1B09-F146-AF31-CE3CFADEEA82}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm rot="5400000">
+          <a:off x="21696022" y="-563222"/>
+          <a:ext cx="4715102" cy="6247946"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>609599</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>776280</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D20116D4-485A-7040-979C-F4EF5A733E5E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="27355799" y="1117600"/>
+          <a:ext cx="5119681" cy="2400300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>292099</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>90260</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>186350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15" descr="vusB &#10;Micro_AB &#10;vusB &#10;GNO &#10;MKL02Z3ZVFG4 &#10;VDO &#10;PTB2 &#10;PTB3 &#10;PTB4 &#10;vss &#10;vss &#10;PTBO &#10;PTB5 &#10;PTBI &#10;p TAI &#10;p TA 2 &#10;MKL26Z64VFT4 &#10;VREGIN &#10;vouT33 &#10;VDO &#10;VDO &#10;VODA &#10;PTE20 &#10;PTE21 &#10;vssA &#10;usao DM &#10;usao DP &#10;PTA18 &#10;PTA19 &#10;RESET &#10;vss &#10;vss &#10;vss &#10;PTC2 &#10;PTCI &#10;PT06 &#10;PT05 &#10;PTB2 &#10;PTB3 &#10;PTBI &#10;PTBO &#10;FTC o &#10;PTOI &#10;PTC5 &#10;FTC 7 &#10;FTC 6 &#10;FTC 4 &#10;PTC3 &#10;PT03 &#10;PT02 &#10;PT04 &#10;PT07 &#10;p TA 2 &#10;p TAI &#10;PTOO &#10;PTB17 &#10;PTB16 &#10;PTE29 &#10;PTE30 &#10;PTE24 &#10;PTE25 &#10;GNO &#10;23 &#10;22 &#10;21 A7 &#10;20 &#10;19 / AS &#10;17/A3 &#10;15 / Al &#10;13 (LED) &#10;GNO &#10;26/AIZDAC &#10;PROGRAM &#10;GNO &#10;17 (VIN) &#10;74LVIT125 &#10;Teensy-LC ">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{987BAF53-41B8-614B-A9D8-4C82790152C8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="32816799" y="88900"/>
+          <a:ext cx="6402161" cy="4796450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>734785</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>199571</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>97972</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="17" name="Straight Connector 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC266598-1887-7546-A5BE-038185ADD264}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="34084985" y="5016500"/>
+          <a:ext cx="290286" cy="390072"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>290285</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>580571</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>186872</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="Straight Connector 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B2F93E57-6746-F541-9F34-E7AF7500CD84}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="33640485" y="0"/>
+          <a:ext cx="290286" cy="390072"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1762,24 +2112,24 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A4" sqref="A1:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="23" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="23" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1797,7 +2147,7 @@
   <dimension ref="A1:P50"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection sqref="A1:R23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2401,7 +2751,7 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
       <c r="F22" s="15" t="s">
         <v>51</v>
@@ -2571,10 +2921,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CBC2977-27CE-C64F-BE79-A69FB2535F84}">
-  <dimension ref="A1:AC53"/>
+  <dimension ref="A1:AC62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="117" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="P32" sqref="P32:P33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2603,12 +2953,12 @@
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>99</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G2" s="8"/>
       <c r="H2" s="24" t="s">
@@ -2660,48 +3010,67 @@
         <v>1</v>
       </c>
       <c r="P3" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="Q3" s="15" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="R3" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
       <c r="S3" s="15" t="s">
-        <v>129</v>
+        <v>112</v>
       </c>
       <c r="T3" t="s">
-        <v>130</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="V3" s="27"/>
+      <c r="W3" s="27"/>
+      <c r="X3" s="9"/>
+      <c r="Y3" s="9"/>
+      <c r="Z3" s="9"/>
+      <c r="AA3" s="9"/>
+      <c r="AB3" s="9"/>
+      <c r="AC3" s="9"/>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A4" s="30" t="s">
-        <v>121</v>
-      </c>
-      <c r="G4" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="H4" s="12"/>
+      <c r="I4" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="J4" s="7"/>
-      <c r="P4" s="30" t="s">
-        <v>125</v>
-      </c>
-      <c r="V4" s="29" t="s">
-        <v>107</v>
-      </c>
-      <c r="W4" s="29"/>
-      <c r="X4" s="29"/>
-      <c r="Y4" s="29"/>
-      <c r="Z4" s="29"/>
-      <c r="AA4" s="29"/>
-      <c r="AB4" s="29"/>
-      <c r="AC4" s="26"/>
+      <c r="J4" s="37"/>
+      <c r="K4" s="26"/>
+      <c r="L4" s="26"/>
+      <c r="M4" s="26"/>
+      <c r="N4" s="26"/>
+      <c r="O4" s="26"/>
+      <c r="P4" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="V4" s="49"/>
+      <c r="W4" s="49"/>
+      <c r="X4" s="49"/>
+      <c r="Y4" s="49"/>
+      <c r="Z4" s="49"/>
+      <c r="AA4" s="49"/>
+      <c r="AB4" s="49"/>
+      <c r="AC4" s="9"/>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A5" s="16"/>
+      <c r="A5" s="20" t="s">
+        <v>144</v>
+      </c>
       <c r="B5" s="15" t="s">
         <v>26</v>
       </c>
@@ -2718,24 +3087,31 @@
         <v>0</v>
       </c>
       <c r="H5" s="7"/>
-      <c r="I5" s="4" t="s">
+      <c r="I5" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="J5" s="7"/>
+      <c r="J5" s="35"/>
+      <c r="K5" s="34"/>
+      <c r="L5" s="34"/>
+      <c r="M5" s="34"/>
+      <c r="N5" s="34"/>
+      <c r="O5" s="34"/>
       <c r="P5" s="30" t="s">
-        <v>121</v>
-      </c>
-      <c r="V5" s="25"/>
-      <c r="W5" s="25"/>
-      <c r="X5" s="26"/>
-      <c r="Y5" s="26"/>
-      <c r="Z5" s="26"/>
-      <c r="AA5" s="26"/>
-      <c r="AB5" s="26"/>
-      <c r="AC5" s="26"/>
+        <v>105</v>
+      </c>
+      <c r="V5" s="27"/>
+      <c r="W5" s="27"/>
+      <c r="X5" s="9"/>
+      <c r="Y5" s="9"/>
+      <c r="Z5" s="9"/>
+      <c r="AA5" s="9"/>
+      <c r="AB5" s="9"/>
+      <c r="AC5" s="9"/>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A6" s="16"/>
+      <c r="A6" s="20" t="s">
+        <v>145</v>
+      </c>
       <c r="B6" s="15" t="s">
         <v>26</v>
       </c>
@@ -2752,21 +3128,26 @@
         <v>1</v>
       </c>
       <c r="H6" s="7"/>
-      <c r="I6" s="4" t="s">
+      <c r="I6" s="42" t="s">
         <v>49</v>
       </c>
-      <c r="J6" s="7"/>
-      <c r="P6" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="V6" s="25"/>
-      <c r="W6" s="25"/>
-      <c r="X6" s="26"/>
-      <c r="Y6" s="26"/>
-      <c r="Z6" s="26"/>
-      <c r="AA6" s="26"/>
-      <c r="AB6" s="26"/>
-      <c r="AC6" s="26"/>
+      <c r="J6" s="37"/>
+      <c r="K6" s="26"/>
+      <c r="L6" s="26"/>
+      <c r="M6" s="26"/>
+      <c r="N6" s="26"/>
+      <c r="O6" s="26"/>
+      <c r="P6" s="25" t="s">
+        <v>107</v>
+      </c>
+      <c r="V6" s="27"/>
+      <c r="W6" s="27"/>
+      <c r="X6" s="9"/>
+      <c r="Y6" s="9"/>
+      <c r="Z6" s="9"/>
+      <c r="AA6" s="9"/>
+      <c r="AB6" s="9"/>
+      <c r="AC6" s="9"/>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A7" s="16"/>
@@ -2786,25 +3167,32 @@
       <c r="K7" s="15" t="s">
         <v>27</v>
       </c>
+      <c r="L7" s="15" t="s">
+        <v>39</v>
+      </c>
       <c r="N7" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="P7" s="20"/>
-      <c r="V7" s="25">
-        <v>9</v>
-      </c>
-      <c r="W7" s="25"/>
-      <c r="X7" s="26" t="s">
-        <v>100</v>
-      </c>
-      <c r="Y7" s="26"/>
-      <c r="Z7" s="26"/>
-      <c r="AA7" s="26"/>
-      <c r="AB7" s="26"/>
-      <c r="AC7" s="26"/>
+      <c r="O7" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="P7" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="V7" s="27"/>
+      <c r="W7" s="27"/>
+      <c r="X7" s="9"/>
+      <c r="Y7" s="9"/>
+      <c r="Z7" s="9"/>
+      <c r="AA7" s="9"/>
+      <c r="AB7" s="9"/>
+      <c r="AC7" s="9"/>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A8" s="16"/>
+      <c r="B8" s="15" t="s">
+        <v>26</v>
+      </c>
       <c r="C8" s="15" t="s">
         <v>2</v>
       </c>
@@ -2824,23 +3212,32 @@
       <c r="K8" s="15" t="s">
         <v>28</v>
       </c>
+      <c r="L8" s="15" t="s">
+        <v>40</v>
+      </c>
       <c r="N8" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="P8" s="16"/>
-      <c r="V8" s="25"/>
-      <c r="W8" s="25"/>
-      <c r="X8" s="26" t="s">
-        <v>101</v>
-      </c>
-      <c r="Y8" s="26"/>
-      <c r="Z8" s="26"/>
-      <c r="AA8" s="26"/>
-      <c r="AB8" s="26"/>
-      <c r="AC8" s="26"/>
+      <c r="O8" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="P8" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="V8" s="27"/>
+      <c r="W8" s="27"/>
+      <c r="X8" s="9"/>
+      <c r="Y8" s="9"/>
+      <c r="Z8" s="9"/>
+      <c r="AA8" s="9"/>
+      <c r="AB8" s="9"/>
+      <c r="AC8" s="9"/>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A9" s="16"/>
+      <c r="B9" s="15" t="s">
+        <v>26</v>
+      </c>
       <c r="C9" s="15" t="s">
         <v>2</v>
       </c>
@@ -2851,38 +3248,35 @@
         <v>4</v>
       </c>
       <c r="H9" s="7"/>
-      <c r="I9" s="4">
+      <c r="I9" s="39">
         <v>21</v>
       </c>
-      <c r="J9" s="7">
+      <c r="J9" s="40">
         <v>21</v>
       </c>
-      <c r="K9" s="15" t="s">
+      <c r="K9" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="M9" s="15" t="s">
+      <c r="L9" s="41"/>
+      <c r="M9" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="N9" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="P9" s="20"/>
-      <c r="V9" s="25"/>
-      <c r="W9" s="25"/>
-      <c r="X9" s="26" t="s">
-        <v>102</v>
-      </c>
-      <c r="Y9" s="26"/>
-      <c r="Z9" s="26"/>
-      <c r="AA9" s="26"/>
-      <c r="AB9" s="26"/>
-      <c r="AC9" s="26"/>
+      <c r="N9" s="41"/>
+      <c r="O9" s="41"/>
+      <c r="P9" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="V9" s="27"/>
+      <c r="W9" s="27"/>
+      <c r="X9" s="9"/>
+      <c r="Y9" s="9"/>
+      <c r="Z9" s="9"/>
+      <c r="AA9" s="9"/>
+      <c r="AB9" s="9"/>
+      <c r="AC9" s="9"/>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A10" s="16"/>
-      <c r="C10" s="15" t="s">
-        <v>2</v>
-      </c>
       <c r="F10" s="15">
         <v>5</v>
       </c>
@@ -2905,17 +3299,15 @@
       <c r="N10" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="P10" s="20"/>
-      <c r="V10" s="25"/>
-      <c r="W10" s="25"/>
-      <c r="X10" s="26" t="s">
-        <v>103</v>
-      </c>
-      <c r="Y10" s="26"/>
-      <c r="Z10" s="26"/>
-      <c r="AA10" s="26"/>
-      <c r="AB10" s="26"/>
-      <c r="AC10" s="26"/>
+      <c r="P10" s="16"/>
+      <c r="V10" s="27"/>
+      <c r="W10" s="27"/>
+      <c r="X10" s="9"/>
+      <c r="Y10" s="9"/>
+      <c r="Z10" s="9"/>
+      <c r="AA10" s="9"/>
+      <c r="AB10" s="9"/>
+      <c r="AC10" s="9"/>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A11" s="16"/>
@@ -2932,50 +3324,46 @@
         <v>6</v>
       </c>
       <c r="H11" s="7"/>
-      <c r="I11" s="4">
+      <c r="I11" s="39">
         <v>19</v>
       </c>
-      <c r="J11" s="7">
+      <c r="J11" s="40">
         <v>19</v>
       </c>
-      <c r="K11" s="15" t="s">
+      <c r="K11" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="L11" s="31" t="s">
+      <c r="L11" s="41" t="s">
         <v>45</v>
       </c>
-      <c r="O11" s="15" t="s">
+      <c r="M11" s="41"/>
+      <c r="N11" s="41"/>
+      <c r="O11" s="41" t="s">
         <v>26</v>
       </c>
       <c r="P11" s="8" t="s">
-        <v>127</v>
+        <v>110</v>
       </c>
       <c r="Q11" s="8" t="s">
-        <v>126</v>
+        <v>109</v>
       </c>
       <c r="R11" s="8" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="S11" s="8" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
       <c r="T11" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="V11" s="25">
-        <v>2</v>
-      </c>
-      <c r="W11" s="25">
-        <v>2</v>
-      </c>
-      <c r="X11" s="26" t="s">
-        <v>110</v>
-      </c>
-      <c r="Y11" s="26"/>
-      <c r="Z11" s="26"/>
-      <c r="AA11" s="26"/>
-      <c r="AB11" s="26"/>
-      <c r="AC11" s="26"/>
+        <v>116</v>
+      </c>
+      <c r="V11" s="27"/>
+      <c r="W11" s="27"/>
+      <c r="X11" s="9"/>
+      <c r="Y11" s="9"/>
+      <c r="Z11" s="9"/>
+      <c r="AA11" s="9"/>
+      <c r="AB11" s="9"/>
+      <c r="AC11" s="9"/>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A12" s="16"/>
@@ -2989,46 +3377,46 @@
         <v>7</v>
       </c>
       <c r="H12" s="7"/>
-      <c r="I12" s="4">
+      <c r="I12" s="39">
         <v>18</v>
       </c>
-      <c r="J12" s="7">
+      <c r="J12" s="40">
         <v>18</v>
       </c>
-      <c r="K12" s="15" t="s">
+      <c r="K12" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="L12" s="31" t="s">
+      <c r="L12" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="O12" s="15" t="s">
+      <c r="M12" s="41"/>
+      <c r="N12" s="41"/>
+      <c r="O12" s="41" t="s">
         <v>26</v>
       </c>
       <c r="P12" s="8" t="s">
-        <v>127</v>
+        <v>110</v>
       </c>
       <c r="Q12" s="8" t="s">
-        <v>126</v>
+        <v>109</v>
       </c>
       <c r="R12" s="8" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="S12" s="8" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
       <c r="T12" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="V12" s="25"/>
-      <c r="W12" s="25"/>
-      <c r="X12" s="26" t="s">
-        <v>112</v>
-      </c>
-      <c r="Y12" s="26"/>
-      <c r="Z12" s="26"/>
-      <c r="AA12" s="26"/>
-      <c r="AB12" s="26"/>
-      <c r="AC12" s="26"/>
+        <v>116</v>
+      </c>
+      <c r="V12" s="27"/>
+      <c r="W12" s="27"/>
+      <c r="X12" s="9"/>
+      <c r="Y12" s="9"/>
+      <c r="Z12" s="9"/>
+      <c r="AA12" s="9"/>
+      <c r="AB12" s="9"/>
+      <c r="AC12" s="9"/>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A13" s="16"/>
@@ -3051,33 +3439,26 @@
       <c r="K13" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="L13" s="32" t="s">
-        <v>39</v>
-      </c>
       <c r="N13" s="15" t="s">
         <v>2</v>
       </c>
       <c r="O13" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="P13" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="V13" s="25">
-        <v>8</v>
-      </c>
-      <c r="W13" s="25"/>
-      <c r="X13" s="26" t="s">
-        <v>104</v>
-      </c>
-      <c r="Y13" s="26"/>
-      <c r="Z13" s="26"/>
-      <c r="AA13" s="26"/>
-      <c r="AB13" s="26"/>
-      <c r="AC13" s="26"/>
+      <c r="P13" s="16"/>
+      <c r="V13" s="27"/>
+      <c r="W13" s="27"/>
+      <c r="X13" s="9"/>
+      <c r="Y13" s="9"/>
+      <c r="Z13" s="9"/>
+      <c r="AA13" s="9"/>
+      <c r="AB13" s="9"/>
+      <c r="AC13" s="9"/>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A14" s="16"/>
+      <c r="A14" s="20" t="s">
+        <v>143</v>
+      </c>
       <c r="C14" s="15" t="s">
         <v>2</v>
       </c>
@@ -3100,9 +3481,6 @@
       <c r="K14" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="L14" s="32" t="s">
-        <v>40</v>
-      </c>
       <c r="N14" s="15" t="s">
         <v>2</v>
       </c>
@@ -3110,19 +3488,19 @@
         <v>26</v>
       </c>
       <c r="P14" s="16"/>
-      <c r="V14" s="25"/>
-      <c r="W14" s="25"/>
-      <c r="X14" s="26" t="s">
-        <v>114</v>
-      </c>
-      <c r="Y14" s="26"/>
-      <c r="Z14" s="26"/>
-      <c r="AA14" s="26"/>
-      <c r="AB14" s="26"/>
-      <c r="AC14" s="26"/>
+      <c r="V14" s="27"/>
+      <c r="W14" s="27"/>
+      <c r="X14" s="9"/>
+      <c r="Y14" s="9"/>
+      <c r="Z14" s="9"/>
+      <c r="AA14" s="9"/>
+      <c r="AB14" s="9"/>
+      <c r="AC14" s="9"/>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A15" s="16"/>
+      <c r="A15" s="20" t="s">
+        <v>142</v>
+      </c>
       <c r="C15" s="15" t="s">
         <v>2</v>
       </c>
@@ -3152,16 +3530,14 @@
         <v>26</v>
       </c>
       <c r="P15" s="16"/>
-      <c r="V15" s="25"/>
-      <c r="W15" s="25"/>
-      <c r="X15" s="27" t="s">
-        <v>115</v>
-      </c>
-      <c r="Y15" s="26"/>
-      <c r="Z15" s="26"/>
-      <c r="AA15" s="26"/>
-      <c r="AB15" s="26"/>
-      <c r="AC15" s="26"/>
+      <c r="V15" s="27"/>
+      <c r="W15" s="27"/>
+      <c r="X15" s="28"/>
+      <c r="Y15" s="9"/>
+      <c r="Z15" s="9"/>
+      <c r="AA15" s="9"/>
+      <c r="AB15" s="9"/>
+      <c r="AC15" s="9"/>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A16" s="16"/>
@@ -3175,30 +3551,30 @@
         <v>11</v>
       </c>
       <c r="H16" s="7"/>
-      <c r="I16" s="4">
+      <c r="I16" s="39">
         <v>14</v>
       </c>
-      <c r="J16" s="7">
+      <c r="J16" s="40">
         <v>14</v>
       </c>
-      <c r="K16" s="15" t="s">
+      <c r="K16" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="P16" s="16"/>
-      <c r="V16" s="25">
-        <v>2</v>
-      </c>
-      <c r="W16" s="25">
-        <v>2</v>
-      </c>
-      <c r="X16" s="26" t="s">
-        <v>106</v>
-      </c>
-      <c r="Y16" s="26"/>
-      <c r="Z16" s="26"/>
-      <c r="AA16" s="26"/>
-      <c r="AB16" s="26"/>
-      <c r="AC16" s="26"/>
+      <c r="L16" s="41"/>
+      <c r="M16" s="41"/>
+      <c r="N16" s="41"/>
+      <c r="O16" s="41"/>
+      <c r="P16" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="V16" s="27"/>
+      <c r="W16" s="27"/>
+      <c r="X16" s="9"/>
+      <c r="Y16" s="9"/>
+      <c r="Z16" s="9"/>
+      <c r="AA16" s="9"/>
+      <c r="AB16" s="9"/>
+      <c r="AC16" s="9"/>
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A17" s="16"/>
@@ -3212,32 +3588,30 @@
         <v>12</v>
       </c>
       <c r="H17" s="7"/>
-      <c r="I17" s="4" t="s">
+      <c r="I17" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="J17" s="7">
+      <c r="J17" s="40">
         <v>13</v>
       </c>
-      <c r="M17" s="15" t="s">
-        <v>54</v>
-      </c>
+      <c r="K17" s="41"/>
+      <c r="L17" s="41"/>
+      <c r="M17" s="41" t="s">
+        <v>126</v>
+      </c>
+      <c r="N17" s="41"/>
+      <c r="O17" s="41"/>
       <c r="P17" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="V17" s="25">
-        <v>2</v>
-      </c>
-      <c r="W17" s="25">
-        <v>2</v>
-      </c>
-      <c r="X17" s="26" t="s">
-        <v>113</v>
-      </c>
-      <c r="Y17" s="26"/>
-      <c r="Z17" s="26"/>
-      <c r="AA17" s="26"/>
-      <c r="AB17" s="26"/>
-      <c r="AC17" s="26"/>
+        <v>117</v>
+      </c>
+      <c r="V17" s="27"/>
+      <c r="W17" s="27"/>
+      <c r="X17" s="9"/>
+      <c r="Y17" s="9"/>
+      <c r="Z17" s="9"/>
+      <c r="AA17" s="9"/>
+      <c r="AB17" s="9"/>
+      <c r="AC17" s="9"/>
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
@@ -3254,154 +3628,154 @@
       <c r="P18" t="s">
         <v>51</v>
       </c>
-      <c r="V18" s="25">
-        <v>1</v>
-      </c>
-      <c r="W18" s="25">
-        <v>1</v>
-      </c>
-      <c r="X18" s="26" t="s">
-        <v>105</v>
-      </c>
-      <c r="Y18" s="26"/>
-      <c r="Z18" s="26"/>
-      <c r="AA18" s="26"/>
-      <c r="AB18" s="26"/>
-      <c r="AC18" s="26"/>
+      <c r="V18" s="27"/>
+      <c r="W18" s="27"/>
+      <c r="X18" s="9"/>
+      <c r="Y18" s="9"/>
+      <c r="Z18" s="9"/>
+      <c r="AA18" s="9"/>
+      <c r="AB18" s="9"/>
+      <c r="AC18" s="9"/>
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A19" s="8" t="s">
-        <v>62</v>
+      <c r="A19" s="16" t="s">
+        <v>137</v>
       </c>
       <c r="F19" s="15">
         <v>17</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="I19" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I19" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="J19" s="7" t="s">
+      <c r="J19" s="40" t="s">
         <v>51</v>
       </c>
+      <c r="K19" s="41"/>
+      <c r="L19" s="41"/>
+      <c r="M19" s="41"/>
+      <c r="N19" s="41"/>
+      <c r="O19" s="41"/>
       <c r="P19" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="V19" s="25">
-        <v>1</v>
-      </c>
-      <c r="W19" s="25">
-        <v>1</v>
-      </c>
-      <c r="X19" s="26" t="s">
-        <v>109</v>
-      </c>
-      <c r="Y19" s="26"/>
-      <c r="Z19" s="26"/>
-      <c r="AA19" s="26"/>
-      <c r="AB19" s="26"/>
-      <c r="AC19" s="26"/>
+        <v>127</v>
+      </c>
+      <c r="V19" s="27"/>
+      <c r="W19" s="27"/>
+      <c r="X19" s="9"/>
+      <c r="Y19" s="9"/>
+      <c r="Z19" s="9"/>
+      <c r="AA19" s="9"/>
+      <c r="AB19" s="9"/>
+      <c r="AC19" s="9"/>
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>62</v>
+      <c r="A20" s="16" t="s">
+        <v>138</v>
       </c>
       <c r="F20" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="G20" s="3" t="s">
+      <c r="G20" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="H20" s="7"/>
-      <c r="I20" s="4">
+      <c r="H20" s="51" t="s">
+        <v>134</v>
+      </c>
+      <c r="I20" s="47">
         <v>24</v>
       </c>
-      <c r="J20" s="7">
+      <c r="J20" s="48">
         <v>24</v>
       </c>
-      <c r="K20" s="15" t="s">
+      <c r="K20" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="P20" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="V20" s="25">
-        <v>1</v>
-      </c>
-      <c r="W20" s="25">
-        <v>1</v>
-      </c>
-      <c r="X20" s="26" t="s">
-        <v>111</v>
-      </c>
-      <c r="Y20" s="26"/>
-      <c r="Z20" s="26"/>
-      <c r="AA20" s="26"/>
-      <c r="AB20" s="26"/>
-      <c r="AC20" s="26"/>
+      <c r="L20" s="27"/>
+      <c r="M20" s="27"/>
+      <c r="N20" s="27"/>
+      <c r="O20" s="27"/>
+      <c r="P20" s="16"/>
+      <c r="V20" s="27"/>
+      <c r="W20" s="27"/>
+      <c r="X20" s="9"/>
+      <c r="Y20" s="9"/>
+      <c r="Z20" s="9"/>
+      <c r="AA20" s="9"/>
+      <c r="AB20" s="9"/>
+      <c r="AC20" s="9"/>
     </row>
     <row r="21" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A21" s="30" t="s">
-        <v>121</v>
+      <c r="A21" s="16" t="s">
+        <v>139</v>
       </c>
       <c r="F21" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="G21" s="3" t="s">
+      <c r="G21" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="H21" s="7"/>
-      <c r="I21" s="4">
+      <c r="H21" s="51" t="s">
+        <v>135</v>
+      </c>
+      <c r="I21" s="47">
         <v>25</v>
       </c>
-      <c r="J21" s="7">
+      <c r="J21" s="48">
         <v>25</v>
       </c>
-      <c r="K21" s="15" t="s">
+      <c r="K21" s="27" t="s">
         <v>43</v>
       </c>
+      <c r="L21" s="27"/>
+      <c r="M21" s="27"/>
+      <c r="N21" s="27"/>
+      <c r="O21" s="27"/>
       <c r="P21" s="16"/>
-      <c r="V21" s="25"/>
-      <c r="W21" s="25"/>
-      <c r="X21" s="26"/>
-      <c r="Y21" s="26"/>
-      <c r="Z21" s="26"/>
-      <c r="AA21" s="26"/>
-      <c r="AB21" s="26"/>
-      <c r="AC21" s="26"/>
+      <c r="V21" s="27"/>
+      <c r="W21" s="27"/>
+      <c r="X21" s="9"/>
+      <c r="Y21" s="9"/>
+      <c r="Z21" s="9"/>
+      <c r="AA21" s="9"/>
+      <c r="AB21" s="9"/>
+      <c r="AC21" s="9"/>
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>135</v>
-      </c>
+      <c r="A22" s="16"/>
       <c r="F22" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="3" t="s">
+      <c r="G22" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="H22" s="7"/>
-      <c r="I22" s="4" t="s">
+      <c r="H22" s="51" t="s">
+        <v>136</v>
+      </c>
+      <c r="I22" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="J22" s="7"/>
-      <c r="P22" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="V22" s="25"/>
-      <c r="W22" s="25"/>
-      <c r="X22" s="26"/>
-      <c r="Y22" s="26"/>
-      <c r="Z22" s="26"/>
-      <c r="AA22" s="26"/>
-      <c r="AB22" s="26"/>
-      <c r="AC22" s="26"/>
+      <c r="J22" s="37"/>
+      <c r="K22" s="26"/>
+      <c r="L22" s="26"/>
+      <c r="M22" s="26"/>
+      <c r="N22" s="26"/>
+      <c r="O22" s="26"/>
+      <c r="P22" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="V22" s="27"/>
+      <c r="W22" s="27"/>
+      <c r="X22" s="9"/>
+      <c r="Y22" s="9"/>
+      <c r="Z22" s="9"/>
+      <c r="AA22" s="9"/>
+      <c r="AB22" s="9"/>
+      <c r="AC22" s="9"/>
     </row>
     <row r="23" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
-        <v>62</v>
-      </c>
+      <c r="A23" s="16"/>
       <c r="F23" s="15">
         <v>26</v>
       </c>
@@ -3414,185 +3788,851 @@
       <c r="P23" t="s">
         <v>51</v>
       </c>
-      <c r="V23" s="25">
-        <f>SUM(V7:V22)</f>
-        <v>26</v>
-      </c>
-      <c r="W23" s="28">
-        <f>SUM(W7:W22)</f>
-        <v>9</v>
-      </c>
-      <c r="X23" s="26" t="s">
-        <v>108</v>
-      </c>
-      <c r="Y23" s="26"/>
-      <c r="Z23" s="26"/>
-      <c r="AA23" s="26"/>
-      <c r="AB23" s="26"/>
-      <c r="AC23" s="26"/>
+      <c r="V23" s="27"/>
+      <c r="W23" s="29"/>
+      <c r="X23" s="9"/>
+      <c r="Y23" s="9"/>
+      <c r="Z23" s="9"/>
+      <c r="AA23" s="9"/>
+      <c r="AB23" s="9"/>
+      <c r="AC23" s="9"/>
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="V24" s="25"/>
-      <c r="W24" s="25"/>
-      <c r="X24" s="26"/>
-      <c r="Y24" s="26"/>
-      <c r="Z24" s="26"/>
-      <c r="AA24" s="26"/>
-      <c r="AB24" s="26"/>
-      <c r="AC24" s="26"/>
+      <c r="V24" s="27"/>
+      <c r="W24" s="27"/>
+      <c r="X24" s="9"/>
+      <c r="Y24" s="9"/>
+      <c r="Z24" s="9"/>
+      <c r="AA24" s="9"/>
+      <c r="AB24" s="9"/>
+      <c r="AC24" s="9"/>
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.2">
       <c r="H25" s="10"/>
-      <c r="V25" s="25"/>
-      <c r="W25" s="25"/>
-      <c r="X25" s="26"/>
-      <c r="Y25" s="26"/>
-      <c r="Z25" s="26"/>
-      <c r="AA25" s="26"/>
-      <c r="AB25" s="26"/>
-      <c r="AC25" s="26"/>
+      <c r="V25" s="27"/>
+      <c r="W25" s="27"/>
+      <c r="X25" s="9"/>
+      <c r="Y25" s="9"/>
+      <c r="Z25" s="9"/>
+      <c r="AA25" s="9"/>
+      <c r="AB25" s="9"/>
+      <c r="AC25" s="9"/>
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A26" s="10"/>
-      <c r="G26" s="10"/>
-      <c r="V26" s="25"/>
-      <c r="W26" s="25"/>
-      <c r="X26" s="26"/>
-      <c r="Y26" s="26"/>
-      <c r="Z26" s="26"/>
-      <c r="AA26" s="26"/>
-      <c r="AB26" s="26"/>
-      <c r="AC26" s="26"/>
+      <c r="A26" t="s">
+        <v>99</v>
+      </c>
+      <c r="V26" s="27"/>
+      <c r="W26" s="27"/>
+      <c r="X26" s="9"/>
+      <c r="Y26" s="9"/>
+      <c r="Z26" s="9"/>
+      <c r="AA26" s="9"/>
+      <c r="AB26" s="9"/>
+      <c r="AC26" s="9"/>
     </row>
     <row r="27" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A27" s="11"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="11"/>
-    </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A28" s="11"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="11"/>
+      <c r="A27" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="G27" s="8"/>
+      <c r="H27" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="I27" s="8"/>
+    </row>
+    <row r="28" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E28" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="G28" t="s">
+        <v>5</v>
+      </c>
+      <c r="I28" t="s">
+        <v>5</v>
+      </c>
+      <c r="J28" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="K28" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="L28" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="M28" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="N28" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="O28" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="P28" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q28" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="R28" t="s">
+        <v>111</v>
+      </c>
+      <c r="S28" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="T28" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="29" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A29" s="11"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="11"/>
+      <c r="A29" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="B29" s="34"/>
+      <c r="C29" s="34"/>
+      <c r="D29" s="34"/>
+      <c r="E29" s="34"/>
+      <c r="F29" s="34"/>
+      <c r="G29" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="I29" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="J29" s="37"/>
+      <c r="K29" s="26"/>
+      <c r="L29" s="26"/>
+      <c r="M29" s="26"/>
+      <c r="N29" s="26"/>
+      <c r="O29" s="26"/>
+      <c r="P29" s="38" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="30" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A30" s="11"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="11"/>
+      <c r="A30" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="B30" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E30" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F30" s="15">
+        <v>0</v>
+      </c>
+      <c r="G30" s="3">
+        <v>0</v>
+      </c>
+      <c r="H30" s="7"/>
+      <c r="I30" s="32" t="s">
+        <v>133</v>
+      </c>
+      <c r="J30" s="35"/>
+      <c r="K30" s="34"/>
+      <c r="L30" s="34"/>
+      <c r="M30" s="34"/>
+      <c r="N30" s="34"/>
+      <c r="O30" s="34"/>
+      <c r="P30" s="30" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="31" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A31" s="11"/>
-      <c r="G31" s="11"/>
-      <c r="H31" s="11"/>
+      <c r="A31" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E31" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F31" s="15">
+        <v>1</v>
+      </c>
+      <c r="G31" s="3">
+        <v>1</v>
+      </c>
+      <c r="H31" s="7"/>
+      <c r="I31" s="42" t="s">
+        <v>129</v>
+      </c>
+      <c r="J31" s="37"/>
+      <c r="K31" s="26"/>
+      <c r="L31" s="26"/>
+      <c r="M31" s="26"/>
+      <c r="N31" s="26"/>
+      <c r="O31" s="26"/>
+      <c r="P31" s="25" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="32" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A32" s="11"/>
-      <c r="G32" s="11"/>
-      <c r="H32" s="11"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" s="11"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="11"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" s="11"/>
-      <c r="G34" s="11"/>
-      <c r="H34" s="11"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" s="11"/>
-      <c r="G35" s="11"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36" s="11"/>
-      <c r="G36" s="11"/>
-      <c r="H36" s="11"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" s="11"/>
-      <c r="G37" s="11"/>
-      <c r="H37" s="11"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" s="11"/>
-      <c r="G38" s="11"/>
-      <c r="H38" s="11"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39" s="11"/>
-      <c r="G39" s="11"/>
-      <c r="H39" s="11"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A40" s="11"/>
-      <c r="G40" s="11"/>
-      <c r="H40" s="11"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A41" s="11"/>
-      <c r="G41" s="11"/>
-      <c r="H41" s="11"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A42" s="11"/>
-      <c r="G42" s="11"/>
-      <c r="H42" s="11"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A43" s="11"/>
-      <c r="G43" s="11"/>
-      <c r="H43" s="11"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A44" s="11"/>
-      <c r="G44" s="11"/>
-      <c r="H44" s="11"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="G45" s="11"/>
-      <c r="H45" s="11"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="G46" s="11"/>
-      <c r="H46" s="11"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="G47" s="11"/>
-      <c r="H47" s="11"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="G48" s="11"/>
-      <c r="H48" s="11"/>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
+      <c r="A32" s="16"/>
+      <c r="F32" s="15">
+        <v>2</v>
+      </c>
+      <c r="G32" s="3">
+        <v>2</v>
+      </c>
+      <c r="H32" s="7"/>
+      <c r="I32" s="4">
+        <v>23</v>
+      </c>
+      <c r="J32" s="7">
+        <v>23</v>
+      </c>
+      <c r="K32" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="N32" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="O32" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="P32" s="20" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A33" s="16"/>
+      <c r="C33" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E33" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="F33" s="15">
+        <v>3</v>
+      </c>
+      <c r="G33" s="3">
+        <v>3</v>
+      </c>
+      <c r="H33" s="7"/>
+      <c r="I33" s="4">
+        <v>22</v>
+      </c>
+      <c r="J33" s="7">
+        <v>22</v>
+      </c>
+      <c r="K33" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="N33" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="O33" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="P33" s="20" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A34" s="16"/>
+      <c r="C34" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E34" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="F34" s="15">
+        <v>4</v>
+      </c>
+      <c r="G34" s="3">
+        <v>4</v>
+      </c>
+      <c r="H34" s="7"/>
+      <c r="I34" s="39">
+        <v>21</v>
+      </c>
+      <c r="J34" s="40">
+        <v>21</v>
+      </c>
+      <c r="K34" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="L34" s="41"/>
+      <c r="M34" s="41" t="s">
+        <v>124</v>
+      </c>
+      <c r="N34" s="41" t="s">
+        <v>2</v>
+      </c>
+      <c r="O34" s="41"/>
+      <c r="P34" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A35" s="16"/>
+      <c r="C35" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="F35" s="15">
+        <v>5</v>
+      </c>
+      <c r="G35" s="3">
+        <v>5</v>
+      </c>
+      <c r="H35" s="7"/>
+      <c r="I35" s="4">
+        <v>20</v>
+      </c>
+      <c r="J35" s="7">
+        <v>20</v>
+      </c>
+      <c r="K35" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="M35" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="N35" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="P35" s="16"/>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A36" s="16"/>
+      <c r="C36" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="F36" s="15">
+        <v>6</v>
+      </c>
+      <c r="G36" s="3">
+        <v>6</v>
+      </c>
+      <c r="H36" s="7"/>
+      <c r="I36" s="39">
+        <v>19</v>
+      </c>
+      <c r="J36" s="40">
+        <v>19</v>
+      </c>
+      <c r="K36" s="41" t="s">
+        <v>31</v>
+      </c>
+      <c r="L36" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="M36" s="41"/>
+      <c r="N36" s="41"/>
+      <c r="O36" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="P36" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q36" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="R36" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="S36" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="T36" s="8" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A37" s="16"/>
+      <c r="E37" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="F37" s="15">
+        <v>7</v>
+      </c>
+      <c r="G37" s="3">
+        <v>7</v>
+      </c>
+      <c r="H37" s="7"/>
+      <c r="I37" s="39">
+        <v>18</v>
+      </c>
+      <c r="J37" s="40">
+        <v>18</v>
+      </c>
+      <c r="K37" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="L37" s="41" t="s">
+        <v>44</v>
+      </c>
+      <c r="M37" s="41"/>
+      <c r="N37" s="41"/>
+      <c r="O37" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="P37" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q37" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="R37" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="S37" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="T37" s="8" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A38" s="16"/>
+      <c r="E38" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F38" s="15">
+        <v>8</v>
+      </c>
+      <c r="G38" s="3">
+        <v>8</v>
+      </c>
+      <c r="H38" s="7"/>
+      <c r="I38" s="4">
+        <v>17</v>
+      </c>
+      <c r="J38" s="7">
+        <v>17</v>
+      </c>
+      <c r="K38" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="L38" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="N38" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="O38" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="P38" s="16"/>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A39" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="C39" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E39" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="F39" s="15">
+        <v>9</v>
+      </c>
+      <c r="G39" s="3">
+        <v>9</v>
+      </c>
+      <c r="H39" s="7"/>
+      <c r="I39" s="4">
+        <v>16</v>
+      </c>
+      <c r="J39" s="7">
+        <v>16</v>
+      </c>
+      <c r="K39" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="L39" s="43" t="s">
+        <v>40</v>
+      </c>
+      <c r="N39" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="O39" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="P39" s="16"/>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A40" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="C40" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D40" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E40" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F40" s="15">
+        <v>10</v>
+      </c>
+      <c r="G40" s="3">
+        <v>10</v>
+      </c>
+      <c r="H40" s="7"/>
+      <c r="I40" s="4">
+        <v>15</v>
+      </c>
+      <c r="J40" s="7">
+        <v>15</v>
+      </c>
+      <c r="K40" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="O40" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="P40" s="16"/>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A41" s="16"/>
+      <c r="D41" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="F41" s="15">
+        <v>11</v>
+      </c>
+      <c r="G41" s="3">
+        <v>11</v>
+      </c>
+      <c r="H41" s="7"/>
+      <c r="I41" s="39">
+        <v>14</v>
+      </c>
+      <c r="J41" s="40">
+        <v>14</v>
+      </c>
+      <c r="K41" s="41" t="s">
+        <v>36</v>
+      </c>
+      <c r="L41" s="41"/>
+      <c r="M41" s="41"/>
+      <c r="N41" s="41"/>
+      <c r="O41" s="41"/>
+      <c r="P41" s="8" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A42" s="16"/>
+      <c r="D42" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="F42" s="15">
+        <v>12</v>
+      </c>
+      <c r="G42" s="3">
+        <v>12</v>
+      </c>
+      <c r="H42" s="7"/>
+      <c r="I42" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="J42" s="40">
+        <v>13</v>
+      </c>
+      <c r="K42" s="41"/>
+      <c r="L42" s="41"/>
+      <c r="M42" s="41" t="s">
+        <v>126</v>
+      </c>
+      <c r="N42" s="41"/>
+      <c r="O42" s="41"/>
+      <c r="P42" s="8" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>51</v>
+      </c>
+      <c r="G43" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="H43" s="13"/>
+      <c r="I43" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="J43" s="7"/>
+      <c r="P43" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A44" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="F44" s="15">
+        <v>17</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="I44" s="39" t="s">
+        <v>10</v>
+      </c>
+      <c r="J44" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="K44" s="41"/>
+      <c r="L44" s="41"/>
+      <c r="M44" s="41"/>
+      <c r="N44" s="41"/>
+      <c r="O44" s="41"/>
+      <c r="P44" s="8" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A45" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="F45" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="G45" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="H45" s="51" t="s">
+        <v>134</v>
+      </c>
+      <c r="I45" s="47">
+        <v>24</v>
+      </c>
+      <c r="J45" s="48">
+        <v>24</v>
+      </c>
+      <c r="K45" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="L45" s="27"/>
+      <c r="M45" s="27"/>
+      <c r="N45" s="27"/>
+      <c r="O45" s="27"/>
+      <c r="P45" s="16"/>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A46" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="F46" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="G46" s="50" t="s">
+        <v>4</v>
+      </c>
+      <c r="H46" s="51" t="s">
+        <v>135</v>
+      </c>
+      <c r="I46" s="47">
+        <v>25</v>
+      </c>
+      <c r="J46" s="48">
+        <v>25</v>
+      </c>
+      <c r="K46" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="L46" s="27"/>
+      <c r="M46" s="27"/>
+      <c r="N46" s="27"/>
+      <c r="O46" s="27"/>
+      <c r="P46" s="16"/>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A47" s="16"/>
+      <c r="F47" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="G47" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="H47" s="51" t="s">
+        <v>136</v>
+      </c>
+      <c r="I47" s="42" t="s">
+        <v>66</v>
+      </c>
+      <c r="J47" s="37"/>
+      <c r="K47" s="26"/>
+      <c r="L47" s="26"/>
+      <c r="M47" s="26"/>
+      <c r="N47" s="26"/>
+      <c r="O47" s="26"/>
+      <c r="P47" s="25" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="16"/>
+      <c r="F48" s="15">
+        <v>26</v>
+      </c>
+      <c r="G48" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="H48" s="14"/>
+      <c r="I48" s="6"/>
+      <c r="J48" s="7"/>
+      <c r="P48" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="49" spans="9:21" x14ac:dyDescent="0.2">
+      <c r="I49" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="K49" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="P49" s="16"/>
+    </row>
+    <row r="50" spans="9:21" x14ac:dyDescent="0.2">
+      <c r="I50" s="45" t="s">
+        <v>131</v>
+      </c>
+      <c r="K50" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="P50" s="16"/>
+      <c r="U50" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
+    <row r="51" spans="9:21" x14ac:dyDescent="0.2">
+      <c r="I51" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="P51" s="16"/>
+      <c r="U51" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
+    <row r="52" spans="9:21" x14ac:dyDescent="0.2">
+      <c r="I52" s="45" t="s">
+        <v>6</v>
+      </c>
+      <c r="P52" s="16"/>
+      <c r="U52" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
+    <row r="53" spans="9:21" x14ac:dyDescent="0.2">
+      <c r="I53" s="45">
+        <v>24</v>
+      </c>
+      <c r="J53" s="15">
+        <v>24</v>
+      </c>
+      <c r="P53" s="16"/>
+      <c r="U53" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
+    <row r="54" spans="9:21" x14ac:dyDescent="0.2">
+      <c r="I54" s="45">
+        <v>25</v>
+      </c>
+      <c r="J54" s="15">
+        <v>25</v>
+      </c>
+      <c r="P54" s="16"/>
+      <c r="U54" t="s">
         <v>95</v>
       </c>
+    </row>
+    <row r="55" spans="9:21" x14ac:dyDescent="0.2">
+      <c r="I55" s="45">
+        <v>26</v>
+      </c>
+      <c r="J55" s="15">
+        <v>26</v>
+      </c>
+      <c r="P55" s="16"/>
+    </row>
+    <row r="56" spans="9:21" x14ac:dyDescent="0.2">
+      <c r="I56" s="45">
+        <v>27</v>
+      </c>
+      <c r="J56" s="15">
+        <v>27</v>
+      </c>
+      <c r="P56" s="16"/>
+    </row>
+    <row r="57" spans="9:21" x14ac:dyDescent="0.2">
+      <c r="I57" s="45">
+        <v>28</v>
+      </c>
+      <c r="J57" s="15">
+        <v>28</v>
+      </c>
+      <c r="P57" s="16"/>
+    </row>
+    <row r="58" spans="9:21" x14ac:dyDescent="0.2">
+      <c r="I58" s="45">
+        <v>29</v>
+      </c>
+      <c r="J58" s="15">
+        <v>29</v>
+      </c>
+      <c r="P58" s="16"/>
+    </row>
+    <row r="59" spans="9:21" x14ac:dyDescent="0.2">
+      <c r="I59" s="45">
+        <v>30</v>
+      </c>
+      <c r="J59" s="15">
+        <v>30</v>
+      </c>
+      <c r="P59" s="16"/>
+    </row>
+    <row r="60" spans="9:21" x14ac:dyDescent="0.2">
+      <c r="I60" s="45">
+        <v>31</v>
+      </c>
+      <c r="J60" s="15">
+        <v>31</v>
+      </c>
+      <c r="P60" s="16"/>
+    </row>
+    <row r="61" spans="9:21" x14ac:dyDescent="0.2">
+      <c r="I61" s="45">
+        <v>32</v>
+      </c>
+      <c r="J61" s="15">
+        <v>32</v>
+      </c>
+      <c r="P61" s="16"/>
+    </row>
+    <row r="62" spans="9:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I62" s="46">
+        <v>33</v>
+      </c>
+      <c r="J62" s="15">
+        <v>33</v>
+      </c>
+      <c r="P62" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3600,9 +4640,10 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{CF74EE04-8972-D048-A403-865EBF5C5826}"/>
+    <hyperlink ref="A27" r:id="rId1" xr:uid="{CF74EE04-8972-D048-A403-865EBF5C5826}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{5F2D9B69-2151-9947-A08D-C8EC4C5057AC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Configure IO expanders and I2C addresses
</commit_message>
<xml_diff>
--- a/Electronic Design/Core 64 Pin Usage Mapping.xlsx
+++ b/Electronic Design/Core 64 Pin Usage Mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1c02d23ac1278198/00_MBP2011-Documents/Electronics/Core 64 Interactive Badge/Core-64-Interactive-Core-Memory-Badge/Electronic Design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="293" documentId="114_{C854064A-3C16-0445-B75C-033646BE2CC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{48C22F0B-A1D8-4E4E-971A-18946189BD53}"/>
+  <xr:revisionPtr revIDLastSave="298" documentId="114_{C854064A-3C16-0445-B75C-033646BE2CC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{11C3D507-05CC-254B-820E-CE11EF77A75C}"/>
   <bookViews>
-    <workbookView xWindow="-33020" yWindow="-10340" windowWidth="32480" windowHeight="28340" activeTab="2" xr2:uid="{A4752792-CA31-B046-B883-84F8D68A57EC}"/>
+    <workbookView xWindow="-33060" yWindow="-10340" windowWidth="32480" windowHeight="28340" activeTab="2" xr2:uid="{A4752792-CA31-B046-B883-84F8D68A57EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Reference Pinouts" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="150">
   <si>
     <t>Custom</t>
   </si>
@@ -473,6 +473,18 @@
   </si>
   <si>
     <t>SAO Port 1, GPIO 1 (TX)</t>
+  </si>
+  <si>
+    <t>IOEXP_ID32_INT_A</t>
+  </si>
+  <si>
+    <t>IOEXP_ID32_INT_B</t>
+  </si>
+  <si>
+    <t>IOEXP_ID33_INT_A</t>
+  </si>
+  <si>
+    <t>IOEXP_ID33_INT_B</t>
   </si>
 </sst>
 </file>
@@ -859,13 +871,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2923,8 +2935,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CBC2977-27CE-C64F-BE79-A69FB2535F84}">
   <dimension ref="A1:AC62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="117" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="P32" sqref="P32:P33"/>
+    <sheetView tabSelected="1" zoomScale="117" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44:A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3058,13 +3070,13 @@
       <c r="P4" s="38" t="s">
         <v>108</v>
       </c>
-      <c r="V4" s="49"/>
-      <c r="W4" s="49"/>
-      <c r="X4" s="49"/>
-      <c r="Y4" s="49"/>
-      <c r="Z4" s="49"/>
-      <c r="AA4" s="49"/>
-      <c r="AB4" s="49"/>
+      <c r="V4" s="51"/>
+      <c r="W4" s="51"/>
+      <c r="X4" s="51"/>
+      <c r="Y4" s="51"/>
+      <c r="Z4" s="51"/>
+      <c r="AA4" s="51"/>
+      <c r="AB4" s="51"/>
       <c r="AC4" s="9"/>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.2">
@@ -3150,7 +3162,9 @@
       <c r="AC6" s="9"/>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A7" s="16"/>
+      <c r="A7" s="16" t="s">
+        <v>146</v>
+      </c>
       <c r="F7" s="15">
         <v>2</v>
       </c>
@@ -3189,7 +3203,9 @@
       <c r="AC7" s="9"/>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A8" s="16"/>
+      <c r="A8" s="16" t="s">
+        <v>147</v>
+      </c>
       <c r="B8" s="15" t="s">
         <v>26</v>
       </c>
@@ -3234,7 +3250,9 @@
       <c r="AC8" s="9"/>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A9" s="16"/>
+      <c r="A9" s="16" t="s">
+        <v>148</v>
+      </c>
       <c r="B9" s="15" t="s">
         <v>26</v>
       </c>
@@ -3276,7 +3294,9 @@
       <c r="AC9" s="9"/>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A10" s="16"/>
+      <c r="A10" s="16" t="s">
+        <v>149</v>
+      </c>
       <c r="F10" s="15">
         <v>5</v>
       </c>
@@ -3680,7 +3700,7 @@
       <c r="G20" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="H20" s="51" t="s">
+      <c r="H20" s="50" t="s">
         <v>134</v>
       </c>
       <c r="I20" s="47">
@@ -3713,10 +3733,10 @@
       <c r="F21" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="G21" s="50" t="s">
+      <c r="G21" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="H21" s="51" t="s">
+      <c r="H21" s="50" t="s">
         <v>135</v>
       </c>
       <c r="I21" s="47">
@@ -3750,7 +3770,7 @@
       <c r="G22" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="H22" s="51" t="s">
+      <c r="H22" s="50" t="s">
         <v>136</v>
       </c>
       <c r="I22" s="42" t="s">
@@ -3986,7 +4006,9 @@
       </c>
     </row>
     <row r="32" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A32" s="16"/>
+      <c r="A32" s="16" t="s">
+        <v>146</v>
+      </c>
       <c r="F32" s="15">
         <v>2</v>
       </c>
@@ -4014,7 +4036,9 @@
       </c>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A33" s="16"/>
+      <c r="A33" s="16" t="s">
+        <v>147</v>
+      </c>
       <c r="C33" s="15" t="s">
         <v>2</v>
       </c>
@@ -4048,7 +4072,9 @@
       </c>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A34" s="16"/>
+      <c r="A34" s="16" t="s">
+        <v>148</v>
+      </c>
       <c r="C34" s="15" t="s">
         <v>2</v>
       </c>
@@ -4084,7 +4110,9 @@
       </c>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A35" s="16"/>
+      <c r="A35" s="16" t="s">
+        <v>149</v>
+      </c>
       <c r="C35" s="15" t="s">
         <v>2</v>
       </c>
@@ -4414,7 +4442,7 @@
       <c r="G45" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="H45" s="51" t="s">
+      <c r="H45" s="50" t="s">
         <v>134</v>
       </c>
       <c r="I45" s="47">
@@ -4439,10 +4467,10 @@
       <c r="F46" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="G46" s="50" t="s">
+      <c r="G46" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="H46" s="51" t="s">
+      <c r="H46" s="50" t="s">
         <v>135</v>
       </c>
       <c r="I46" s="47">
@@ -4468,7 +4496,7 @@
       <c r="G47" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="H47" s="51" t="s">
+      <c r="H47" s="50" t="s">
         <v>136</v>
       </c>
       <c r="I47" s="42" t="s">

</xml_diff>

<commit_message>
Remove I2CIOESetup() to allow set-up in each driver independently
Pin usage mapping updated with 17 for LED array (was wrong at 14) and 14 is SD Card Clock.
Clean-up #define pin definitions in HardwareIOMap.h for all hardware versions through v0.3.0.
</commit_message>
<xml_diff>
--- a/Electronic Design/Core 64 Pin Usage Mapping.xlsx
+++ b/Electronic Design/Core 64 Pin Usage Mapping.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ageppert/Dropbox/Electronics/Core 64 Interactive Badge/Core-64-Interactive-Core-Memory-Badge/Electronic Design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E9A2E11-B832-9A4D-B277-5921A877226B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AAB0B69-FC3F-FA4E-BE04-8B33E986117F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19620" activeTab="2" xr2:uid="{A4752792-CA31-B046-B883-84F8D68A57EC}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="153">
   <si>
     <t>Custom</t>
   </si>
@@ -491,6 +491,9 @@
   </si>
   <si>
     <t>Interrupt capable: Teensy 3.2 all digital pins.</t>
+  </si>
+  <si>
+    <t>SDCARD CLK</t>
   </si>
 </sst>
 </file>
@@ -753,7 +756,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -883,11 +886,14 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2944,8 +2950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CBC2977-27CE-C64F-BE79-A69FB2535F84}">
   <dimension ref="A1:AC63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="117" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="117" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="I38" sqref="I38:O38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3079,13 +3085,13 @@
       <c r="P4" s="38" t="s">
         <v>108</v>
       </c>
-      <c r="V4" s="51"/>
-      <c r="W4" s="51"/>
-      <c r="X4" s="51"/>
-      <c r="Y4" s="51"/>
-      <c r="Z4" s="51"/>
-      <c r="AA4" s="51"/>
-      <c r="AB4" s="51"/>
+      <c r="V4" s="52"/>
+      <c r="W4" s="52"/>
+      <c r="X4" s="52"/>
+      <c r="Y4" s="52"/>
+      <c r="Z4" s="52"/>
+      <c r="AA4" s="52"/>
+      <c r="AB4" s="52"/>
       <c r="AC4" s="9"/>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.2">
@@ -3459,22 +3465,26 @@
         <v>8</v>
       </c>
       <c r="H13" s="7"/>
-      <c r="I13" s="4">
+      <c r="I13" s="39">
         <v>17</v>
       </c>
-      <c r="J13" s="7">
+      <c r="J13" s="40">
         <v>17</v>
       </c>
-      <c r="K13" s="15" t="s">
+      <c r="K13" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="N13" s="15" t="s">
+      <c r="L13" s="41"/>
+      <c r="M13" s="41"/>
+      <c r="N13" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="O13" s="15" t="s">
+      <c r="O13" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="P13" s="16"/>
+      <c r="P13" s="8" t="s">
+        <v>119</v>
+      </c>
       <c r="V13" s="27"/>
       <c r="W13" s="27"/>
       <c r="X13" s="9"/>
@@ -3594,7 +3604,7 @@
       <c r="N16" s="41"/>
       <c r="O16" s="41"/>
       <c r="P16" s="8" t="s">
-        <v>119</v>
+        <v>152</v>
       </c>
       <c r="V16" s="27"/>
       <c r="W16" s="27"/>
@@ -3828,7 +3838,7 @@
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.2">
       <c r="F24" s="7"/>
-      <c r="G24" s="52" t="s">
+      <c r="G24" s="51" t="s">
         <v>150</v>
       </c>
       <c r="V24" s="27"/>
@@ -4255,25 +4265,28 @@
         <v>8</v>
       </c>
       <c r="H38" s="7"/>
-      <c r="I38" s="4">
+      <c r="I38" s="39">
         <v>17</v>
       </c>
-      <c r="J38" s="7">
+      <c r="J38" s="40">
         <v>17</v>
       </c>
-      <c r="K38" s="15" t="s">
+      <c r="K38" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="L38" s="43" t="s">
+      <c r="L38" s="53" t="s">
         <v>39</v>
       </c>
-      <c r="N38" s="15" t="s">
+      <c r="M38" s="41"/>
+      <c r="N38" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="O38" s="15" t="s">
+      <c r="O38" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="P38" s="16"/>
+      <c r="P38" s="8" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A39" s="20" t="s">
@@ -4372,7 +4385,7 @@
       <c r="N41" s="41"/>
       <c r="O41" s="41"/>
       <c r="P41" s="8" t="s">
-        <v>119</v>
+        <v>152</v>
       </c>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.2">
@@ -4676,7 +4689,7 @@
       <c r="P62" s="16"/>
     </row>
     <row r="63" spans="7:21" x14ac:dyDescent="0.2">
-      <c r="G63" s="52" t="s">
+      <c r="G63" s="51" t="s">
         <v>151</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Bring core array enable pin alive with IO Expander
</commit_message>
<xml_diff>
--- a/Electronic Design/Core 64 Pin Usage Mapping.xlsx
+++ b/Electronic Design/Core 64 Pin Usage Mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ageppert/Dropbox/Electronics/Core 64 Interactive Badge/Core-64-Interactive-Core-Memory-Badge/Electronic Design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AAB0B69-FC3F-FA4E-BE04-8B33E986117F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF3BE4D2-860D-3848-A6DC-9A4461ED5B38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19620" activeTab="2" xr2:uid="{A4752792-CA31-B046-B883-84F8D68A57EC}"/>
   </bookViews>
@@ -475,18 +475,6 @@
     <t>SAO Port 1, GPIO 1 (TX)</t>
   </si>
   <si>
-    <t>IOEXP_ID32_INT_A</t>
-  </si>
-  <si>
-    <t>IOEXP_ID32_INT_B</t>
-  </si>
-  <si>
-    <t>IOEXP_ID33_INT_A</t>
-  </si>
-  <si>
-    <t>IOEXP_ID33_INT_B</t>
-  </si>
-  <si>
     <t>Interrupt capable: Teensy LC 2 - 12, 14, 15, 20 - 23</t>
   </si>
   <si>
@@ -494,6 +482,18 @@
   </si>
   <si>
     <t>SDCARD CLK</t>
+  </si>
+  <si>
+    <t>IOEXP_ID38_INT_A</t>
+  </si>
+  <si>
+    <t>IOEXP_ID38_INT_B</t>
+  </si>
+  <si>
+    <t>IOEXP_ID39_INT_A</t>
+  </si>
+  <si>
+    <t>IOEXP_ID39_INT_B</t>
   </si>
 </sst>
 </file>
@@ -889,10 +889,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2950,8 +2950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CBC2977-27CE-C64F-BE79-A69FB2535F84}">
   <dimension ref="A1:AC63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="117" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="I38" sqref="I38:O38"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="117" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32:A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3085,13 +3085,13 @@
       <c r="P4" s="38" t="s">
         <v>108</v>
       </c>
-      <c r="V4" s="52"/>
-      <c r="W4" s="52"/>
-      <c r="X4" s="52"/>
-      <c r="Y4" s="52"/>
-      <c r="Z4" s="52"/>
-      <c r="AA4" s="52"/>
-      <c r="AB4" s="52"/>
+      <c r="V4" s="53"/>
+      <c r="W4" s="53"/>
+      <c r="X4" s="53"/>
+      <c r="Y4" s="53"/>
+      <c r="Z4" s="53"/>
+      <c r="AA4" s="53"/>
+      <c r="AB4" s="53"/>
       <c r="AC4" s="9"/>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.2">
@@ -3178,7 +3178,7 @@
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A7" s="16" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="F7" s="15">
         <v>2</v>
@@ -3219,7 +3219,7 @@
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="B8" s="15" t="s">
         <v>26</v>
@@ -3266,7 +3266,7 @@
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A9" s="16" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="B9" s="15" t="s">
         <v>26</v>
@@ -3310,7 +3310,7 @@
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="F10" s="15">
         <v>5</v>
@@ -3604,7 +3604,7 @@
       <c r="N16" s="41"/>
       <c r="O16" s="41"/>
       <c r="P16" s="8" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="V16" s="27"/>
       <c r="W16" s="27"/>
@@ -3839,7 +3839,7 @@
     <row r="24" spans="1:29" x14ac:dyDescent="0.2">
       <c r="F24" s="7"/>
       <c r="G24" s="51" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="V24" s="27"/>
       <c r="W24" s="27"/>
@@ -4030,7 +4030,7 @@
     </row>
     <row r="32" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A32" s="16" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="F32" s="15">
         <v>2</v>
@@ -4060,7 +4060,7 @@
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A33" s="16" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="C33" s="15" t="s">
         <v>2</v>
@@ -4096,7 +4096,7 @@
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A34" s="16" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C34" s="15" t="s">
         <v>2</v>
@@ -4134,7 +4134,7 @@
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A35" s="16" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="C35" s="15" t="s">
         <v>2</v>
@@ -4274,7 +4274,7 @@
       <c r="K38" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="L38" s="53" t="s">
+      <c r="L38" s="52" t="s">
         <v>39</v>
       </c>
       <c r="M38" s="41"/>
@@ -4385,7 +4385,7 @@
       <c r="N41" s="41"/>
       <c r="O41" s="41"/>
       <c r="P41" s="8" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.2">
@@ -4690,7 +4690,7 @@
     </row>
     <row r="63" spans="7:21" x14ac:dyDescent="0.2">
       <c r="G63" s="51" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Test analog input for hall switch.
</commit_message>
<xml_diff>
--- a/Electronic Design/Core 64 Pin Usage Mapping.xlsx
+++ b/Electronic Design/Core 64 Pin Usage Mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ageppert/Dropbox/Electronics/Core 64 Interactive Badge/Core-64-Interactive-Core-Memory-Badge/Electronic Design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B804AA5-7401-AD41-8603-7B8DE7F02E9A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6860B26C-2E85-6A4F-8BFF-D150D2E9028A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="27480" activeTab="1" xr2:uid="{A4752792-CA31-B046-B883-84F8D68A57EC}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="179">
   <si>
     <t>Custom</t>
   </si>
@@ -531,9 +531,6 @@
     <t>HALL 3</t>
   </si>
   <si>
-    <t>SAO 1</t>
-  </si>
-  <si>
     <t>SPARE ANALOG (or pseudo digital input)</t>
   </si>
   <si>
@@ -562,6 +559,18 @@
   </si>
   <si>
     <t>TFT ILI9341 BACKLIGHT LED BRIGHTNESS</t>
+  </si>
+  <si>
+    <t>SAO Port 1&amp;2, GPIO 2 (RX)</t>
+  </si>
+  <si>
+    <t>SAO Port 1&amp;2, GPIO 1 (TX)</t>
+  </si>
+  <si>
+    <t>SAO 1&amp;2</t>
+  </si>
+  <si>
+    <t>Testing hall sensor 2</t>
   </si>
 </sst>
 </file>
@@ -948,9 +957,6 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -967,6 +973,9 @@
     <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2241,8 +2250,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CBC2977-27CE-C64F-BE79-A69FB2535F84}">
   <dimension ref="A1:AC90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="117" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="R71" sqref="R71"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="117" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="P35" sqref="P35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3001,13 +3010,13 @@
       <c r="P31" s="36" t="s">
         <v>107</v>
       </c>
-      <c r="V31" s="47"/>
-      <c r="W31" s="47"/>
-      <c r="X31" s="47"/>
-      <c r="Y31" s="47"/>
-      <c r="Z31" s="47"/>
-      <c r="AA31" s="47"/>
-      <c r="AB31" s="47"/>
+      <c r="V31" s="54"/>
+      <c r="W31" s="54"/>
+      <c r="X31" s="54"/>
+      <c r="Y31" s="54"/>
+      <c r="Z31" s="54"/>
+      <c r="AA31" s="54"/>
+      <c r="AB31" s="54"/>
       <c r="AC31" s="9"/>
     </row>
     <row r="32" spans="1:29" x14ac:dyDescent="0.2">
@@ -3127,7 +3136,9 @@
       <c r="O34" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="P34" s="19"/>
+      <c r="P34" s="19" t="s">
+        <v>178</v>
+      </c>
       <c r="V34" s="26"/>
       <c r="W34" s="26"/>
       <c r="X34" s="9"/>
@@ -3508,7 +3519,7 @@
         <v>26</v>
       </c>
       <c r="P42" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="V42" s="26"/>
       <c r="W42" s="26"/>
@@ -3924,7 +3935,7 @@
     </row>
     <row r="57" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A57" s="8" t="s">
-        <v>137</v>
+        <v>175</v>
       </c>
       <c r="B57" s="14" t="s">
         <v>26</v>
@@ -3954,7 +3965,7 @@
     </row>
     <row r="58" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A58" s="8" t="s">
-        <v>138</v>
+        <v>176</v>
       </c>
       <c r="B58" s="14" t="s">
         <v>26</v>
@@ -4011,7 +4022,7 @@
         <v>26</v>
       </c>
       <c r="P59" s="8" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="60" spans="1:29" x14ac:dyDescent="0.2">
@@ -4049,7 +4060,7 @@
         <v>26</v>
       </c>
       <c r="P60" s="8" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
     </row>
     <row r="61" spans="1:29" x14ac:dyDescent="0.2">
@@ -4166,7 +4177,7 @@
         <v>113</v>
       </c>
       <c r="S63" s="8" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="T63" s="8"/>
     </row>
@@ -4211,7 +4222,7 @@
         <v>113</v>
       </c>
       <c r="S64" s="8" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="T64" s="8"/>
     </row>
@@ -4251,18 +4262,18 @@
       <c r="P65" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="Q65" s="54" t="s">
-        <v>175</v>
-      </c>
-      <c r="R65" s="52"/>
-      <c r="S65" s="52"/>
+      <c r="Q65" s="53" t="s">
+        <v>174</v>
+      </c>
+      <c r="R65" s="51"/>
+      <c r="S65" s="51"/>
     </row>
     <row r="66" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A66" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="B66" s="52" t="s">
-        <v>168</v>
+      <c r="B66" s="51" t="s">
+        <v>167</v>
       </c>
       <c r="C66" s="14" t="s">
         <v>2</v>
@@ -4301,8 +4312,8 @@
       </c>
     </row>
     <row r="67" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A67" s="52" t="s">
-        <v>167</v>
+      <c r="A67" s="51" t="s">
+        <v>166</v>
       </c>
       <c r="C67" s="14" t="s">
         <v>2</v>
@@ -4340,8 +4351,8 @@
       </c>
     </row>
     <row r="68" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A68" s="52" t="s">
-        <v>169</v>
+      <c r="A68" s="51" t="s">
+        <v>168</v>
       </c>
       <c r="D68" s="14" t="s">
         <v>120</v>
@@ -4366,13 +4377,13 @@
       <c r="M68" s="39"/>
       <c r="N68" s="39"/>
       <c r="O68" s="39"/>
-      <c r="P68" s="52" t="s">
-        <v>174</v>
+      <c r="P68" s="51" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="69" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A69" s="52" t="s">
-        <v>170</v>
+      <c r="A69" s="51" t="s">
+        <v>169</v>
       </c>
       <c r="D69" s="14" t="s">
         <v>121</v>
@@ -4400,10 +4411,10 @@
       <c r="P69" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="Q69" s="52" t="s">
-        <v>171</v>
-      </c>
-      <c r="R69" s="52"/>
+      <c r="Q69" s="51" t="s">
+        <v>170</v>
+      </c>
+      <c r="R69" s="51"/>
     </row>
     <row r="70" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
@@ -4499,10 +4510,10 @@
       <c r="N73" s="39"/>
       <c r="O73" s="39"/>
       <c r="P73" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="Q73" s="53" t="s">
-        <v>173</v>
+        <v>165</v>
+      </c>
+      <c r="Q73" s="52" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="74" spans="1:21" x14ac:dyDescent="0.2">
@@ -4537,7 +4548,7 @@
         <v>51</v>
       </c>
       <c r="G75" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H75" s="13"/>
       <c r="I75" s="6"/>
@@ -4547,7 +4558,7 @@
       </c>
     </row>
     <row r="76" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="I76" s="48" t="s">
+      <c r="I76" s="47" t="s">
         <v>128</v>
       </c>
       <c r="J76" s="39"/>
@@ -4563,7 +4574,7 @@
       </c>
     </row>
     <row r="77" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="I77" s="49" t="s">
+      <c r="I77" s="48" t="s">
         <v>129</v>
       </c>
       <c r="J77" s="39"/>
@@ -4582,7 +4593,7 @@
       </c>
     </row>
     <row r="78" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="I78" s="50" t="s">
+      <c r="I78" s="49" t="s">
         <v>4</v>
       </c>
       <c r="J78" s="32"/>
@@ -4608,7 +4619,7 @@
       </c>
     </row>
     <row r="80" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="I80" s="49">
+      <c r="I80" s="48">
         <v>24</v>
       </c>
       <c r="J80" s="39">
@@ -4627,7 +4638,7 @@
       </c>
     </row>
     <row r="81" spans="7:21" x14ac:dyDescent="0.2">
-      <c r="I81" s="49">
+      <c r="I81" s="48">
         <v>25</v>
       </c>
       <c r="J81" s="39">
@@ -4646,7 +4657,7 @@
       </c>
     </row>
     <row r="82" spans="7:21" x14ac:dyDescent="0.2">
-      <c r="I82" s="49">
+      <c r="I82" s="48">
         <v>26</v>
       </c>
       <c r="J82" s="39">
@@ -4662,7 +4673,7 @@
       </c>
     </row>
     <row r="83" spans="7:21" x14ac:dyDescent="0.2">
-      <c r="I83" s="49">
+      <c r="I83" s="48">
         <v>27</v>
       </c>
       <c r="J83" s="39">
@@ -4678,7 +4689,7 @@
       </c>
     </row>
     <row r="84" spans="7:21" x14ac:dyDescent="0.2">
-      <c r="I84" s="49">
+      <c r="I84" s="48">
         <v>28</v>
       </c>
       <c r="J84" s="39">
@@ -4694,7 +4705,7 @@
       </c>
     </row>
     <row r="85" spans="7:21" x14ac:dyDescent="0.2">
-      <c r="I85" s="49">
+      <c r="I85" s="48">
         <v>29</v>
       </c>
       <c r="J85" s="39">
@@ -4710,7 +4721,7 @@
       </c>
     </row>
     <row r="86" spans="7:21" x14ac:dyDescent="0.2">
-      <c r="I86" s="49">
+      <c r="I86" s="48">
         <v>30</v>
       </c>
       <c r="J86" s="39">
@@ -4726,7 +4737,7 @@
       </c>
     </row>
     <row r="87" spans="7:21" x14ac:dyDescent="0.2">
-      <c r="I87" s="49">
+      <c r="I87" s="48">
         <v>31</v>
       </c>
       <c r="J87" s="39">
@@ -4742,7 +4753,7 @@
       </c>
     </row>
     <row r="88" spans="7:21" x14ac:dyDescent="0.2">
-      <c r="I88" s="49">
+      <c r="I88" s="48">
         <v>32</v>
       </c>
       <c r="J88" s="39">
@@ -4758,7 +4769,7 @@
       </c>
     </row>
     <row r="89" spans="7:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="I89" s="51">
+      <c r="I89" s="50">
         <v>33</v>
       </c>
       <c r="J89" s="39">

</xml_diff>

<commit_message>
Consider Teensy 3.5 for more IO
</commit_message>
<xml_diff>
--- a/Electronic Design/Core 64 Pin Usage Mapping.xlsx
+++ b/Electronic Design/Core 64 Pin Usage Mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ageppert/Dropbox/Electronics/Core 64 Interactive Badge/Core-64-Interactive-Core-Memory-Badge/Electronic Design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6860B26C-2E85-6A4F-8BFF-D150D2E9028A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC722629-7FEE-CD46-B601-42DD77AB91ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="27480" activeTab="1" xr2:uid="{A4752792-CA31-B046-B883-84F8D68A57EC}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="189">
   <si>
     <t>Custom</t>
   </si>
@@ -571,6 +571,36 @@
   </si>
   <si>
     <t>Testing hall sensor 2</t>
+  </si>
+  <si>
+    <t>Stuff to add</t>
+  </si>
+  <si>
+    <t>TFT Reset, needs dedicated line or skip it.</t>
+  </si>
+  <si>
+    <t>Sparkfun Teensy View</t>
+  </si>
+  <si>
+    <t>Reset</t>
+  </si>
+  <si>
+    <t>Data/control</t>
+  </si>
+  <si>
+    <t>DO</t>
+  </si>
+  <si>
+    <t>DI</t>
+  </si>
+  <si>
+    <t>CLK</t>
+  </si>
+  <si>
+    <t>TFT</t>
+  </si>
+  <si>
+    <t>LED Backlight Brightness</t>
   </si>
 </sst>
 </file>
@@ -2248,10 +2278,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CBC2977-27CE-C64F-BE79-A69FB2535F84}">
-  <dimension ref="A1:AC90"/>
+  <dimension ref="A1:AC100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="117" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="P35" sqref="P35"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="117" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="O102" sqref="O102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4789,6 +4819,81 @@
         <v>140</v>
       </c>
     </row>
+    <row r="91" spans="7:21" x14ac:dyDescent="0.2">
+      <c r="L91" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="92" spans="7:21" x14ac:dyDescent="0.2">
+      <c r="L92" s="14" t="s">
+        <v>187</v>
+      </c>
+      <c r="O92" s="14">
+        <v>1</v>
+      </c>
+      <c r="P92" s="8" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="93" spans="7:21" x14ac:dyDescent="0.2">
+      <c r="O93" s="14">
+        <v>2</v>
+      </c>
+      <c r="P93" s="8" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="95" spans="7:21" x14ac:dyDescent="0.2">
+      <c r="L95" t="s">
+        <v>181</v>
+      </c>
+      <c r="O95" s="14">
+        <v>3</v>
+      </c>
+      <c r="P95" s="8" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="96" spans="7:21" x14ac:dyDescent="0.2">
+      <c r="O96" s="14">
+        <v>4</v>
+      </c>
+      <c r="P96" s="8" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="97" spans="15:16" x14ac:dyDescent="0.2">
+      <c r="O97" s="14">
+        <v>5</v>
+      </c>
+      <c r="P97" s="8" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="98" spans="15:16" x14ac:dyDescent="0.2">
+      <c r="O98" s="14">
+        <v>6</v>
+      </c>
+      <c r="P98" s="8" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="99" spans="15:16" x14ac:dyDescent="0.2">
+      <c r="O99" s="14">
+        <v>7</v>
+      </c>
+      <c r="P99" s="8" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="100" spans="15:16" x14ac:dyDescent="0.2">
+      <c r="O100" s="14">
+        <v>8</v>
+      </c>
+      <c r="P100" s="8" t="s">
+        <v>122</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="V31:AB31"/>

</xml_diff>

<commit_message>
Update grammar in pin usage map
</commit_message>
<xml_diff>
--- a/Electronic Design/Core 64 Pin Usage Mapping.xlsx
+++ b/Electronic Design/Core 64 Pin Usage Mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ageppert/Dropbox/Electronics/Core 64 Interactive Badge/Core-64-Interactive-Core-Memory-Badge/Electronic Design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6860B26C-2E85-6A4F-8BFF-D150D2E9028A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E309DF72-F170-FF49-9403-EAD825A32D08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="27480" activeTab="1" xr2:uid="{A4752792-CA31-B046-B883-84F8D68A57EC}"/>
+    <workbookView xWindow="-20" yWindow="460" windowWidth="51200" windowHeight="27480" activeTab="1" xr2:uid="{A4752792-CA31-B046-B883-84F8D68A57EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Reference Pinouts" sheetId="3" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="188">
   <si>
     <t>Custom</t>
   </si>
@@ -571,6 +571,33 @@
   </si>
   <si>
     <t>Testing hall sensor 2</t>
+  </si>
+  <si>
+    <t>SD CARD CS</t>
+  </si>
+  <si>
+    <t>TFT CS</t>
+  </si>
+  <si>
+    <t>TOUCH CS</t>
+  </si>
+  <si>
+    <t>Spare CS</t>
+  </si>
+  <si>
+    <t>Can these 5 CS be on the matrix drive wires?</t>
+  </si>
+  <si>
+    <t>IR MODULATOR</t>
+  </si>
+  <si>
+    <t>Primary Core64 Usage</t>
+  </si>
+  <si>
+    <t>QWIIC</t>
+  </si>
+  <si>
+    <t>Sparkfun OLED Teensy View CS (or generic)</t>
   </si>
 </sst>
 </file>
@@ -839,7 +866,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -975,6 +1002,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2248,10 +2281,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CBC2977-27CE-C64F-BE79-A69FB2535F84}">
-  <dimension ref="A1:AC90"/>
+  <dimension ref="A1:AC97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="117" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="P35" sqref="P35"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="117" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="M96" sqref="M96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3851,7 +3884,7 @@
     </row>
     <row r="55" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>0</v>
+        <v>185</v>
       </c>
       <c r="B55" s="14" t="s">
         <v>1</v>
@@ -3893,7 +3926,7 @@
         <v>1</v>
       </c>
       <c r="P55" t="s">
-        <v>102</v>
+        <v>185</v>
       </c>
       <c r="Q55" s="14" t="s">
         <v>103</v>
@@ -4105,6 +4138,9 @@
       <c r="A62" s="8" t="s">
         <v>72</v>
       </c>
+      <c r="B62" s="56" t="s">
+        <v>184</v>
+      </c>
       <c r="C62" s="14" t="s">
         <v>2</v>
       </c>
@@ -4179,7 +4215,9 @@
       <c r="S63" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="T63" s="8"/>
+      <c r="T63" s="8" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="64" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A64" s="8" t="s">
@@ -4224,7 +4262,9 @@
       <c r="S64" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="T64" s="8"/>
+      <c r="T64" s="8" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="65" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A65" s="8" t="s">
@@ -4789,9 +4829,42 @@
         <v>140</v>
       </c>
     </row>
+    <row r="93" spans="7:21" x14ac:dyDescent="0.2">
+      <c r="P93" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q93" s="55" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="94" spans="7:21" x14ac:dyDescent="0.2">
+      <c r="P94" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="Q94" s="55"/>
+    </row>
+    <row r="95" spans="7:21" x14ac:dyDescent="0.2">
+      <c r="P95" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="Q95" s="55"/>
+    </row>
+    <row r="96" spans="7:21" x14ac:dyDescent="0.2">
+      <c r="P96" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q96" s="55"/>
+    </row>
+    <row r="97" spans="16:17" x14ac:dyDescent="0.2">
+      <c r="P97" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="Q97" s="55"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="V31:AB31"/>
+    <mergeCell ref="Q93:Q97"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
Add Arduino and Teensyduino Loader version numbers
</commit_message>
<xml_diff>
--- a/Electronic Design/Core 64 Pin Usage Mapping.xlsx
+++ b/Electronic Design/Core 64 Pin Usage Mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ageppert/Dropbox/Electronics/Core 64 Interactive Badge/Core-64-Interactive-Core-Memory-Badge/Electronic Design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC722629-7FEE-CD46-B601-42DD77AB91ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B80928FB-A1E0-EE43-B7DC-8F5075C30DF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="27480" activeTab="1" xr2:uid="{A4752792-CA31-B046-B883-84F8D68A57EC}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="32620" windowHeight="22680" activeTab="1" xr2:uid="{A4752792-CA31-B046-B883-84F8D68A57EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Reference Pinouts" sheetId="3" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="202">
   <si>
     <t>Custom</t>
   </si>
@@ -507,12 +507,6 @@
     <t>SENSE OUT B</t>
   </si>
   <si>
-    <t>Matrix Drive 17 Q9P</t>
-  </si>
-  <si>
-    <t>Matrix Drive 13 Q7P</t>
-  </si>
-  <si>
     <t>I2C BUS</t>
   </si>
   <si>
@@ -534,21 +528,6 @@
     <t>SPARE ANALOG (or pseudo digital input)</t>
   </si>
   <si>
-    <t>TFT ILI9341 CS</t>
-  </si>
-  <si>
-    <t>TFT ILI9341 D/C</t>
-  </si>
-  <si>
-    <t>TFT ILI9341 SDI (MOSI)</t>
-  </si>
-  <si>
-    <t>TFT ILI9341 SDO (MISO)</t>
-  </si>
-  <si>
-    <t>TFT ILI9341 SCK</t>
-  </si>
-  <si>
     <t>A14/DAC</t>
   </si>
   <si>
@@ -558,9 +537,6 @@
     <t>SDCARD_CS</t>
   </si>
   <si>
-    <t>TFT ILI9341 BACKLIGHT LED BRIGHTNESS</t>
-  </si>
-  <si>
     <t>SAO Port 1&amp;2, GPIO 2 (RX)</t>
   </si>
   <si>
@@ -573,34 +549,97 @@
     <t>Testing hall sensor 2</t>
   </si>
   <si>
-    <t>Stuff to add</t>
-  </si>
-  <si>
-    <t>TFT Reset, needs dedicated line or skip it.</t>
-  </si>
-  <si>
-    <t>Sparkfun Teensy View</t>
-  </si>
-  <si>
-    <t>Reset</t>
-  </si>
-  <si>
-    <t>Data/control</t>
-  </si>
-  <si>
-    <t>DO</t>
-  </si>
-  <si>
-    <t>DI</t>
-  </si>
-  <si>
-    <t>CLK</t>
-  </si>
-  <si>
-    <t>TFT</t>
-  </si>
-  <si>
-    <t>LED Backlight Brightness</t>
+    <t>A15</t>
+  </si>
+  <si>
+    <t>A16</t>
+  </si>
+  <si>
+    <t>A17</t>
+  </si>
+  <si>
+    <t>A18</t>
+  </si>
+  <si>
+    <t>A19</t>
+  </si>
+  <si>
+    <t>A20</t>
+  </si>
+  <si>
+    <t>Matrix Drive 1 - Q1P (normally high)</t>
+  </si>
+  <si>
+    <t>Matrix Drive 3 - Q2P (normally high)</t>
+  </si>
+  <si>
+    <t>Matrix Drive 5 - Q3P (normally high)</t>
+  </si>
+  <si>
+    <t>Matrix Drive 7 - Q4P (normally high)</t>
+  </si>
+  <si>
+    <t>Matrix Drive 9 - Q5P (normally high)</t>
+  </si>
+  <si>
+    <t>Matrix Drive 19 Q10P (normally high)</t>
+  </si>
+  <si>
+    <t>Matrix Drive 17 Q9P (normally high)</t>
+  </si>
+  <si>
+    <t>Matrix Drive 15 Q8P (normally high)</t>
+  </si>
+  <si>
+    <t>Matrix Drive 13 Q7P (normally high)</t>
+  </si>
+  <si>
+    <t>Matrix Drive 11 - Q6P (normally high)</t>
+  </si>
+  <si>
+    <t>TFT Reset (cannot be shared pin)</t>
+  </si>
+  <si>
+    <t>SPI SDI (MOSI)</t>
+  </si>
+  <si>
+    <t>SPI SDO (MISO)</t>
+  </si>
+  <si>
+    <t>SPI SCK</t>
+  </si>
+  <si>
+    <t>TFT BACKLIGHT LED BRIGHTNESS</t>
+  </si>
+  <si>
+    <t>LED - Built-in (heart beat)</t>
+  </si>
+  <si>
+    <t>TFT CS</t>
+  </si>
+  <si>
+    <t>TFT D/C</t>
+  </si>
+  <si>
+    <t>OLED CS</t>
+  </si>
+  <si>
+    <t>OLED Data/control</t>
+  </si>
+  <si>
+    <t>Spare SPI CS</t>
+  </si>
+  <si>
+    <t>Spare SPI Data/Control</t>
+  </si>
+  <si>
+    <t>Teensy View Data/control (default)</t>
+  </si>
+  <si>
+    <t>Teensy View CS (default)</t>
+  </si>
+  <si>
+    <t>Teensy View Reset (cannot be shared pin) (default)</t>
   </si>
 </sst>
 </file>
@@ -695,7 +734,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -735,6 +774,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -869,7 +926,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1000,10 +1057,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1034,13 +1094,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>66222</xdr:colOff>
       <xdr:row>54</xdr:row>
       <xdr:rowOff>117928</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>1569357</xdr:colOff>
       <xdr:row>69</xdr:row>
       <xdr:rowOff>9074</xdr:rowOff>
@@ -1095,14 +1155,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>19</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>1302658</xdr:colOff>
       <xdr:row>52</xdr:row>
       <xdr:rowOff>8165</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>3628</xdr:colOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>3627</xdr:colOff>
       <xdr:row>76</xdr:row>
       <xdr:rowOff>68037</xdr:rowOff>
     </xdr:to>
@@ -1156,13 +1216,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>27</xdr:col>
+      <xdr:col>28</xdr:col>
       <xdr:colOff>183243</xdr:colOff>
       <xdr:row>52</xdr:row>
       <xdr:rowOff>143328</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>34</xdr:col>
+      <xdr:col>35</xdr:col>
       <xdr:colOff>226223</xdr:colOff>
       <xdr:row>76</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
@@ -1217,13 +1277,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>34</xdr:col>
+      <xdr:col>35</xdr:col>
       <xdr:colOff>290285</xdr:colOff>
       <xdr:row>51</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>42</xdr:col>
+      <xdr:col>43</xdr:col>
       <xdr:colOff>112486</xdr:colOff>
       <xdr:row>82</xdr:row>
       <xdr:rowOff>21867</xdr:rowOff>
@@ -1278,13 +1338,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>1203035</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>94188</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>1578429</xdr:colOff>
       <xdr:row>44</xdr:row>
       <xdr:rowOff>21777</xdr:rowOff>
@@ -1339,13 +1399,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>19</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>1282700</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
+      <xdr:col>27</xdr:col>
       <xdr:colOff>716410</xdr:colOff>
       <xdr:row>51</xdr:row>
       <xdr:rowOff>16102</xdr:rowOff>
@@ -1400,13 +1460,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>27</xdr:col>
+      <xdr:col>28</xdr:col>
       <xdr:colOff>609599</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>33</xdr:col>
+      <xdr:col>34</xdr:col>
       <xdr:colOff>776280</xdr:colOff>
       <xdr:row>44</xdr:row>
       <xdr:rowOff>50800</xdr:rowOff>
@@ -1444,13 +1504,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>34</xdr:col>
+      <xdr:col>35</xdr:col>
       <xdr:colOff>292099</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>42</xdr:col>
+      <xdr:col>43</xdr:col>
       <xdr:colOff>90260</xdr:colOff>
       <xdr:row>50</xdr:row>
       <xdr:rowOff>186350</xdr:rowOff>
@@ -1505,13 +1565,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>35</xdr:col>
+      <xdr:col>36</xdr:col>
       <xdr:colOff>734785</xdr:colOff>
       <xdr:row>51</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>36</xdr:col>
+      <xdr:col>37</xdr:col>
       <xdr:colOff>199571</xdr:colOff>
       <xdr:row>53</xdr:row>
       <xdr:rowOff>97972</xdr:rowOff>
@@ -1560,13 +1620,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>35</xdr:col>
+      <xdr:col>36</xdr:col>
       <xdr:colOff>290285</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>35</xdr:col>
+      <xdr:col>36</xdr:col>
       <xdr:colOff>580571</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>186872</xdr:rowOff>
@@ -1615,13 +1675,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>1203035</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>94188</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>1578429</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>21777</xdr:rowOff>
@@ -1676,13 +1736,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
@@ -1724,14 +1784,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>20</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>814102</xdr:colOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>814103</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>156127</xdr:rowOff>
     </xdr:to>
@@ -1785,13 +1845,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>28</xdr:col>
+      <xdr:col>29</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>33</xdr:col>
+      <xdr:col>34</xdr:col>
       <xdr:colOff>413078</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>54274</xdr:rowOff>
@@ -1829,14 +1889,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>34</xdr:col>
+      <xdr:col>35</xdr:col>
       <xdr:colOff>43419</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>120362</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>41</xdr:col>
-      <xdr:colOff>670879</xdr:colOff>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>670880</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>151598</xdr:rowOff>
     </xdr:to>
@@ -1890,13 +1950,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>35</xdr:col>
+      <xdr:col>36</xdr:col>
       <xdr:colOff>94988</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>21709</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>35</xdr:col>
+      <xdr:col>36</xdr:col>
       <xdr:colOff>385274</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>205542</xdr:rowOff>
@@ -2278,2625 +2338,2652 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CBC2977-27CE-C64F-BE79-A69FB2535F84}">
-  <dimension ref="A1:AC100"/>
+  <dimension ref="A1:AD95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="117" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="O102" sqref="O102"/>
+    <sheetView tabSelected="1" topLeftCell="C43" zoomScale="117" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="Q68" sqref="Q68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="14"/>
-    <col min="3" max="3" width="5.6640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.6640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" style="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.83203125" style="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.83203125" customWidth="1"/>
-    <col min="8" max="8" width="21" customWidth="1"/>
-    <col min="9" max="9" width="15.83203125" customWidth="1"/>
-    <col min="10" max="10" width="8.83203125" style="14" customWidth="1"/>
-    <col min="11" max="11" width="6.83203125" style="14" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.5" style="14" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.6640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.6640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.83203125" style="14"/>
-    <col min="16" max="16" width="57" customWidth="1"/>
-    <col min="17" max="17" width="12.1640625" customWidth="1"/>
-    <col min="18" max="18" width="14" customWidth="1"/>
-    <col min="20" max="20" width="17.33203125" customWidth="1"/>
-    <col min="22" max="23" width="10.83203125" style="14"/>
+    <col min="1" max="2" width="29.5" customWidth="1"/>
+    <col min="3" max="3" width="28.83203125" style="14" customWidth="1"/>
+    <col min="4" max="4" width="5.6640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.6640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.83203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.83203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.83203125" customWidth="1"/>
+    <col min="9" max="9" width="21" customWidth="1"/>
+    <col min="10" max="10" width="15.83203125" customWidth="1"/>
+    <col min="11" max="11" width="8.83203125" style="14" customWidth="1"/>
+    <col min="12" max="12" width="6.83203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.5" style="14" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.6640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.6640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.83203125" style="14"/>
+    <col min="17" max="17" width="57" customWidth="1"/>
+    <col min="18" max="18" width="21" customWidth="1"/>
+    <col min="19" max="19" width="14" customWidth="1"/>
+    <col min="21" max="21" width="17.33203125" customWidth="1"/>
+    <col min="23" max="24" width="10.83203125" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="22" t="s">
         <v>97</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="B2" s="22"/>
+      <c r="I2" s="18" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="C3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="D3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="E3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="F3" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="G3" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>5</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>5</v>
       </c>
-      <c r="J3" s="14" t="s">
+      <c r="K3" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="K3" s="14" t="s">
+      <c r="L3" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="L3" s="14" t="s">
+      <c r="M3" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="M3" s="14" t="s">
+      <c r="N3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="N3" s="14" t="s">
+      <c r="O3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="O3" s="14" t="s">
+      <c r="P3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>52</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="11"/>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="11"/>
+      <c r="J4" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="J4" s="7"/>
-      <c r="P4" s="20" t="s">
+      <c r="K4" s="7"/>
+      <c r="Q4" s="20" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="15"/>
+      <c r="C5" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="E5" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="F5" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="14">
+      <c r="G5" s="14">
         <v>0</v>
       </c>
-      <c r="G5" s="3">
+      <c r="H5" s="3">
         <v>0</v>
       </c>
-      <c r="H5" s="7"/>
-      <c r="I5" s="4" t="s">
+      <c r="I5" s="7"/>
+      <c r="J5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="J5" s="7"/>
-      <c r="P5" s="21" t="s">
+      <c r="K5" s="7"/>
+      <c r="Q5" s="21" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="15"/>
+      <c r="C6" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="E6" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="F6" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="14">
+      <c r="G6" s="14">
         <v>1</v>
       </c>
-      <c r="G6" s="3">
+      <c r="H6" s="3">
         <v>1</v>
       </c>
-      <c r="H6" s="7"/>
-      <c r="I6" s="4" t="s">
+      <c r="I6" s="7"/>
+      <c r="J6" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="J6" s="7"/>
-      <c r="P6" s="9" t="s">
+      <c r="K6" s="7"/>
+      <c r="Q6" s="9" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="F7" s="14">
+      <c r="B7" s="15"/>
+      <c r="G7" s="14">
         <v>2</v>
       </c>
-      <c r="G7" s="3">
+      <c r="H7" s="3">
         <v>2</v>
       </c>
-      <c r="H7" s="7"/>
-      <c r="I7" s="4">
+      <c r="I7" s="7"/>
+      <c r="J7" s="4">
         <v>23</v>
       </c>
-      <c r="J7" s="7">
+      <c r="K7" s="7">
         <v>23</v>
       </c>
-      <c r="K7" s="14" t="s">
+      <c r="L7" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="L7" s="14" t="s">
+      <c r="M7" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="N7" s="14" t="s">
+      <c r="O7" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="O7" s="14" t="s">
+      <c r="P7" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="P7" s="19" t="s">
+      <c r="Q7" s="19" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="15"/>
+      <c r="C8" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="D8" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="F8" s="14">
+      <c r="G8" s="14">
         <v>3</v>
       </c>
-      <c r="G8" s="3">
+      <c r="H8" s="3">
         <v>3</v>
       </c>
-      <c r="H8" s="7"/>
-      <c r="I8" s="4">
+      <c r="I8" s="7"/>
+      <c r="J8" s="4">
         <v>22</v>
       </c>
-      <c r="J8" s="7">
+      <c r="K8" s="7">
         <v>22</v>
       </c>
-      <c r="K8" s="14" t="s">
+      <c r="L8" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="L8" s="14" t="s">
+      <c r="M8" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="N8" s="14" t="s">
+      <c r="O8" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="O8" s="14" t="s">
+      <c r="P8" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="P8" s="15" t="s">
+      <c r="Q8" s="15" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="15"/>
+      <c r="C9" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="D9" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="F9" s="14">
+      <c r="G9" s="14">
         <v>4</v>
       </c>
-      <c r="G9" s="3">
+      <c r="H9" s="3">
         <v>4</v>
       </c>
-      <c r="H9" s="7"/>
-      <c r="I9" s="4">
+      <c r="I9" s="7"/>
+      <c r="J9" s="4">
         <v>21</v>
       </c>
-      <c r="J9" s="7">
+      <c r="K9" s="7">
         <v>21</v>
       </c>
-      <c r="K9" s="14" t="s">
+      <c r="L9" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="M9" s="14" t="s">
+      <c r="N9" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="P9" s="19" t="s">
+      <c r="Q9" s="19" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="F10" s="14">
+      <c r="B10" s="15"/>
+      <c r="G10" s="14">
         <v>5</v>
       </c>
-      <c r="G10" s="3">
+      <c r="H10" s="3">
         <v>5</v>
       </c>
-      <c r="H10" s="7"/>
-      <c r="I10" s="4">
+      <c r="I10" s="7"/>
+      <c r="J10" s="4">
         <v>20</v>
       </c>
-      <c r="J10" s="7">
+      <c r="K10" s="7">
         <v>20</v>
       </c>
-      <c r="K10" s="14" t="s">
+      <c r="L10" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="M10" s="14" t="s">
+      <c r="N10" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="N10" s="14" t="s">
+      <c r="O10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="P10" s="19" t="s">
+      <c r="Q10" s="19" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="B11" s="15"/>
+      <c r="D11" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="E11" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="F11" s="14">
+      <c r="G11" s="14">
         <v>6</v>
       </c>
-      <c r="G11" s="3">
+      <c r="H11" s="3">
         <v>6</v>
       </c>
-      <c r="H11" s="7"/>
-      <c r="I11" s="4">
+      <c r="I11" s="7"/>
+      <c r="J11" s="4">
         <v>19</v>
       </c>
-      <c r="J11" s="7">
+      <c r="K11" s="7">
         <v>19</v>
       </c>
-      <c r="K11" s="14" t="s">
+      <c r="L11" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="L11" s="14" t="s">
+      <c r="M11" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="O11" s="14" t="s">
+      <c r="P11" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="P11" s="8" t="s">
+      <c r="Q11" s="8" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="B12" s="15"/>
+      <c r="F12" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="F12" s="14">
+      <c r="G12" s="14">
         <v>7</v>
       </c>
-      <c r="G12" s="3">
+      <c r="H12" s="3">
         <v>7</v>
       </c>
-      <c r="H12" s="7"/>
-      <c r="I12" s="4">
+      <c r="I12" s="7"/>
+      <c r="J12" s="4">
         <v>18</v>
       </c>
-      <c r="J12" s="7">
+      <c r="K12" s="7">
         <v>18</v>
       </c>
-      <c r="K12" s="14" t="s">
+      <c r="L12" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="L12" s="14" t="s">
+      <c r="M12" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="O12" s="14" t="s">
+      <c r="P12" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="P12" s="8" t="s">
+      <c r="Q12" s="8" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="B13" s="15"/>
+      <c r="F13" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="F13" s="14">
+      <c r="G13" s="14">
         <v>8</v>
       </c>
-      <c r="G13" s="3">
+      <c r="H13" s="3">
         <v>8</v>
       </c>
-      <c r="H13" s="7"/>
-      <c r="I13" s="4">
+      <c r="I13" s="7"/>
+      <c r="J13" s="4">
         <v>17</v>
       </c>
-      <c r="J13" s="7">
+      <c r="K13" s="7">
         <v>17</v>
       </c>
-      <c r="K13" s="14" t="s">
+      <c r="L13" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="N13" s="14" t="s">
+      <c r="O13" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="O13" s="14" t="s">
+      <c r="P13" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="P13" s="19" t="s">
+      <c r="Q13" s="19" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="B14" s="15"/>
+      <c r="D14" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E14" s="14" t="s">
+      <c r="F14" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="F14" s="14">
+      <c r="G14" s="14">
         <v>9</v>
       </c>
-      <c r="G14" s="3">
+      <c r="H14" s="3">
         <v>9</v>
       </c>
-      <c r="H14" s="7"/>
-      <c r="I14" s="4">
+      <c r="I14" s="7"/>
+      <c r="J14" s="4">
         <v>16</v>
       </c>
-      <c r="J14" s="7">
+      <c r="K14" s="7">
         <v>16</v>
       </c>
-      <c r="K14" s="14" t="s">
+      <c r="L14" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="N14" s="14" t="s">
+      <c r="O14" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="O14" s="14" t="s">
+      <c r="P14" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="P14" s="15" t="s">
+      <c r="Q14" s="15" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="B15" s="15"/>
+      <c r="D15" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="E15" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="14" t="s">
+      <c r="F15" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="F15" s="14">
+      <c r="G15" s="14">
         <v>10</v>
       </c>
-      <c r="G15" s="3">
+      <c r="H15" s="3">
         <v>10</v>
       </c>
-      <c r="H15" s="7"/>
-      <c r="I15" s="4">
+      <c r="I15" s="7"/>
+      <c r="J15" s="4">
         <v>15</v>
       </c>
-      <c r="J15" s="7">
+      <c r="K15" s="7">
         <v>15</v>
       </c>
-      <c r="K15" s="14" t="s">
+      <c r="L15" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="O15" s="14" t="s">
+      <c r="P15" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="P15" s="15" t="s">
+      <c r="Q15" s="15" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="B16" s="15"/>
+      <c r="E16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="F16" s="14">
+      <c r="G16" s="14">
         <v>11</v>
       </c>
-      <c r="G16" s="3">
+      <c r="H16" s="3">
         <v>11</v>
       </c>
-      <c r="H16" s="7"/>
-      <c r="I16" s="4">
+      <c r="I16" s="7"/>
+      <c r="J16" s="4">
         <v>14</v>
       </c>
-      <c r="J16" s="7">
+      <c r="K16" s="7">
         <v>14</v>
       </c>
-      <c r="K16" s="14" t="s">
+      <c r="L16" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="P16" s="15" t="s">
+      <c r="Q16" s="15" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A17" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="D17" s="14" t="s">
+      <c r="B17" s="15"/>
+      <c r="E17" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="F17" s="14">
+      <c r="G17" s="14">
         <v>12</v>
       </c>
-      <c r="G17" s="3">
+      <c r="H17" s="3">
         <v>12</v>
       </c>
-      <c r="H17" s="7"/>
-      <c r="I17" s="4" t="s">
+      <c r="I17" s="7"/>
+      <c r="J17" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="J17" s="7">
+      <c r="K17" s="7">
         <v>13</v>
       </c>
-      <c r="M17" s="14" t="s">
+      <c r="N17" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="P17" s="15" t="s">
+      <c r="Q17" s="15" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>51</v>
       </c>
-      <c r="G18" s="16" t="s">
+      <c r="H18" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="H18" s="12"/>
-      <c r="I18" s="17" t="s">
+      <c r="I18" s="12"/>
+      <c r="J18" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="J18" s="7"/>
-      <c r="P18" t="s">
+      <c r="K18" s="7"/>
+      <c r="Q18" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="F19" s="14">
+      <c r="B19" s="8"/>
+      <c r="G19" s="14">
         <v>17</v>
       </c>
-      <c r="G19" s="3" t="s">
+      <c r="H19" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I19" s="4" t="s">
+      <c r="J19" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J19" s="7" t="s">
+      <c r="K19" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="P19" s="8" t="s">
+      <c r="Q19" s="8" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>62</v>
       </c>
-      <c r="F20" s="14" t="s">
+      <c r="G20" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="G20" s="3" t="s">
+      <c r="H20" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H20" s="7"/>
-      <c r="I20" s="4">
+      <c r="I20" s="7"/>
+      <c r="J20" s="4">
         <v>24</v>
       </c>
-      <c r="J20" s="7">
+      <c r="K20" s="7">
         <v>24</v>
       </c>
-      <c r="K20" s="14" t="s">
+      <c r="L20" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="P20" s="8" t="s">
+      <c r="Q20" s="8" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>68</v>
       </c>
-      <c r="F21" s="14" t="s">
+      <c r="G21" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="G21" s="3" t="s">
+      <c r="H21" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H21" s="7"/>
-      <c r="I21" s="4">
+      <c r="I21" s="7"/>
+      <c r="J21" s="4">
         <v>25</v>
       </c>
-      <c r="J21" s="7">
+      <c r="K21" s="7">
         <v>25</v>
       </c>
-      <c r="K21" s="14" t="s">
+      <c r="L21" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="P21" s="8" t="s">
+      <c r="Q21" s="8" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>116</v>
       </c>
-      <c r="F22" s="14" t="s">
+      <c r="G22" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="3" t="s">
+      <c r="H22" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H22" s="7"/>
-      <c r="I22" s="4" t="s">
+      <c r="I22" s="7"/>
+      <c r="J22" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="J22" s="7"/>
-      <c r="P22" t="s">
+      <c r="K22" s="7"/>
+      <c r="Q22" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="23" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:30" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="F23" s="14">
+      <c r="B23" s="8"/>
+      <c r="G23" s="14">
         <v>26</v>
       </c>
-      <c r="G23" s="5" t="s">
+      <c r="H23" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H23" s="13"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="7"/>
-      <c r="P23" t="s">
+      <c r="I23" s="13"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="7"/>
+      <c r="Q23" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="U25" t="s">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="V25" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="U26" t="s">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="V26" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A29" s="22" t="s">
         <v>97</v>
       </c>
-      <c r="G29" s="8"/>
-      <c r="H29" s="23" t="s">
+      <c r="B29" s="22"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="I29" s="8"/>
-    </row>
-    <row r="30" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="J29" s="8"/>
+    </row>
+    <row r="30" spans="1:30" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>0</v>
       </c>
-      <c r="B30" s="14" t="s">
+      <c r="C30" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C30" s="14" t="s">
+      <c r="D30" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D30" s="14" t="s">
+      <c r="E30" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E30" s="14" t="s">
+      <c r="F30" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="F30" s="14" t="s">
+      <c r="G30" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="G30" t="s">
+      <c r="H30" t="s">
         <v>5</v>
       </c>
-      <c r="I30" t="s">
+      <c r="J30" t="s">
         <v>5</v>
       </c>
-      <c r="J30" s="14" t="s">
+      <c r="K30" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="K30" s="14" t="s">
+      <c r="L30" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="L30" s="14" t="s">
+      <c r="M30" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="M30" s="14" t="s">
+      <c r="N30" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="N30" s="14" t="s">
+      <c r="O30" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="O30" s="14" t="s">
+      <c r="P30" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="P30" t="s">
+      <c r="Q30" t="s">
         <v>102</v>
       </c>
-      <c r="Q30" s="14" t="s">
+      <c r="R30" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="R30" t="s">
+      <c r="S30" t="s">
         <v>110</v>
       </c>
-      <c r="S30" s="14" t="s">
+      <c r="T30" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="T30" t="s">
+      <c r="U30" t="s">
         <v>112</v>
       </c>
-      <c r="V30" s="26"/>
       <c r="W30" s="26"/>
-      <c r="X30" s="9"/>
+      <c r="X30" s="26"/>
       <c r="Y30" s="9"/>
       <c r="Z30" s="9"/>
       <c r="AA30" s="9"/>
       <c r="AB30" s="9"/>
       <c r="AC30" s="9"/>
-    </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD30" s="9"/>
+    </row>
+    <row r="31" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A31" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="B31" s="32"/>
+      <c r="B31" s="29"/>
       <c r="C31" s="32"/>
       <c r="D31" s="32"/>
       <c r="E31" s="32"/>
       <c r="F31" s="32"/>
-      <c r="G31" s="30" t="s">
+      <c r="G31" s="32"/>
+      <c r="H31" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="H31" s="11"/>
-      <c r="I31" s="34" t="s">
+      <c r="I31" s="11"/>
+      <c r="J31" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="J31" s="35"/>
-      <c r="K31" s="25"/>
+      <c r="K31" s="35"/>
       <c r="L31" s="25"/>
       <c r="M31" s="25"/>
       <c r="N31" s="25"/>
       <c r="O31" s="25"/>
-      <c r="P31" s="36" t="s">
+      <c r="P31" s="25"/>
+      <c r="Q31" s="36" t="s">
         <v>107</v>
       </c>
-      <c r="V31" s="54"/>
-      <c r="W31" s="54"/>
-      <c r="X31" s="54"/>
-      <c r="Y31" s="54"/>
-      <c r="Z31" s="54"/>
-      <c r="AA31" s="54"/>
-      <c r="AB31" s="54"/>
-      <c r="AC31" s="9"/>
-    </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="W31" s="57"/>
+      <c r="X31" s="57"/>
+      <c r="Y31" s="57"/>
+      <c r="Z31" s="57"/>
+      <c r="AA31" s="57"/>
+      <c r="AB31" s="57"/>
+      <c r="AC31" s="57"/>
+      <c r="AD31" s="9"/>
+    </row>
+    <row r="32" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A32" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="B32" s="39" t="s">
+      <c r="B32" s="8"/>
+      <c r="C32" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="C32" s="39"/>
-      <c r="D32" s="39" t="s">
+      <c r="D32" s="39"/>
+      <c r="E32" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="E32" s="39" t="s">
+      <c r="F32" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="F32" s="39">
+      <c r="G32" s="39">
         <v>0</v>
       </c>
-      <c r="G32" s="3">
+      <c r="H32" s="3">
         <v>0</v>
       </c>
-      <c r="H32" s="7"/>
-      <c r="I32" s="31" t="s">
+      <c r="I32" s="7"/>
+      <c r="J32" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="J32" s="33"/>
-      <c r="K32" s="32"/>
+      <c r="K32" s="33"/>
       <c r="L32" s="32"/>
       <c r="M32" s="32"/>
       <c r="N32" s="32"/>
       <c r="O32" s="32"/>
-      <c r="P32" s="29" t="s">
+      <c r="P32" s="32"/>
+      <c r="Q32" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="V32" s="26"/>
       <c r="W32" s="26"/>
-      <c r="X32" s="9"/>
+      <c r="X32" s="26"/>
       <c r="Y32" s="9"/>
       <c r="Z32" s="9"/>
       <c r="AA32" s="9"/>
       <c r="AB32" s="9"/>
       <c r="AC32" s="9"/>
-    </row>
-    <row r="33" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD32" s="9"/>
+    </row>
+    <row r="33" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A33" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="B33" s="39" t="s">
+      <c r="B33" s="8"/>
+      <c r="C33" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="C33" s="39"/>
-      <c r="D33" s="39" t="s">
+      <c r="D33" s="39"/>
+      <c r="E33" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="E33" s="39" t="s">
+      <c r="F33" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="F33" s="39">
+      <c r="G33" s="39">
         <v>1</v>
       </c>
-      <c r="G33" s="3">
+      <c r="H33" s="3">
         <v>1</v>
       </c>
-      <c r="H33" s="7"/>
-      <c r="I33" s="40" t="s">
+      <c r="I33" s="7"/>
+      <c r="J33" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="J33" s="35"/>
-      <c r="K33" s="25"/>
+      <c r="K33" s="35"/>
       <c r="L33" s="25"/>
       <c r="M33" s="25"/>
       <c r="N33" s="25"/>
       <c r="O33" s="25"/>
-      <c r="P33" s="24" t="s">
+      <c r="P33" s="25"/>
+      <c r="Q33" s="24" t="s">
         <v>147</v>
       </c>
-      <c r="V33" s="26"/>
       <c r="W33" s="26"/>
-      <c r="X33" s="9"/>
+      <c r="X33" s="26"/>
       <c r="Y33" s="9"/>
       <c r="Z33" s="9"/>
       <c r="AA33" s="9"/>
       <c r="AB33" s="9"/>
       <c r="AC33" s="9"/>
-    </row>
-    <row r="34" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD33" s="9"/>
+    </row>
+    <row r="34" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A34" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="B34" s="39"/>
+      <c r="B34" s="8"/>
       <c r="C34" s="39"/>
       <c r="D34" s="39"/>
       <c r="E34" s="39"/>
-      <c r="F34" s="39">
+      <c r="F34" s="39"/>
+      <c r="G34" s="39">
         <v>2</v>
       </c>
-      <c r="G34" s="3">
+      <c r="H34" s="3">
         <v>2</v>
       </c>
-      <c r="H34" s="7"/>
-      <c r="I34" s="4">
+      <c r="I34" s="7"/>
+      <c r="J34" s="4">
         <v>23</v>
       </c>
-      <c r="J34" s="7">
+      <c r="K34" s="7">
         <v>23</v>
       </c>
-      <c r="K34" s="14" t="s">
+      <c r="L34" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="L34" s="14" t="s">
+      <c r="M34" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="N34" s="14" t="s">
+      <c r="O34" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="O34" s="14" t="s">
+      <c r="P34" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="P34" s="19" t="s">
-        <v>178</v>
-      </c>
-      <c r="V34" s="26"/>
+      <c r="Q34" s="19" t="s">
+        <v>170</v>
+      </c>
       <c r="W34" s="26"/>
-      <c r="X34" s="9"/>
+      <c r="X34" s="26"/>
       <c r="Y34" s="9"/>
       <c r="Z34" s="9"/>
       <c r="AA34" s="9"/>
       <c r="AB34" s="9"/>
       <c r="AC34" s="9"/>
-    </row>
-    <row r="35" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD34" s="9"/>
+    </row>
+    <row r="35" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A35" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="B35" s="39" t="s">
+      <c r="B35" s="8"/>
+      <c r="C35" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="C35" s="39" t="s">
+      <c r="D35" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="D35" s="39"/>
       <c r="E35" s="39"/>
-      <c r="F35" s="39">
+      <c r="F35" s="39"/>
+      <c r="G35" s="39">
         <v>3</v>
       </c>
-      <c r="G35" s="3">
+      <c r="H35" s="3">
         <v>3</v>
       </c>
-      <c r="H35" s="7"/>
-      <c r="I35" s="4">
+      <c r="I35" s="7"/>
+      <c r="J35" s="4">
         <v>22</v>
       </c>
-      <c r="J35" s="7">
+      <c r="K35" s="7">
         <v>22</v>
       </c>
-      <c r="K35" s="14" t="s">
+      <c r="L35" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="L35" s="14" t="s">
+      <c r="M35" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="N35" s="14" t="s">
+      <c r="O35" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="O35" s="14" t="s">
+      <c r="P35" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="P35" s="19"/>
-      <c r="V35" s="26"/>
+      <c r="Q35" s="19"/>
       <c r="W35" s="26"/>
-      <c r="X35" s="9"/>
+      <c r="X35" s="26"/>
       <c r="Y35" s="9"/>
       <c r="Z35" s="9"/>
       <c r="AA35" s="9"/>
       <c r="AB35" s="9"/>
       <c r="AC35" s="9"/>
-    </row>
-    <row r="36" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD35" s="9"/>
+    </row>
+    <row r="36" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A36" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="B36" s="39" t="s">
+      <c r="B36" s="8"/>
+      <c r="C36" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="C36" s="39" t="s">
+      <c r="D36" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="D36" s="39"/>
       <c r="E36" s="39"/>
-      <c r="F36" s="39">
+      <c r="F36" s="39"/>
+      <c r="G36" s="39">
         <v>4</v>
       </c>
-      <c r="G36" s="3">
+      <c r="H36" s="3">
         <v>4</v>
       </c>
-      <c r="H36" s="7"/>
-      <c r="I36" s="37">
+      <c r="I36" s="7"/>
+      <c r="J36" s="37">
         <v>21</v>
       </c>
-      <c r="J36" s="38">
+      <c r="K36" s="38">
         <v>21</v>
       </c>
-      <c r="K36" s="39" t="s">
+      <c r="L36" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="L36" s="39"/>
-      <c r="M36" s="39" t="s">
+      <c r="M36" s="39"/>
+      <c r="N36" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="N36" s="39"/>
       <c r="O36" s="39"/>
-      <c r="P36" s="8" t="s">
+      <c r="P36" s="39"/>
+      <c r="Q36" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="V36" s="26"/>
       <c r="W36" s="26"/>
-      <c r="X36" s="9"/>
+      <c r="X36" s="26"/>
       <c r="Y36" s="9"/>
       <c r="Z36" s="9"/>
       <c r="AA36" s="9"/>
       <c r="AB36" s="9"/>
       <c r="AC36" s="9"/>
-    </row>
-    <row r="37" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD36" s="9"/>
+    </row>
+    <row r="37" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A37" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="B37" s="39"/>
+      <c r="B37" s="8"/>
       <c r="C37" s="39"/>
       <c r="D37" s="39"/>
       <c r="E37" s="39"/>
-      <c r="F37" s="39">
+      <c r="F37" s="39"/>
+      <c r="G37" s="39">
         <v>5</v>
       </c>
-      <c r="G37" s="3">
+      <c r="H37" s="3">
         <v>5</v>
       </c>
-      <c r="H37" s="7"/>
-      <c r="I37" s="4">
+      <c r="I37" s="7"/>
+      <c r="J37" s="4">
         <v>20</v>
       </c>
-      <c r="J37" s="7">
+      <c r="K37" s="7">
         <v>20</v>
       </c>
-      <c r="K37" s="14" t="s">
+      <c r="L37" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="M37" s="14" t="s">
+      <c r="N37" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="N37" s="14" t="s">
+      <c r="O37" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="P37" s="15"/>
-      <c r="V37" s="26"/>
+      <c r="Q37" s="15"/>
       <c r="W37" s="26"/>
-      <c r="X37" s="9"/>
+      <c r="X37" s="26"/>
       <c r="Y37" s="9"/>
       <c r="Z37" s="9"/>
       <c r="AA37" s="9"/>
       <c r="AB37" s="9"/>
       <c r="AC37" s="9"/>
-    </row>
-    <row r="38" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD37" s="9"/>
+    </row>
+    <row r="38" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A38" s="15"/>
-      <c r="C38" s="14" t="s">
+      <c r="B38" s="15"/>
+      <c r="D38" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D38" s="14" t="s">
+      <c r="E38" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="F38" s="14">
+      <c r="G38" s="14">
         <v>6</v>
       </c>
-      <c r="G38" s="3">
+      <c r="H38" s="3">
         <v>6</v>
       </c>
-      <c r="H38" s="7"/>
-      <c r="I38" s="37">
+      <c r="I38" s="7"/>
+      <c r="J38" s="37">
         <v>19</v>
       </c>
-      <c r="J38" s="38">
+      <c r="K38" s="38">
         <v>19</v>
       </c>
-      <c r="K38" s="39" t="s">
+      <c r="L38" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="L38" s="39" t="s">
+      <c r="M38" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="M38" s="39"/>
       <c r="N38" s="39"/>
-      <c r="O38" s="39" t="s">
+      <c r="O38" s="39"/>
+      <c r="P38" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="P38" s="8" t="s">
+      <c r="Q38" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="Q38" s="8" t="s">
+      <c r="R38" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="R38" s="8" t="s">
+      <c r="S38" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="S38" s="8" t="s">
+      <c r="T38" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="T38" s="8"/>
-      <c r="V38" s="26"/>
+      <c r="U38" s="8"/>
       <c r="W38" s="26"/>
-      <c r="X38" s="9"/>
+      <c r="X38" s="26"/>
       <c r="Y38" s="9"/>
       <c r="Z38" s="9"/>
       <c r="AA38" s="9"/>
       <c r="AB38" s="9"/>
       <c r="AC38" s="9"/>
-    </row>
-    <row r="39" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD38" s="9"/>
+    </row>
+    <row r="39" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A39" s="15"/>
-      <c r="E39" s="14" t="s">
+      <c r="B39" s="15"/>
+      <c r="F39" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="F39" s="14">
+      <c r="G39" s="14">
         <v>7</v>
       </c>
-      <c r="G39" s="3">
+      <c r="H39" s="3">
         <v>7</v>
       </c>
-      <c r="H39" s="7"/>
-      <c r="I39" s="37">
+      <c r="I39" s="7"/>
+      <c r="J39" s="37">
         <v>18</v>
       </c>
-      <c r="J39" s="38">
+      <c r="K39" s="38">
         <v>18</v>
       </c>
-      <c r="K39" s="39" t="s">
+      <c r="L39" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="L39" s="39" t="s">
+      <c r="M39" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="M39" s="39"/>
       <c r="N39" s="39"/>
-      <c r="O39" s="39" t="s">
+      <c r="O39" s="39"/>
+      <c r="P39" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="P39" s="8" t="s">
+      <c r="Q39" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="Q39" s="8" t="s">
+      <c r="R39" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="R39" s="8" t="s">
+      <c r="S39" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="S39" s="8" t="s">
+      <c r="T39" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="T39" s="8"/>
-      <c r="V39" s="26"/>
+      <c r="U39" s="8"/>
       <c r="W39" s="26"/>
-      <c r="X39" s="9"/>
+      <c r="X39" s="26"/>
       <c r="Y39" s="9"/>
       <c r="Z39" s="9"/>
       <c r="AA39" s="9"/>
       <c r="AB39" s="9"/>
       <c r="AC39" s="9"/>
-    </row>
-    <row r="40" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD39" s="9"/>
+    </row>
+    <row r="40" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A40" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="B40" s="39"/>
+      <c r="B40" s="8"/>
       <c r="C40" s="39"/>
       <c r="D40" s="39"/>
-      <c r="E40" s="39" t="s">
+      <c r="E40" s="39"/>
+      <c r="F40" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="F40" s="39">
+      <c r="G40" s="39">
         <v>8</v>
       </c>
-      <c r="G40" s="3">
+      <c r="H40" s="3">
         <v>8</v>
       </c>
-      <c r="H40" s="7"/>
-      <c r="I40" s="37">
+      <c r="I40" s="7"/>
+      <c r="J40" s="37">
         <v>17</v>
       </c>
-      <c r="J40" s="38">
+      <c r="K40" s="38">
         <v>17</v>
       </c>
-      <c r="K40" s="39" t="s">
+      <c r="L40" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="L40" s="39"/>
       <c r="M40" s="39"/>
-      <c r="N40" s="39" t="s">
+      <c r="N40" s="39"/>
+      <c r="O40" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="O40" s="39" t="s">
+      <c r="P40" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="P40" s="8" t="s">
+      <c r="Q40" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="Q40" s="39" t="s">
+      <c r="R40" s="39" t="s">
         <v>150</v>
       </c>
-      <c r="V40" s="26"/>
       <c r="W40" s="26"/>
-      <c r="X40" s="9"/>
+      <c r="X40" s="26"/>
       <c r="Y40" s="9"/>
       <c r="Z40" s="9"/>
       <c r="AA40" s="9"/>
       <c r="AB40" s="9"/>
       <c r="AC40" s="9"/>
-    </row>
-    <row r="41" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD40" s="9"/>
+    </row>
+    <row r="41" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A41" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="B41" s="39"/>
-      <c r="C41" s="39" t="s">
+      <c r="B41" s="8"/>
+      <c r="C41" s="39"/>
+      <c r="D41" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="D41" s="39"/>
-      <c r="E41" s="39" t="s">
+      <c r="E41" s="39"/>
+      <c r="F41" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="F41" s="39">
+      <c r="G41" s="39">
         <v>9</v>
       </c>
-      <c r="G41" s="3">
+      <c r="H41" s="3">
         <v>9</v>
       </c>
-      <c r="H41" s="7"/>
-      <c r="I41" s="4">
+      <c r="I41" s="7"/>
+      <c r="J41" s="4">
         <v>16</v>
       </c>
-      <c r="J41" s="7">
+      <c r="K41" s="7">
         <v>16</v>
       </c>
-      <c r="K41" s="14" t="s">
+      <c r="L41" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="N41" s="14" t="s">
+      <c r="O41" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="O41" s="14" t="s">
+      <c r="P41" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="P41" s="8"/>
-      <c r="Q41" s="39" t="s">
+      <c r="Q41" s="8"/>
+      <c r="R41" s="39" t="s">
         <v>151</v>
       </c>
-      <c r="V41" s="26"/>
       <c r="W41" s="26"/>
-      <c r="X41" s="9"/>
+      <c r="X41" s="26"/>
       <c r="Y41" s="9"/>
       <c r="Z41" s="9"/>
       <c r="AA41" s="9"/>
       <c r="AB41" s="9"/>
       <c r="AC41" s="9"/>
-    </row>
-    <row r="42" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD41" s="9"/>
+    </row>
+    <row r="42" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A42" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="B42" s="39"/>
-      <c r="C42" s="39" t="s">
+      <c r="B42" s="8"/>
+      <c r="C42" s="39"/>
+      <c r="D42" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="D42" s="39" t="s">
+      <c r="E42" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="E42" s="39" t="s">
+      <c r="F42" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="F42" s="39">
+      <c r="G42" s="39">
         <v>10</v>
       </c>
-      <c r="G42" s="3">
+      <c r="H42" s="3">
         <v>10</v>
       </c>
-      <c r="H42" s="7"/>
-      <c r="I42" s="37">
+      <c r="I42" s="7"/>
+      <c r="J42" s="37">
         <v>15</v>
       </c>
-      <c r="J42" s="38">
+      <c r="K42" s="38">
         <v>15</v>
       </c>
-      <c r="K42" s="39" t="s">
+      <c r="L42" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="L42" s="39"/>
       <c r="M42" s="39"/>
       <c r="N42" s="39"/>
-      <c r="O42" s="39" t="s">
+      <c r="O42" s="39"/>
+      <c r="P42" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="P42" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="V42" s="26"/>
+      <c r="Q42" s="8" t="s">
+        <v>165</v>
+      </c>
       <c r="W42" s="26"/>
-      <c r="X42" s="27"/>
-      <c r="Y42" s="9"/>
+      <c r="X42" s="26"/>
+      <c r="Y42" s="27"/>
       <c r="Z42" s="9"/>
       <c r="AA42" s="9"/>
       <c r="AB42" s="9"/>
       <c r="AC42" s="9"/>
-    </row>
-    <row r="43" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD42" s="9"/>
+    </row>
+    <row r="43" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A43" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="B43" s="39"/>
+      <c r="B43" s="8"/>
       <c r="C43" s="39"/>
-      <c r="D43" s="39" t="s">
+      <c r="D43" s="39"/>
+      <c r="E43" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="E43" s="39"/>
-      <c r="F43" s="39">
+      <c r="F43" s="39"/>
+      <c r="G43" s="39">
         <v>11</v>
       </c>
-      <c r="G43" s="3">
+      <c r="H43" s="3">
         <v>11</v>
       </c>
-      <c r="H43" s="7"/>
-      <c r="I43" s="37">
+      <c r="I43" s="7"/>
+      <c r="J43" s="37">
         <v>14</v>
       </c>
-      <c r="J43" s="38">
+      <c r="K43" s="38">
         <v>14</v>
       </c>
-      <c r="K43" s="39" t="s">
+      <c r="L43" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="L43" s="39"/>
       <c r="M43" s="39"/>
       <c r="N43" s="39"/>
       <c r="O43" s="39"/>
-      <c r="P43" s="8" t="s">
+      <c r="P43" s="39"/>
+      <c r="Q43" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="V43" s="26"/>
       <c r="W43" s="26"/>
-      <c r="X43" s="9"/>
+      <c r="X43" s="26"/>
       <c r="Y43" s="9"/>
       <c r="Z43" s="9"/>
       <c r="AA43" s="9"/>
       <c r="AB43" s="9"/>
       <c r="AC43" s="9"/>
-    </row>
-    <row r="44" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD43" s="9"/>
+    </row>
+    <row r="44" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A44" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="B44" s="39"/>
+      <c r="B44" s="8"/>
       <c r="C44" s="39"/>
-      <c r="D44" s="39" t="s">
+      <c r="D44" s="39"/>
+      <c r="E44" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="E44" s="39"/>
-      <c r="F44" s="39">
+      <c r="F44" s="39"/>
+      <c r="G44" s="39">
         <v>12</v>
       </c>
-      <c r="G44" s="3">
+      <c r="H44" s="3">
         <v>12</v>
       </c>
-      <c r="H44" s="7"/>
-      <c r="I44" s="37" t="s">
+      <c r="I44" s="7"/>
+      <c r="J44" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="J44" s="38">
+      <c r="K44" s="38">
         <v>13</v>
       </c>
-      <c r="K44" s="39"/>
       <c r="L44" s="39"/>
-      <c r="M44" s="39" t="s">
+      <c r="M44" s="39"/>
+      <c r="N44" s="39" t="s">
         <v>124</v>
       </c>
-      <c r="N44" s="39"/>
       <c r="O44" s="39"/>
-      <c r="P44" s="8" t="s">
+      <c r="P44" s="39"/>
+      <c r="Q44" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="Q44" s="8" t="s">
+      <c r="R44" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="V44" s="26"/>
       <c r="W44" s="26"/>
-      <c r="X44" s="9"/>
+      <c r="X44" s="26"/>
       <c r="Y44" s="9"/>
       <c r="Z44" s="9"/>
       <c r="AA44" s="9"/>
       <c r="AB44" s="9"/>
       <c r="AC44" s="9"/>
-    </row>
-    <row r="45" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD44" s="9"/>
+    </row>
+    <row r="45" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>51</v>
       </c>
-      <c r="G45" s="16" t="s">
+      <c r="H45" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="H45" s="12"/>
-      <c r="I45" s="17" t="s">
+      <c r="I45" s="12"/>
+      <c r="J45" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="J45" s="7"/>
-      <c r="P45" t="s">
+      <c r="K45" s="7"/>
+      <c r="Q45" t="s">
         <v>51</v>
       </c>
-      <c r="V45" s="26"/>
       <c r="W45" s="26"/>
-      <c r="X45" s="9"/>
+      <c r="X45" s="26"/>
       <c r="Y45" s="9"/>
       <c r="Z45" s="9"/>
       <c r="AA45" s="9"/>
       <c r="AB45" s="9"/>
       <c r="AC45" s="9"/>
-    </row>
-    <row r="46" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD45" s="9"/>
+    </row>
+    <row r="46" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A46" s="15" t="s">
         <v>134</v>
       </c>
-      <c r="F46" s="14">
+      <c r="B46" s="15"/>
+      <c r="G46" s="14">
         <v>17</v>
       </c>
-      <c r="G46" s="3" t="s">
+      <c r="H46" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I46" s="37" t="s">
+      <c r="J46" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="J46" s="38" t="s">
+      <c r="K46" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="K46" s="39"/>
       <c r="L46" s="39"/>
       <c r="M46" s="39"/>
       <c r="N46" s="39"/>
       <c r="O46" s="39"/>
-      <c r="P46" s="8" t="s">
+      <c r="P46" s="39"/>
+      <c r="Q46" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="V46" s="26"/>
       <c r="W46" s="26"/>
-      <c r="X46" s="9"/>
+      <c r="X46" s="26"/>
       <c r="Y46" s="9"/>
       <c r="Z46" s="9"/>
       <c r="AA46" s="9"/>
       <c r="AB46" s="9"/>
       <c r="AC46" s="9"/>
-    </row>
-    <row r="47" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD46" s="9"/>
+    </row>
+    <row r="47" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A47" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="F47" s="14" t="s">
+      <c r="B47" s="15"/>
+      <c r="G47" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="G47" s="44" t="s">
+      <c r="H47" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="H47" s="43" t="s">
+      <c r="I47" s="43" t="s">
         <v>131</v>
       </c>
-      <c r="I47" s="42">
+      <c r="J47" s="42">
         <v>24</v>
       </c>
-      <c r="J47" s="43">
+      <c r="K47" s="43">
         <v>24</v>
       </c>
-      <c r="K47" s="26" t="s">
+      <c r="L47" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="L47" s="26"/>
       <c r="M47" s="26"/>
       <c r="N47" s="26"/>
       <c r="O47" s="26"/>
-      <c r="P47" s="15"/>
-      <c r="V47" s="26"/>
+      <c r="P47" s="26"/>
+      <c r="Q47" s="15"/>
       <c r="W47" s="26"/>
-      <c r="X47" s="9"/>
+      <c r="X47" s="26"/>
       <c r="Y47" s="9"/>
       <c r="Z47" s="9"/>
       <c r="AA47" s="9"/>
       <c r="AB47" s="9"/>
       <c r="AC47" s="9"/>
-    </row>
-    <row r="48" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD47" s="9"/>
+    </row>
+    <row r="48" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A48" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="F48" s="14" t="s">
+      <c r="B48" s="15"/>
+      <c r="G48" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="G48" s="44" t="s">
+      <c r="H48" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="H48" s="43" t="s">
+      <c r="I48" s="43" t="s">
         <v>132</v>
       </c>
-      <c r="I48" s="42">
+      <c r="J48" s="42">
         <v>25</v>
       </c>
-      <c r="J48" s="43">
+      <c r="K48" s="43">
         <v>25</v>
       </c>
-      <c r="K48" s="26" t="s">
+      <c r="L48" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="L48" s="26"/>
       <c r="M48" s="26"/>
       <c r="N48" s="26"/>
       <c r="O48" s="26"/>
-      <c r="P48" s="15"/>
-      <c r="V48" s="26"/>
+      <c r="P48" s="26"/>
+      <c r="Q48" s="15"/>
       <c r="W48" s="26"/>
-      <c r="X48" s="9"/>
+      <c r="X48" s="26"/>
       <c r="Y48" s="9"/>
       <c r="Z48" s="9"/>
       <c r="AA48" s="9"/>
       <c r="AB48" s="9"/>
       <c r="AC48" s="9"/>
-    </row>
-    <row r="49" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD48" s="9"/>
+    </row>
+    <row r="49" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A49" s="15"/>
-      <c r="F49" s="14" t="s">
+      <c r="B49" s="15"/>
+      <c r="G49" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="G49" s="44" t="s">
+      <c r="H49" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="H49" s="43" t="s">
+      <c r="I49" s="43" t="s">
         <v>133</v>
       </c>
-      <c r="I49" s="40" t="s">
+      <c r="J49" s="40" t="s">
         <v>66</v>
       </c>
-      <c r="J49" s="35"/>
-      <c r="K49" s="25"/>
+      <c r="K49" s="35"/>
       <c r="L49" s="25"/>
       <c r="M49" s="25"/>
       <c r="N49" s="25"/>
       <c r="O49" s="25"/>
-      <c r="P49" s="24" t="s">
+      <c r="P49" s="25"/>
+      <c r="Q49" s="24" t="s">
         <v>148</v>
       </c>
-      <c r="V49" s="26"/>
       <c r="W49" s="26"/>
-      <c r="X49" s="9"/>
+      <c r="X49" s="26"/>
       <c r="Y49" s="9"/>
       <c r="Z49" s="9"/>
       <c r="AA49" s="9"/>
       <c r="AB49" s="9"/>
       <c r="AC49" s="9"/>
-    </row>
-    <row r="50" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AD49" s="9"/>
+    </row>
+    <row r="50" spans="1:30" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="15"/>
-      <c r="F50" s="14">
+      <c r="B50" s="15"/>
+      <c r="G50" s="14">
         <v>26</v>
       </c>
-      <c r="G50" s="5" t="s">
+      <c r="H50" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H50" s="13"/>
-      <c r="I50" s="6"/>
-      <c r="J50" s="7"/>
-      <c r="P50" t="s">
+      <c r="I50" s="13"/>
+      <c r="J50" s="6"/>
+      <c r="K50" s="7"/>
+      <c r="Q50" t="s">
         <v>51</v>
       </c>
-      <c r="V50" s="26"/>
-      <c r="W50" s="28"/>
-      <c r="X50" s="9"/>
+      <c r="W50" s="26"/>
+      <c r="X50" s="28"/>
       <c r="Y50" s="9"/>
       <c r="Z50" s="9"/>
       <c r="AA50" s="9"/>
       <c r="AB50" s="9"/>
       <c r="AC50" s="9"/>
-    </row>
-    <row r="51" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="F51" s="7"/>
-      <c r="G51" s="45" t="s">
+      <c r="AD50" s="9"/>
+    </row>
+    <row r="51" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="G51" s="7"/>
+      <c r="H51" s="45" t="s">
         <v>139</v>
       </c>
-      <c r="V51" s="26"/>
       <c r="W51" s="26"/>
-      <c r="X51" s="9"/>
+      <c r="X51" s="26"/>
       <c r="Y51" s="9"/>
       <c r="Z51" s="9"/>
       <c r="AA51" s="9"/>
       <c r="AB51" s="9"/>
       <c r="AC51" s="9"/>
-    </row>
-    <row r="52" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="H52" s="10"/>
-      <c r="V52" s="26"/>
+      <c r="AD51" s="9"/>
+    </row>
+    <row r="52" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="I52" s="10"/>
       <c r="W52" s="26"/>
-      <c r="X52" s="9"/>
+      <c r="X52" s="26"/>
       <c r="Y52" s="9"/>
       <c r="Z52" s="9"/>
       <c r="AA52" s="9"/>
       <c r="AB52" s="9"/>
       <c r="AC52" s="9"/>
-    </row>
-    <row r="53" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD52" s="9"/>
+    </row>
+    <row r="53" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>146</v>
       </c>
-      <c r="V53" s="26"/>
       <c r="W53" s="26"/>
-      <c r="X53" s="9"/>
+      <c r="X53" s="26"/>
       <c r="Y53" s="9"/>
       <c r="Z53" s="9"/>
       <c r="AA53" s="9"/>
       <c r="AB53" s="9"/>
       <c r="AC53" s="9"/>
-    </row>
-    <row r="54" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD53" s="9"/>
+    </row>
+    <row r="54" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A54" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="G54" s="8"/>
-      <c r="H54" s="23" t="s">
+      <c r="B54" s="22"/>
+      <c r="H54" s="8"/>
+      <c r="I54" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="I54" s="8"/>
-    </row>
-    <row r="55" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="J54" s="8"/>
+    </row>
+    <row r="55" spans="1:30" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="B55" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="C55" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C55" s="14" t="s">
+      <c r="D55" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D55" s="14" t="s">
+      <c r="E55" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E55" s="14" t="s">
+      <c r="F55" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="F55" s="14" t="s">
+      <c r="G55" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="G55" t="s">
+      <c r="H55" t="s">
         <v>5</v>
       </c>
-      <c r="I55" t="s">
+      <c r="J55" t="s">
         <v>5</v>
       </c>
-      <c r="J55" s="14" t="s">
+      <c r="K55" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="K55" s="14" t="s">
+      <c r="L55" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="L55" s="14" t="s">
+      <c r="M55" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="M55" s="14" t="s">
+      <c r="N55" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="N55" s="14" t="s">
+      <c r="O55" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="O55" s="14" t="s">
+      <c r="P55" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="P55" t="s">
+      <c r="Q55" t="s">
         <v>102</v>
       </c>
-      <c r="Q55" s="14" t="s">
+      <c r="R55" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="R55" t="s">
+      <c r="S55" t="s">
         <v>110</v>
       </c>
-      <c r="S55" s="14" t="s">
+      <c r="T55" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="T55" t="s">
+      <c r="U55" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="56" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A56" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="B56" s="32"/>
+      <c r="B56" s="29"/>
       <c r="C56" s="32"/>
       <c r="D56" s="32"/>
       <c r="E56" s="32"/>
       <c r="F56" s="32"/>
-      <c r="G56" s="30" t="s">
+      <c r="G56" s="32"/>
+      <c r="H56" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="I56" s="34" t="s">
+      <c r="J56" s="34" t="s">
         <v>149</v>
       </c>
-      <c r="J56" s="35"/>
-      <c r="K56" s="25"/>
+      <c r="K56" s="35"/>
       <c r="L56" s="25"/>
       <c r="M56" s="25"/>
       <c r="N56" s="25"/>
       <c r="O56" s="25"/>
-      <c r="P56" s="36" t="s">
+      <c r="P56" s="25"/>
+      <c r="Q56" s="36" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="57" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A57" s="8" t="s">
-        <v>175</v>
-      </c>
-      <c r="B57" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="B57" s="8"/>
+      <c r="C57" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="E57" s="14" t="s">
+      <c r="F57" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="F57" s="14">
+      <c r="G57" s="14">
         <v>0</v>
       </c>
-      <c r="G57" s="3">
+      <c r="H57" s="3">
         <v>0</v>
       </c>
-      <c r="H57" s="7"/>
-      <c r="I57" s="31" t="s">
+      <c r="I57" s="7"/>
+      <c r="J57" s="31" t="s">
         <v>130</v>
       </c>
-      <c r="J57" s="33"/>
-      <c r="K57" s="32"/>
+      <c r="K57" s="33"/>
       <c r="L57" s="32"/>
       <c r="M57" s="32"/>
       <c r="N57" s="32"/>
       <c r="O57" s="32"/>
-      <c r="P57" s="29" t="s">
+      <c r="P57" s="32"/>
+      <c r="Q57" s="29" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="58" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A58" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="B58" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="B58" s="8"/>
+      <c r="C58" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="E58" s="14" t="s">
+      <c r="F58" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="F58" s="14">
+      <c r="G58" s="14">
         <v>1</v>
       </c>
-      <c r="G58" s="3">
+      <c r="H58" s="3">
         <v>1</v>
       </c>
-      <c r="H58" s="7"/>
-      <c r="I58" s="40" t="s">
+      <c r="I58" s="7"/>
+      <c r="J58" s="40" t="s">
         <v>127</v>
       </c>
-      <c r="J58" s="35"/>
-      <c r="K58" s="25"/>
+      <c r="K58" s="35"/>
       <c r="L58" s="25"/>
       <c r="M58" s="25"/>
       <c r="N58" s="25"/>
       <c r="O58" s="25"/>
-      <c r="P58" s="24" t="s">
+      <c r="P58" s="25"/>
+      <c r="Q58" s="24" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="59" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A59" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="F59" s="14">
+        <v>177</v>
+      </c>
+      <c r="B59" s="56" t="s">
+        <v>195</v>
+      </c>
+      <c r="G59" s="14">
         <v>2</v>
       </c>
-      <c r="G59" s="3">
+      <c r="H59" s="3">
         <v>2</v>
       </c>
-      <c r="H59" s="7"/>
-      <c r="I59" s="37">
+      <c r="I59" s="7"/>
+      <c r="J59" s="37">
         <v>23</v>
       </c>
-      <c r="J59" s="38">
+      <c r="K59" s="38">
         <v>23</v>
       </c>
-      <c r="K59" s="39" t="s">
+      <c r="L59" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="L59" s="39"/>
       <c r="M59" s="39"/>
-      <c r="N59" s="39" t="s">
+      <c r="N59" s="39"/>
+      <c r="O59" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="O59" s="39" t="s">
+      <c r="P59" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="P59" s="8" t="s">
+      <c r="Q59" s="8" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="60" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A60" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="C60" s="14" t="s">
+      <c r="B60" s="56" t="s">
+        <v>196</v>
+      </c>
+      <c r="D60" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E60" s="14" t="s">
+      <c r="F60" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="F60" s="14">
+      <c r="G60" s="14">
         <v>3</v>
       </c>
-      <c r="G60" s="3">
+      <c r="H60" s="3">
         <v>3</v>
       </c>
-      <c r="H60" s="7"/>
-      <c r="I60" s="37">
+      <c r="I60" s="7"/>
+      <c r="J60" s="37">
         <v>22</v>
       </c>
-      <c r="J60" s="38">
+      <c r="K60" s="38">
         <v>22</v>
       </c>
-      <c r="K60" s="39" t="s">
+      <c r="L60" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="L60" s="39"/>
       <c r="M60" s="39"/>
-      <c r="N60" s="39" t="s">
+      <c r="N60" s="39"/>
+      <c r="O60" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="O60" s="39" t="s">
+      <c r="P60" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="P60" s="8" t="s">
+      <c r="Q60" s="8" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="61" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A61" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="C61" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="D61" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E61" s="14" t="s">
+      <c r="F61" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="F61" s="14">
+      <c r="G61" s="14">
         <v>4</v>
       </c>
-      <c r="G61" s="3">
+      <c r="H61" s="3">
         <v>4</v>
       </c>
-      <c r="H61" s="7"/>
-      <c r="I61" s="37">
+      <c r="I61" s="7"/>
+      <c r="J61" s="37">
         <v>21</v>
       </c>
-      <c r="J61" s="38">
+      <c r="K61" s="38">
         <v>21</v>
       </c>
-      <c r="K61" s="39" t="s">
+      <c r="L61" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="L61" s="39"/>
-      <c r="M61" s="39" t="s">
+      <c r="M61" s="39"/>
+      <c r="N61" s="39" t="s">
         <v>122</v>
       </c>
-      <c r="N61" s="39" t="s">
+      <c r="O61" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="O61" s="39"/>
-      <c r="P61" s="8" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="62" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="P61" s="39"/>
+      <c r="Q61" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="R61" s="39" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="62" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A62" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="C62" s="14" t="s">
+      <c r="B62" s="56" t="s">
+        <v>199</v>
+      </c>
+      <c r="D62" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="F62" s="14">
+      <c r="G62" s="14">
         <v>5</v>
       </c>
-      <c r="G62" s="3">
+      <c r="H62" s="3">
         <v>5</v>
       </c>
-      <c r="H62" s="7"/>
-      <c r="I62" s="37">
+      <c r="I62" s="7"/>
+      <c r="J62" s="37">
         <v>20</v>
       </c>
-      <c r="J62" s="38">
+      <c r="K62" s="38">
         <v>20</v>
       </c>
-      <c r="K62" s="39" t="s">
+      <c r="L62" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="L62" s="39"/>
-      <c r="M62" s="39" t="s">
+      <c r="M62" s="39"/>
+      <c r="N62" s="39" t="s">
         <v>122</v>
       </c>
-      <c r="N62" s="39" t="s">
+      <c r="O62" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="O62" s="39"/>
-      <c r="P62" s="8" t="s">
+      <c r="P62" s="39"/>
+      <c r="Q62" s="8" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="63" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="R62" s="39" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="63" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A63" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="C63" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="B63" s="53" t="s">
+        <v>166</v>
+      </c>
+      <c r="D63" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="F63" s="14">
+      <c r="G63" s="14">
         <v>6</v>
       </c>
-      <c r="G63" s="3">
+      <c r="H63" s="3">
         <v>6</v>
       </c>
-      <c r="H63" s="7"/>
-      <c r="I63" s="37">
+      <c r="I63" s="7"/>
+      <c r="J63" s="37">
         <v>19</v>
       </c>
-      <c r="J63" s="38">
+      <c r="K63" s="38">
         <v>19</v>
       </c>
-      <c r="K63" s="39" t="s">
+      <c r="L63" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="L63" s="39" t="s">
+      <c r="M63" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="M63" s="39"/>
       <c r="N63" s="39"/>
-      <c r="O63" s="39" t="s">
+      <c r="O63" s="39"/>
+      <c r="P63" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="P63" s="8" t="s">
-        <v>159</v>
-      </c>
       <c r="Q63" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="R63" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="R63" s="8" t="s">
+      <c r="S63" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="S63" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="T63" s="8"/>
-    </row>
-    <row r="64" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="T63" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="U63" s="8"/>
+    </row>
+    <row r="64" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A64" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="E64" s="14" t="s">
+      <c r="B64" s="8"/>
+      <c r="F64" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="F64" s="14">
+      <c r="G64" s="14">
         <v>7</v>
       </c>
-      <c r="G64" s="3">
+      <c r="H64" s="3">
         <v>7</v>
       </c>
-      <c r="H64" s="7"/>
-      <c r="I64" s="37">
+      <c r="I64" s="7"/>
+      <c r="J64" s="37">
         <v>18</v>
       </c>
-      <c r="J64" s="38">
+      <c r="K64" s="38">
         <v>18</v>
       </c>
-      <c r="K64" s="39" t="s">
+      <c r="L64" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="L64" s="39" t="s">
+      <c r="M64" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="M64" s="39"/>
       <c r="N64" s="39"/>
-      <c r="O64" s="39" t="s">
+      <c r="O64" s="39"/>
+      <c r="P64" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="P64" s="8" t="s">
-        <v>159</v>
-      </c>
       <c r="Q64" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="R64" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="R64" s="8" t="s">
+      <c r="S64" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="S64" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="T64" s="8"/>
-    </row>
-    <row r="65" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="T64" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="U64" s="8"/>
+    </row>
+    <row r="65" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A65" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="E65" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="B65" s="55" t="s">
+        <v>193</v>
+      </c>
+      <c r="F65" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="F65" s="14">
+      <c r="G65" s="14">
         <v>8</v>
       </c>
-      <c r="G65" s="3">
+      <c r="H65" s="3">
         <v>8</v>
       </c>
-      <c r="H65" s="7"/>
-      <c r="I65" s="37">
+      <c r="I65" s="7"/>
+      <c r="J65" s="37">
         <v>17</v>
       </c>
-      <c r="J65" s="38">
+      <c r="K65" s="38">
         <v>17</v>
       </c>
-      <c r="K65" s="39" t="s">
+      <c r="L65" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="L65" s="46" t="s">
+      <c r="M65" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="M65" s="39"/>
-      <c r="N65" s="39" t="s">
+      <c r="N65" s="39"/>
+      <c r="O65" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="O65" s="39" t="s">
+      <c r="P65" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="P65" s="8" t="s">
+      <c r="Q65" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="Q65" s="53" t="s">
-        <v>174</v>
-      </c>
-      <c r="R65" s="51"/>
+      <c r="R65" s="52" t="s">
+        <v>191</v>
+      </c>
       <c r="S65" s="51"/>
-    </row>
-    <row r="66" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="T65" s="51"/>
+    </row>
+    <row r="66" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A66" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="B66" s="51" t="s">
-        <v>167</v>
-      </c>
-      <c r="C66" s="14" t="s">
+      <c r="B66" s="55" t="s">
+        <v>194</v>
+      </c>
+      <c r="D66" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E66" s="14" t="s">
+      <c r="F66" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="F66" s="14">
+      <c r="G66" s="14">
         <v>9</v>
       </c>
-      <c r="G66" s="3">
+      <c r="H66" s="3">
         <v>9</v>
       </c>
-      <c r="H66" s="7"/>
-      <c r="I66" s="37">
+      <c r="I66" s="7"/>
+      <c r="J66" s="37">
         <v>16</v>
       </c>
-      <c r="J66" s="38">
+      <c r="K66" s="38">
         <v>16</v>
       </c>
-      <c r="K66" s="39" t="s">
+      <c r="L66" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="L66" s="46" t="s">
+      <c r="M66" s="46" t="s">
         <v>40</v>
       </c>
-      <c r="M66" s="39"/>
-      <c r="N66" s="39" t="s">
+      <c r="N66" s="39"/>
+      <c r="O66" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="O66" s="39" t="s">
+      <c r="P66" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="P66" s="8" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="67" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A67" s="51" t="s">
-        <v>166</v>
-      </c>
-      <c r="C67" s="14" t="s">
+      <c r="Q66" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="R66" s="55" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="67" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A67" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="B67" s="56" t="s">
+        <v>200</v>
+      </c>
+      <c r="D67" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D67" s="14" t="s">
+      <c r="E67" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="E67" s="14" t="s">
+      <c r="F67" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="F67" s="14">
+      <c r="G67" s="14">
         <v>10</v>
       </c>
-      <c r="G67" s="3">
+      <c r="H67" s="3">
         <v>10</v>
       </c>
-      <c r="H67" s="7"/>
-      <c r="I67" s="37">
+      <c r="I67" s="7"/>
+      <c r="J67" s="37">
         <v>15</v>
       </c>
-      <c r="J67" s="38">
+      <c r="K67" s="38">
         <v>15</v>
       </c>
-      <c r="K67" s="39" t="s">
+      <c r="L67" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="L67" s="39"/>
       <c r="M67" s="39"/>
       <c r="N67" s="39"/>
-      <c r="O67" s="39" t="s">
+      <c r="O67" s="39"/>
+      <c r="P67" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="P67" s="8" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="68" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="Q67" s="56" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="68" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A68" s="51" t="s">
-        <v>168</v>
-      </c>
-      <c r="D68" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="E68" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="F68" s="14">
+      <c r="G68" s="14">
         <v>11</v>
       </c>
-      <c r="G68" s="3">
+      <c r="H68" s="3">
         <v>11</v>
       </c>
-      <c r="H68" s="7"/>
-      <c r="I68" s="37">
+      <c r="I68" s="7"/>
+      <c r="J68" s="37">
         <v>14</v>
       </c>
-      <c r="J68" s="38">
+      <c r="K68" s="38">
         <v>14</v>
       </c>
-      <c r="K68" s="39" t="s">
+      <c r="L68" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="L68" s="39"/>
       <c r="M68" s="39"/>
       <c r="N68" s="39"/>
       <c r="O68" s="39"/>
-      <c r="P68" s="51" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="69" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="P68" s="39"/>
+      <c r="Q68" s="54" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="69" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A69" s="51" t="s">
-        <v>169</v>
-      </c>
-      <c r="D69" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="B69" s="14"/>
+      <c r="E69" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="F69" s="14">
+      <c r="G69" s="14">
         <v>12</v>
       </c>
-      <c r="G69" s="3">
+      <c r="H69" s="3">
         <v>12</v>
       </c>
-      <c r="H69" s="7"/>
-      <c r="I69" s="37" t="s">
+      <c r="I69" s="7"/>
+      <c r="J69" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="J69" s="38">
+      <c r="K69" s="38">
         <v>13</v>
       </c>
-      <c r="K69" s="39"/>
       <c r="L69" s="39"/>
-      <c r="M69" s="39" t="s">
+      <c r="M69" s="39"/>
+      <c r="N69" s="39" t="s">
         <v>124</v>
       </c>
-      <c r="N69" s="39"/>
       <c r="O69" s="39"/>
-      <c r="P69" s="8" t="s">
-        <v>115</v>
-      </c>
+      <c r="P69" s="39"/>
       <c r="Q69" s="51" t="s">
-        <v>170</v>
-      </c>
-      <c r="R69" s="51"/>
-    </row>
-    <row r="70" spans="1:21" x14ac:dyDescent="0.2">
+        <v>190</v>
+      </c>
+      <c r="R69" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="S69" s="9"/>
+    </row>
+    <row r="70" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>51</v>
       </c>
-      <c r="G70" s="16" t="s">
+      <c r="H70" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="H70" s="12"/>
-      <c r="I70" s="17" t="s">
+      <c r="I70" s="12"/>
+      <c r="J70" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="J70" s="7"/>
-      <c r="P70" t="s">
+      <c r="K70" s="7"/>
+      <c r="Q70" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="71" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A71" s="15" t="s">
         <v>134</v>
       </c>
-      <c r="F71" s="14" t="s">
+      <c r="B71" s="15"/>
+      <c r="G71" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="G71" s="3" t="s">
+      <c r="H71" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="I71" s="37" t="s">
+      <c r="J71" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="J71" s="38" t="s">
+      <c r="K71" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="K71" s="39"/>
       <c r="L71" s="39"/>
       <c r="M71" s="39"/>
       <c r="N71" s="39"/>
       <c r="O71" s="39"/>
-      <c r="P71" s="8" t="s">
+      <c r="P71" s="39"/>
+      <c r="Q71" s="8" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="72" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A72" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="F72" s="14" t="s">
+      <c r="B72" s="15"/>
+      <c r="G72" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="G72" s="44" t="s">
+      <c r="H72" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="H72" s="43" t="s">
+      <c r="I72" s="43" t="s">
         <v>131</v>
       </c>
-      <c r="I72" s="37" t="s">
+      <c r="J72" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="J72" s="38"/>
-      <c r="K72" s="39" t="s">
+      <c r="K72" s="38"/>
+      <c r="L72" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="L72" s="39"/>
       <c r="M72" s="39"/>
       <c r="N72" s="39"/>
       <c r="O72" s="39"/>
-      <c r="P72" s="8" t="s">
+      <c r="P72" s="39"/>
+      <c r="Q72" s="8" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="73" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A73" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="F73" s="14" t="s">
+      <c r="B73" s="15"/>
+      <c r="G73" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="G73" s="44" t="s">
+      <c r="H73" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="H73" s="43" t="s">
+      <c r="I73" s="43" t="s">
         <v>132</v>
       </c>
-      <c r="I73" s="37" t="s">
+      <c r="J73" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="J73" s="38"/>
-      <c r="K73" s="39" t="s">
+      <c r="K73" s="38"/>
+      <c r="L73" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="L73" s="39"/>
       <c r="M73" s="39"/>
       <c r="N73" s="39"/>
       <c r="O73" s="39"/>
-      <c r="P73" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="Q73" s="52" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="74" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="P73" s="39"/>
+      <c r="Q73" s="8" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="74" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A74" s="15"/>
-      <c r="F74" s="14" t="s">
+      <c r="B74" s="15"/>
+      <c r="G74" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="G74" s="44" t="s">
+      <c r="H74" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="H74" s="43" t="s">
+      <c r="I74" s="43" t="s">
         <v>133</v>
       </c>
-      <c r="I74" s="40" t="s">
+      <c r="J74" s="40" t="s">
         <v>66</v>
       </c>
-      <c r="J74" s="35"/>
-      <c r="K74" s="25"/>
+      <c r="K74" s="35"/>
       <c r="L74" s="25"/>
       <c r="M74" s="25"/>
       <c r="N74" s="25"/>
       <c r="O74" s="25"/>
-      <c r="P74" s="24" t="s">
+      <c r="P74" s="25"/>
+      <c r="Q74" s="24" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="75" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A75" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="F75" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="B75" s="8"/>
+      <c r="G75" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="G75" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="H75" s="13"/>
-      <c r="I75" s="6"/>
-      <c r="J75" s="7"/>
-      <c r="P75" t="s">
+      <c r="H75" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="I75" s="13"/>
+      <c r="J75" s="6"/>
+      <c r="K75" s="7"/>
+      <c r="Q75" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="76" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="I76" s="47" t="s">
+    <row r="76" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="J76" s="47" t="s">
         <v>128</v>
       </c>
-      <c r="J76" s="39"/>
-      <c r="K76" s="39" t="s">
+      <c r="K76" s="39"/>
+      <c r="L76" s="39" t="s">
         <v>128</v>
       </c>
-      <c r="L76" s="39"/>
       <c r="M76" s="39"/>
       <c r="N76" s="39"/>
       <c r="O76" s="39"/>
-      <c r="P76" s="8" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="77" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="I77" s="48" t="s">
+      <c r="P76" s="39"/>
+      <c r="Q76" s="8" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="77" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="J77" s="48" t="s">
         <v>129</v>
       </c>
-      <c r="J77" s="39"/>
-      <c r="K77" s="39" t="s">
+      <c r="K77" s="39"/>
+      <c r="L77" s="39" t="s">
         <v>129</v>
       </c>
-      <c r="L77" s="39"/>
       <c r="M77" s="39"/>
       <c r="N77" s="39"/>
       <c r="O77" s="39"/>
-      <c r="P77" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="U77" t="s">
+      <c r="P77" s="39"/>
+      <c r="Q77" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="V77" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="78" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="I78" s="49" t="s">
+    <row r="78" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="J78" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="J78" s="32"/>
       <c r="K78" s="32"/>
       <c r="L78" s="32"/>
       <c r="M78" s="32"/>
       <c r="N78" s="32"/>
       <c r="O78" s="32"/>
-      <c r="P78" s="29" t="s">
+      <c r="P78" s="32"/>
+      <c r="Q78" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="U78" t="s">
+      <c r="V78" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="79" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="I79" s="41" t="s">
+    <row r="79" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="J79" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="P79" s="15"/>
-      <c r="U79" t="s">
+      <c r="Q79" s="15"/>
+      <c r="V79" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="80" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="I80" s="48">
+    <row r="80" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="J80" s="48">
         <v>24</v>
       </c>
-      <c r="J80" s="39">
+      <c r="K80" s="39">
         <v>24</v>
       </c>
-      <c r="K80" s="39"/>
       <c r="L80" s="39"/>
       <c r="M80" s="39"/>
       <c r="N80" s="39"/>
       <c r="O80" s="39"/>
-      <c r="P80" s="8" t="s">
+      <c r="P80" s="39"/>
+      <c r="Q80" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="U80" t="s">
+      <c r="V80" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="81" spans="7:21" x14ac:dyDescent="0.2">
-      <c r="I81" s="48">
+    <row r="81" spans="8:22" x14ac:dyDescent="0.2">
+      <c r="J81" s="48">
         <v>25</v>
       </c>
-      <c r="J81" s="39">
+      <c r="K81" s="39">
         <v>25</v>
       </c>
-      <c r="K81" s="39"/>
       <c r="L81" s="39"/>
       <c r="M81" s="39"/>
       <c r="N81" s="39"/>
-      <c r="O81" s="39"/>
-      <c r="P81" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="U81" t="s">
+      <c r="O81" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="P81" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q81" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="V81" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="82" spans="7:21" x14ac:dyDescent="0.2">
-      <c r="I82" s="48">
+    <row r="82" spans="8:22" x14ac:dyDescent="0.2">
+      <c r="J82" s="48">
         <v>26</v>
       </c>
-      <c r="J82" s="39">
+      <c r="K82" s="39">
         <v>26</v>
       </c>
-      <c r="K82" s="39"/>
-      <c r="L82" s="39"/>
+      <c r="L82" s="39" t="s">
+        <v>171</v>
+      </c>
       <c r="M82" s="39"/>
       <c r="N82" s="39"/>
       <c r="O82" s="39"/>
-      <c r="P82" s="8" t="s">
+      <c r="P82" s="39"/>
+      <c r="Q82" s="8" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="83" spans="7:21" x14ac:dyDescent="0.2">
-      <c r="I83" s="48">
+    <row r="83" spans="8:22" x14ac:dyDescent="0.2">
+      <c r="J83" s="48">
         <v>27</v>
       </c>
-      <c r="J83" s="39">
+      <c r="K83" s="39">
         <v>27</v>
       </c>
-      <c r="K83" s="39"/>
-      <c r="L83" s="39"/>
+      <c r="L83" s="39" t="s">
+        <v>172</v>
+      </c>
       <c r="M83" s="39"/>
       <c r="N83" s="39"/>
       <c r="O83" s="39"/>
-      <c r="P83" s="8" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="84" spans="7:21" x14ac:dyDescent="0.2">
-      <c r="I84" s="48">
+      <c r="P83" s="39"/>
+      <c r="Q83" s="8" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="84" spans="8:22" x14ac:dyDescent="0.2">
+      <c r="J84" s="48">
         <v>28</v>
       </c>
-      <c r="J84" s="39">
+      <c r="K84" s="39">
         <v>28</v>
       </c>
-      <c r="K84" s="39"/>
-      <c r="L84" s="39"/>
+      <c r="L84" s="39" t="s">
+        <v>173</v>
+      </c>
       <c r="M84" s="39"/>
       <c r="N84" s="39"/>
       <c r="O84" s="39"/>
-      <c r="P84" s="8" t="s">
+      <c r="P84" s="39"/>
+      <c r="Q84" s="8" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="85" spans="7:21" x14ac:dyDescent="0.2">
-      <c r="I85" s="48">
+    <row r="85" spans="8:22" x14ac:dyDescent="0.2">
+      <c r="J85" s="48">
         <v>29</v>
       </c>
-      <c r="J85" s="39">
+      <c r="K85" s="39">
         <v>29</v>
       </c>
-      <c r="K85" s="39"/>
-      <c r="L85" s="39"/>
+      <c r="L85" s="39" t="s">
+        <v>174</v>
+      </c>
       <c r="M85" s="39"/>
       <c r="N85" s="39"/>
       <c r="O85" s="39"/>
-      <c r="P85" s="8" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="86" spans="7:21" x14ac:dyDescent="0.2">
-      <c r="I86" s="48">
+      <c r="P85" s="39"/>
+      <c r="Q85" s="8" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="86" spans="8:22" x14ac:dyDescent="0.2">
+      <c r="J86" s="48">
         <v>30</v>
       </c>
-      <c r="J86" s="39">
+      <c r="K86" s="39">
         <v>30</v>
       </c>
-      <c r="K86" s="39"/>
-      <c r="L86" s="39"/>
+      <c r="L86" s="39" t="s">
+        <v>175</v>
+      </c>
       <c r="M86" s="39"/>
       <c r="N86" s="39"/>
       <c r="O86" s="39"/>
-      <c r="P86" s="8" t="s">
+      <c r="P86" s="39"/>
+      <c r="Q86" s="8" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="87" spans="7:21" x14ac:dyDescent="0.2">
-      <c r="I87" s="48">
+    <row r="87" spans="8:22" x14ac:dyDescent="0.2">
+      <c r="J87" s="48">
         <v>31</v>
       </c>
-      <c r="J87" s="39">
+      <c r="K87" s="39">
         <v>31</v>
       </c>
-      <c r="K87" s="39"/>
-      <c r="L87" s="39"/>
+      <c r="L87" s="39" t="s">
+        <v>176</v>
+      </c>
       <c r="M87" s="39"/>
       <c r="N87" s="39"/>
       <c r="O87" s="39"/>
-      <c r="P87" s="8" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="88" spans="7:21" x14ac:dyDescent="0.2">
-      <c r="I88" s="48">
+      <c r="P87" s="39"/>
+      <c r="Q87" s="8" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="88" spans="8:22" x14ac:dyDescent="0.2">
+      <c r="J88" s="48">
         <v>32</v>
       </c>
-      <c r="J88" s="39">
+      <c r="K88" s="39">
         <v>32</v>
       </c>
-      <c r="K88" s="39"/>
       <c r="L88" s="39"/>
       <c r="M88" s="39"/>
       <c r="N88" s="39"/>
-      <c r="O88" s="39"/>
-      <c r="P88" s="8" t="s">
+      <c r="O88" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="P88" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q88" s="8" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="89" spans="7:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="I89" s="50">
+    <row r="89" spans="8:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="J89" s="50">
         <v>33</v>
       </c>
-      <c r="J89" s="39">
+      <c r="K89" s="39">
         <v>33</v>
       </c>
-      <c r="K89" s="39"/>
       <c r="L89" s="39"/>
       <c r="M89" s="39"/>
       <c r="N89" s="39"/>
       <c r="O89" s="39"/>
-      <c r="P89" s="8" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="90" spans="7:21" x14ac:dyDescent="0.2">
-      <c r="G90" s="45" t="s">
+      <c r="P89" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q89" s="8" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="90" spans="8:22" x14ac:dyDescent="0.2">
+      <c r="H90" s="45" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="91" spans="7:21" x14ac:dyDescent="0.2">
-      <c r="L91" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="92" spans="7:21" x14ac:dyDescent="0.2">
-      <c r="L92" s="14" t="s">
-        <v>187</v>
-      </c>
-      <c r="O92" s="14">
-        <v>1</v>
-      </c>
-      <c r="P92" s="8" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="93" spans="7:21" x14ac:dyDescent="0.2">
-      <c r="O93" s="14">
-        <v>2</v>
-      </c>
-      <c r="P93" s="8" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="95" spans="7:21" x14ac:dyDescent="0.2">
-      <c r="L95" t="s">
-        <v>181</v>
-      </c>
-      <c r="O95" s="14">
-        <v>3</v>
-      </c>
-      <c r="P95" s="8" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="96" spans="7:21" x14ac:dyDescent="0.2">
-      <c r="O96" s="14">
-        <v>4</v>
-      </c>
-      <c r="P96" s="8" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="97" spans="15:16" x14ac:dyDescent="0.2">
-      <c r="O97" s="14">
-        <v>5</v>
-      </c>
-      <c r="P97" s="8" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="98" spans="15:16" x14ac:dyDescent="0.2">
-      <c r="O98" s="14">
-        <v>6</v>
-      </c>
-      <c r="P98" s="8" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="99" spans="15:16" x14ac:dyDescent="0.2">
-      <c r="O99" s="14">
-        <v>7</v>
-      </c>
-      <c r="P99" s="8" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="100" spans="15:16" x14ac:dyDescent="0.2">
-      <c r="O100" s="14">
-        <v>8</v>
-      </c>
-      <c r="P100" s="8" t="s">
-        <v>122</v>
-      </c>
+    <row r="91" spans="8:22" x14ac:dyDescent="0.2">
+      <c r="M91"/>
+    </row>
+    <row r="95" spans="8:22" x14ac:dyDescent="0.2">
+      <c r="M95"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="V31:AB31"/>
+    <mergeCell ref="W31:AC31"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
Update Pin Usage, drop hall switches, add IR TX pin, clean-up power names
</commit_message>
<xml_diff>
--- a/Electronic Design/Core 64 Pin Usage Mapping.xlsx
+++ b/Electronic Design/Core 64 Pin Usage Mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ageppert/Dropbox/Electronics/Core 64 Interactive Badge/Core-64-Interactive-Core-Memory-Badge/Electronic Design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B80928FB-A1E0-EE43-B7DC-8F5075C30DF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE583DC6-064D-F942-9471-BD708E65E7BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="32620" windowHeight="22680" activeTab="1" xr2:uid="{A4752792-CA31-B046-B883-84F8D68A57EC}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="46660" windowHeight="26460" activeTab="1" xr2:uid="{A4752792-CA31-B046-B883-84F8D68A57EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Reference Pinouts" sheetId="3" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="203">
   <si>
     <t>Custom</t>
   </si>
@@ -351,12 +351,6 @@
     <t>TEENSY_GND</t>
   </si>
   <si>
-    <t>TEENSY_VUSB to Core 64 Power Switch</t>
-  </si>
-  <si>
-    <t>TEENSY_3V3 from Teensy 3.3V aka 3V3_100mA</t>
-  </si>
-  <si>
     <t>TEENSY_VIN from +VSW</t>
   </si>
   <si>
@@ -516,15 +510,6 @@
     <t>HALL 1</t>
   </si>
   <si>
-    <t>HALL 2</t>
-  </si>
-  <si>
-    <t>HALL 4</t>
-  </si>
-  <si>
-    <t>HALL 3</t>
-  </si>
-  <si>
     <t>SPARE ANALOG (or pseudo digital input)</t>
   </si>
   <si>
@@ -600,15 +585,6 @@
     <t>TFT Reset (cannot be shared pin)</t>
   </si>
   <si>
-    <t>SPI SDI (MOSI)</t>
-  </si>
-  <si>
-    <t>SPI SDO (MISO)</t>
-  </si>
-  <si>
-    <t>SPI SCK</t>
-  </si>
-  <si>
     <t>TFT BACKLIGHT LED BRIGHTNESS</t>
   </si>
   <si>
@@ -640,13 +616,40 @@
   </si>
   <si>
     <t>Teensy View Reset (cannot be shared pin) (default)</t>
+  </si>
+  <si>
+    <t>IR MODULATOR</t>
+  </si>
+  <si>
+    <t>SPI SCK (default)</t>
+  </si>
+  <si>
+    <t>SPI SDI (MOSI) default</t>
+  </si>
+  <si>
+    <t>SPI SDO (MISO) default</t>
+  </si>
+  <si>
+    <t>TEENSY_3V3_AREF</t>
+  </si>
+  <si>
+    <t>TEENSY_AREF Connect back to TEENSY_3V3_AREF</t>
+  </si>
+  <si>
+    <t>TEENSY_VIN connect to 5V0</t>
+  </si>
+  <si>
+    <t>TEENSY_VUSB supply to Core64 Power Switch SPDT</t>
+  </si>
+  <si>
+    <t>Unused</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -729,6 +732,20 @@
     </font>
     <font>
       <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -926,7 +943,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1067,6 +1084,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1155,16 +1176,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>1302658</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>8165</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>32659</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>322952</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>28</xdr:col>
-      <xdr:colOff>3627</xdr:colOff>
-      <xdr:row>76</xdr:row>
-      <xdr:rowOff>68037</xdr:rowOff>
+      <xdr:colOff>57902</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>57183</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1194,8 +1215,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm rot="5400000">
-          <a:off x="21368657" y="4694466"/>
-          <a:ext cx="4962072" cy="5800270"/>
+          <a:off x="25230814" y="10912746"/>
+          <a:ext cx="5031325" cy="5799944"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1217,15 +1238,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>28</xdr:col>
-      <xdr:colOff>183243</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>143328</xdr:rowOff>
+      <xdr:colOff>259226</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>317002</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>35</xdr:col>
-      <xdr:colOff>226223</xdr:colOff>
-      <xdr:row>76</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:colOff>302206</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>181273</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1255,8 +1276,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="26929443" y="5248728"/>
-          <a:ext cx="5821480" cy="4885872"/>
+          <a:off x="30847773" y="11291105"/>
+          <a:ext cx="5817681" cy="4955125"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1278,15 +1299,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>35</xdr:col>
-      <xdr:colOff>290285</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:colOff>626780</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>233918</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>43</xdr:col>
-      <xdr:colOff>112486</xdr:colOff>
-      <xdr:row>82</xdr:row>
-      <xdr:rowOff>21867</xdr:rowOff>
+      <xdr:colOff>448981</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>152123</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1316,8 +1337,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="32814985" y="5092700"/>
-          <a:ext cx="6426201" cy="6155967"/>
+          <a:off x="36990028" y="11208021"/>
+          <a:ext cx="6421859" cy="6246495"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1467,7 +1488,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>34</xdr:col>
-      <xdr:colOff>776280</xdr:colOff>
+      <xdr:colOff>776279</xdr:colOff>
       <xdr:row>44</xdr:row>
       <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
@@ -1565,16 +1586,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>36</xdr:col>
-      <xdr:colOff>734785</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>235469</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>157718</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>37</xdr:col>
-      <xdr:colOff>199571</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>97972</xdr:rowOff>
+      <xdr:colOff>525212</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>11134</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1589,8 +1610,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="34084985" y="5016500"/>
-          <a:ext cx="290286" cy="390072"/>
+          <a:off x="38248631" y="11131821"/>
+          <a:ext cx="289743" cy="396151"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1791,7 +1812,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
-      <xdr:colOff>814103</xdr:colOff>
+      <xdr:colOff>814102</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>156127</xdr:rowOff>
     </xdr:to>
@@ -1852,7 +1873,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>34</xdr:col>
-      <xdr:colOff>413078</xdr:colOff>
+      <xdr:colOff>413077</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>54274</xdr:rowOff>
     </xdr:to>
@@ -1896,7 +1917,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>42</xdr:col>
-      <xdr:colOff>670880</xdr:colOff>
+      <xdr:colOff>670879</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>151598</xdr:rowOff>
     </xdr:to>
@@ -2340,14 +2361,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CBC2977-27CE-C64F-BE79-A69FB2535F84}">
   <dimension ref="A1:AD95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C43" zoomScale="117" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="Q68" sqref="Q68"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="117" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E83" sqref="E83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="29.5" customWidth="1"/>
-    <col min="3" max="3" width="28.83203125" style="14" customWidth="1"/>
+    <col min="3" max="3" width="21.5" style="14" customWidth="1"/>
     <col min="4" max="4" width="5.6640625" style="14" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.6640625" style="14" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.83203125" style="14" bestFit="1" customWidth="1"/>
@@ -2964,7 +2985,7 @@
     </row>
     <row r="22" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G22" s="14" t="s">
         <v>51</v>
@@ -3011,7 +3032,7 @@
     </row>
     <row r="28" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="29" spans="1:30" x14ac:dyDescent="0.2">
@@ -3075,13 +3096,13 @@
         <v>103</v>
       </c>
       <c r="S30" t="s">
+        <v>108</v>
+      </c>
+      <c r="T30" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="U30" t="s">
         <v>110</v>
-      </c>
-      <c r="T30" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="U30" t="s">
-        <v>112</v>
       </c>
       <c r="W30" s="26"/>
       <c r="X30" s="26"/>
@@ -3116,7 +3137,7 @@
       <c r="O31" s="25"/>
       <c r="P31" s="25"/>
       <c r="Q31" s="36" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="W31" s="57"/>
       <c r="X31" s="57"/>
@@ -3129,7 +3150,7 @@
     </row>
     <row r="32" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A32" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B32" s="8"/>
       <c r="C32" s="39" t="s">
@@ -3172,7 +3193,7 @@
     </row>
     <row r="33" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A33" s="8" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B33" s="8"/>
       <c r="C33" s="39" t="s">
@@ -3202,7 +3223,7 @@
       <c r="O33" s="25"/>
       <c r="P33" s="25"/>
       <c r="Q33" s="24" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="W33" s="26"/>
       <c r="X33" s="26"/>
@@ -3215,7 +3236,7 @@
     </row>
     <row r="34" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A34" s="8" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B34" s="8"/>
       <c r="C34" s="39"/>
@@ -3248,7 +3269,7 @@
         <v>26</v>
       </c>
       <c r="Q34" s="19" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="W34" s="26"/>
       <c r="X34" s="26"/>
@@ -3261,7 +3282,7 @@
     </row>
     <row r="35" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A35" s="8" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="39" t="s">
@@ -3309,7 +3330,7 @@
     </row>
     <row r="36" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A36" s="8" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B36" s="8"/>
       <c r="C36" s="39" t="s">
@@ -3343,7 +3364,7 @@
       <c r="O36" s="39"/>
       <c r="P36" s="39"/>
       <c r="Q36" s="8" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="W36" s="26"/>
       <c r="X36" s="26"/>
@@ -3356,7 +3377,7 @@
     </row>
     <row r="37" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A37" s="8" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B37" s="8"/>
       <c r="C37" s="39"/>
@@ -3429,16 +3450,16 @@
         <v>26</v>
       </c>
       <c r="Q38" s="8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="R38" s="8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="S38" s="8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="T38" s="8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="U38" s="8"/>
       <c r="W38" s="26"/>
@@ -3481,16 +3502,16 @@
         <v>26</v>
       </c>
       <c r="Q39" s="8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="R39" s="8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="S39" s="8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="T39" s="8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="U39" s="8"/>
       <c r="W39" s="26"/>
@@ -3504,7 +3525,7 @@
     </row>
     <row r="40" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A40" s="8" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="39"/>
@@ -3538,10 +3559,10 @@
         <v>26</v>
       </c>
       <c r="Q40" s="8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="R40" s="39" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="W40" s="26"/>
       <c r="X40" s="26"/>
@@ -3554,7 +3575,7 @@
     </row>
     <row r="41" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A41" s="8" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B41" s="8"/>
       <c r="C41" s="39"/>
@@ -3589,7 +3610,7 @@
       </c>
       <c r="Q41" s="8"/>
       <c r="R41" s="39" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="W41" s="26"/>
       <c r="X41" s="26"/>
@@ -3602,7 +3623,7 @@
     </row>
     <row r="42" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A42" s="8" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="39"/>
@@ -3638,7 +3659,7 @@
         <v>26</v>
       </c>
       <c r="Q42" s="8" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="W42" s="26"/>
       <c r="X42" s="26"/>
@@ -3651,7 +3672,7 @@
     </row>
     <row r="43" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A43" s="8" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B43" s="8"/>
       <c r="C43" s="39"/>
@@ -3681,7 +3702,7 @@
       <c r="O43" s="39"/>
       <c r="P43" s="39"/>
       <c r="Q43" s="8" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="W43" s="26"/>
       <c r="X43" s="26"/>
@@ -3694,7 +3715,7 @@
     </row>
     <row r="44" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A44" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B44" s="8"/>
       <c r="C44" s="39"/>
@@ -3719,15 +3740,15 @@
       <c r="L44" s="39"/>
       <c r="M44" s="39"/>
       <c r="N44" s="39" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="O44" s="39"/>
       <c r="P44" s="39"/>
       <c r="Q44" s="8" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="R44" s="8" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="W44" s="26"/>
       <c r="X44" s="26"/>
@@ -3764,7 +3785,7 @@
     </row>
     <row r="46" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A46" s="15" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B46" s="15"/>
       <c r="G46" s="14">
@@ -3785,7 +3806,7 @@
       <c r="O46" s="39"/>
       <c r="P46" s="39"/>
       <c r="Q46" s="8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="W46" s="26"/>
       <c r="X46" s="26"/>
@@ -3798,7 +3819,7 @@
     </row>
     <row r="47" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A47" s="15" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B47" s="15"/>
       <c r="G47" s="14" t="s">
@@ -3808,7 +3829,7 @@
         <v>6</v>
       </c>
       <c r="I47" s="43" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="J47" s="42">
         <v>24</v>
@@ -3835,7 +3856,7 @@
     </row>
     <row r="48" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A48" s="15" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B48" s="15"/>
       <c r="G48" s="14" t="s">
@@ -3845,7 +3866,7 @@
         <v>4</v>
       </c>
       <c r="I48" s="43" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="J48" s="42">
         <v>25</v>
@@ -3880,7 +3901,7 @@
         <v>7</v>
       </c>
       <c r="I49" s="43" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="J49" s="40" t="s">
         <v>66</v>
@@ -3892,7 +3913,7 @@
       <c r="O49" s="25"/>
       <c r="P49" s="25"/>
       <c r="Q49" s="24" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="W49" s="26"/>
       <c r="X49" s="26"/>
@@ -3930,7 +3951,7 @@
     <row r="51" spans="1:30" x14ac:dyDescent="0.2">
       <c r="G51" s="7"/>
       <c r="H51" s="45" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="W51" s="26"/>
       <c r="X51" s="26"/>
@@ -3954,7 +3975,7 @@
     </row>
     <row r="53" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="W53" s="26"/>
       <c r="X53" s="26"/>
@@ -3965,16 +3986,16 @@
       <c r="AC53" s="9"/>
       <c r="AD53" s="9"/>
     </row>
-    <row r="54" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:30" ht="26" x14ac:dyDescent="0.3">
       <c r="A54" s="22" t="s">
         <v>96</v>
       </c>
       <c r="B54" s="22"/>
-      <c r="H54" s="8"/>
-      <c r="I54" s="23" t="s">
+      <c r="H54" s="58"/>
+      <c r="I54" s="59" t="s">
         <v>60</v>
       </c>
-      <c r="J54" s="8"/>
+      <c r="J54" s="58"/>
     </row>
     <row r="55" spans="1:30" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
@@ -3984,7 +4005,7 @@
         <v>103</v>
       </c>
       <c r="C55" s="14" t="s">
-        <v>1</v>
+        <v>108</v>
       </c>
       <c r="D55" s="14" t="s">
         <v>2</v>
@@ -4029,13 +4050,13 @@
         <v>103</v>
       </c>
       <c r="S55" t="s">
+        <v>108</v>
+      </c>
+      <c r="T55" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="U55" t="s">
         <v>110</v>
-      </c>
-      <c r="T55" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="U55" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="56" spans="1:30" x14ac:dyDescent="0.2">
@@ -4052,7 +4073,7 @@
         <v>4</v>
       </c>
       <c r="J56" s="34" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="K56" s="35"/>
       <c r="L56" s="25"/>
@@ -4061,12 +4082,12 @@
       <c r="O56" s="25"/>
       <c r="P56" s="25"/>
       <c r="Q56" s="36" t="s">
-        <v>107</v>
+        <v>200</v>
       </c>
     </row>
     <row r="57" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A57" s="8" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="B57" s="8"/>
       <c r="C57" s="14" t="s">
@@ -4083,7 +4104,7 @@
       </c>
       <c r="I57" s="7"/>
       <c r="J57" s="31" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="K57" s="33"/>
       <c r="L57" s="32"/>
@@ -4097,7 +4118,7 @@
     </row>
     <row r="58" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A58" s="8" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="14" t="s">
@@ -4114,7 +4135,7 @@
       </c>
       <c r="I58" s="7"/>
       <c r="J58" s="40" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="K58" s="35"/>
       <c r="L58" s="25"/>
@@ -4123,15 +4144,15 @@
       <c r="O58" s="25"/>
       <c r="P58" s="25"/>
       <c r="Q58" s="24" t="s">
-        <v>106</v>
+        <v>198</v>
       </c>
     </row>
     <row r="59" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A59" s="8" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="B59" s="56" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="G59" s="14">
         <v>2</v>
@@ -4166,13 +4187,13 @@
         <v>70</v>
       </c>
       <c r="B60" s="56" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="D60" s="14" t="s">
         <v>2</v>
       </c>
       <c r="F60" s="14" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G60" s="14">
         <v>3</v>
@@ -4204,13 +4225,13 @@
     </row>
     <row r="61" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A61" s="8" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="D61" s="14" t="s">
         <v>2</v>
       </c>
       <c r="F61" s="14" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G61" s="14">
         <v>4</v>
@@ -4230,17 +4251,17 @@
       </c>
       <c r="M61" s="39"/>
       <c r="N61" s="39" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="O61" s="39" t="s">
         <v>2</v>
       </c>
       <c r="P61" s="39"/>
       <c r="Q61" s="8" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="R61" s="39" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
     </row>
     <row r="62" spans="1:30" x14ac:dyDescent="0.2">
@@ -4248,7 +4269,10 @@
         <v>72</v>
       </c>
       <c r="B62" s="56" t="s">
-        <v>199</v>
+        <v>191</v>
+      </c>
+      <c r="C62" s="14" t="s">
+        <v>194</v>
       </c>
       <c r="D62" s="14" t="s">
         <v>2</v>
@@ -4271,7 +4295,7 @@
       </c>
       <c r="M62" s="39"/>
       <c r="N62" s="39" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="O62" s="39" t="s">
         <v>2</v>
@@ -4281,15 +4305,15 @@
         <v>78</v>
       </c>
       <c r="R62" s="39" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
     </row>
     <row r="63" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A63" s="8" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="B63" s="53" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="D63" s="14" t="s">
         <v>2</v>
@@ -4319,16 +4343,16 @@
         <v>26</v>
       </c>
       <c r="Q63" s="8" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="R63" s="8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="S63" s="8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="T63" s="8" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="U63" s="8"/>
     </row>
@@ -4365,25 +4389,25 @@
         <v>26</v>
       </c>
       <c r="Q64" s="8" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="R64" s="8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="S64" s="8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="T64" s="8" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="U64" s="8"/>
     </row>
-    <row r="65" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A65" s="8" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="B65" s="55" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="F65" s="14" t="s">
         <v>16</v>
@@ -4415,20 +4439,20 @@
         <v>26</v>
       </c>
       <c r="Q65" s="8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="R65" s="52" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="S65" s="51"/>
       <c r="T65" s="51"/>
     </row>
-    <row r="66" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A66" s="8" t="s">
         <v>76</v>
       </c>
       <c r="B66" s="55" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="D66" s="14" t="s">
         <v>2</v>
@@ -4462,19 +4486,17 @@
       <c r="P66" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="Q66" s="8" t="s">
-        <v>160</v>
-      </c>
+      <c r="Q66" s="8"/>
       <c r="R66" s="55" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="67" spans="1:22" x14ac:dyDescent="0.2">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="67" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A67" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B67" s="56" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="D67" s="14" t="s">
         <v>2</v>
@@ -4508,15 +4530,15 @@
         <v>26</v>
       </c>
       <c r="Q67" s="56" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="68" spans="1:22" x14ac:dyDescent="0.2">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="68" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A68" s="51" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="E68" s="14" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G68" s="14">
         <v>11</v>
@@ -4539,16 +4561,16 @@
       <c r="O68" s="39"/>
       <c r="P68" s="39"/>
       <c r="Q68" s="54" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="69" spans="1:22" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="69" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A69" s="51" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="B69" s="14"/>
       <c r="E69" s="14" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G69" s="14">
         <v>12</v>
@@ -4566,19 +4588,19 @@
       <c r="L69" s="39"/>
       <c r="M69" s="39"/>
       <c r="N69" s="39" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="O69" s="39"/>
       <c r="P69" s="39"/>
       <c r="Q69" s="51" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="R69" s="8" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="S69" s="9"/>
     </row>
-    <row r="70" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>51</v>
       </c>
@@ -4594,16 +4616,16 @@
         <v>51</v>
       </c>
     </row>
-    <row r="71" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A71" s="15" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B71" s="15"/>
       <c r="G71" s="14" t="s">
         <v>51</v>
       </c>
       <c r="H71" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="J71" s="37" t="s">
         <v>10</v>
@@ -4617,12 +4639,12 @@
       <c r="O71" s="39"/>
       <c r="P71" s="39"/>
       <c r="Q71" s="8" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="72" spans="1:22" x14ac:dyDescent="0.2">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="72" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A72" s="15" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B72" s="15"/>
       <c r="G72" s="14" t="s">
@@ -4632,7 +4654,7 @@
         <v>6</v>
       </c>
       <c r="I72" s="43" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="J72" s="37" t="s">
         <v>42</v>
@@ -4646,12 +4668,12 @@
       <c r="O72" s="39"/>
       <c r="P72" s="39"/>
       <c r="Q72" s="8" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="73" spans="1:22" x14ac:dyDescent="0.2">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="73" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A73" s="15" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B73" s="15"/>
       <c r="G73" s="14" t="s">
@@ -4661,7 +4683,7 @@
         <v>4</v>
       </c>
       <c r="I73" s="43" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="J73" s="37" t="s">
         <v>43</v>
@@ -4675,11 +4697,13 @@
       <c r="O73" s="39"/>
       <c r="P73" s="39"/>
       <c r="Q73" s="8" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="74" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A74" s="15"/>
+        <v>158</v>
+      </c>
+    </row>
+    <row r="74" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A74" s="15" t="s">
+        <v>202</v>
+      </c>
       <c r="B74" s="15"/>
       <c r="G74" s="14" t="s">
         <v>51</v>
@@ -4688,7 +4712,7 @@
         <v>7</v>
       </c>
       <c r="I74" s="43" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="J74" s="40" t="s">
         <v>66</v>
@@ -4700,19 +4724,19 @@
       <c r="O74" s="25"/>
       <c r="P74" s="25"/>
       <c r="Q74" s="24" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="75" spans="1:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="75" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A75" s="8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B75" s="8"/>
       <c r="G75" s="14" t="s">
         <v>51</v>
       </c>
       <c r="H75" s="5" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="I75" s="13"/>
       <c r="J75" s="6"/>
@@ -4721,42 +4745,35 @@
         <v>51</v>
       </c>
     </row>
-    <row r="76" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:20" x14ac:dyDescent="0.2">
       <c r="J76" s="47" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="K76" s="39"/>
       <c r="L76" s="39" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="M76" s="39"/>
       <c r="N76" s="39"/>
       <c r="O76" s="39"/>
       <c r="P76" s="39"/>
-      <c r="Q76" s="8" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="77" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="Q76" s="8"/>
+    </row>
+    <row r="77" spans="1:20" x14ac:dyDescent="0.2">
       <c r="J77" s="48" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="K77" s="39"/>
       <c r="L77" s="39" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="M77" s="39"/>
       <c r="N77" s="39"/>
       <c r="O77" s="39"/>
       <c r="P77" s="39"/>
-      <c r="Q77" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="V77" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="78" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="Q77" s="8"/>
+    </row>
+    <row r="78" spans="1:20" x14ac:dyDescent="0.2">
       <c r="J78" s="49" t="s">
         <v>4</v>
       </c>
@@ -4769,20 +4786,14 @@
       <c r="Q78" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="V78" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="79" spans="1:22" x14ac:dyDescent="0.2">
+    </row>
+    <row r="79" spans="1:20" x14ac:dyDescent="0.2">
       <c r="J79" s="41" t="s">
         <v>6</v>
       </c>
       <c r="Q79" s="15"/>
-      <c r="V79" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="80" spans="1:22" x14ac:dyDescent="0.2">
+    </row>
+    <row r="80" spans="1:20" x14ac:dyDescent="0.2">
       <c r="J80" s="48">
         <v>24</v>
       </c>
@@ -4797,11 +4808,8 @@
       <c r="Q80" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="V80" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="81" spans="8:22" x14ac:dyDescent="0.2">
+    </row>
+    <row r="81" spans="8:17" x14ac:dyDescent="0.2">
       <c r="J81" s="48">
         <v>25</v>
       </c>
@@ -4818,13 +4826,10 @@
         <v>26</v>
       </c>
       <c r="Q81" s="8" t="s">
-        <v>182</v>
-      </c>
-      <c r="V81" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="82" spans="8:22" x14ac:dyDescent="0.2">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="82" spans="8:17" x14ac:dyDescent="0.2">
       <c r="J82" s="48">
         <v>26</v>
       </c>
@@ -4832,7 +4837,7 @@
         <v>26</v>
       </c>
       <c r="L82" s="39" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="M82" s="39"/>
       <c r="N82" s="39"/>
@@ -4842,7 +4847,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="83" spans="8:22" x14ac:dyDescent="0.2">
+    <row r="83" spans="8:17" x14ac:dyDescent="0.2">
       <c r="J83" s="48">
         <v>27</v>
       </c>
@@ -4850,17 +4855,17 @@
         <v>27</v>
       </c>
       <c r="L83" s="39" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="M83" s="39"/>
       <c r="N83" s="39"/>
       <c r="O83" s="39"/>
       <c r="P83" s="39"/>
       <c r="Q83" s="8" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="84" spans="8:22" x14ac:dyDescent="0.2">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="84" spans="8:17" x14ac:dyDescent="0.2">
       <c r="J84" s="48">
         <v>28</v>
       </c>
@@ -4868,7 +4873,7 @@
         <v>28</v>
       </c>
       <c r="L84" s="39" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="M84" s="39"/>
       <c r="N84" s="39"/>
@@ -4878,7 +4883,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="85" spans="8:22" x14ac:dyDescent="0.2">
+    <row r="85" spans="8:17" x14ac:dyDescent="0.2">
       <c r="J85" s="48">
         <v>29</v>
       </c>
@@ -4886,17 +4891,17 @@
         <v>29</v>
       </c>
       <c r="L85" s="39" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="M85" s="39"/>
       <c r="N85" s="39"/>
       <c r="O85" s="39"/>
       <c r="P85" s="39"/>
       <c r="Q85" s="8" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="86" spans="8:22" x14ac:dyDescent="0.2">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="86" spans="8:17" x14ac:dyDescent="0.2">
       <c r="J86" s="48">
         <v>30</v>
       </c>
@@ -4904,7 +4909,7 @@
         <v>30</v>
       </c>
       <c r="L86" s="39" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="M86" s="39"/>
       <c r="N86" s="39"/>
@@ -4914,7 +4919,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="87" spans="8:22" x14ac:dyDescent="0.2">
+    <row r="87" spans="8:17" x14ac:dyDescent="0.2">
       <c r="J87" s="48">
         <v>31</v>
       </c>
@@ -4922,17 +4927,17 @@
         <v>31</v>
       </c>
       <c r="L87" s="39" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="M87" s="39"/>
       <c r="N87" s="39"/>
       <c r="O87" s="39"/>
       <c r="P87" s="39"/>
       <c r="Q87" s="8" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="88" spans="8:22" x14ac:dyDescent="0.2">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="88" spans="8:17" x14ac:dyDescent="0.2">
       <c r="J88" s="48">
         <v>32</v>
       </c>
@@ -4952,7 +4957,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="89" spans="8:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="8:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="J89" s="50">
         <v>33</v>
       </c>
@@ -4967,18 +4972,39 @@
         <v>26</v>
       </c>
       <c r="Q89" s="8" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="90" spans="8:22" x14ac:dyDescent="0.2">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="90" spans="8:17" x14ac:dyDescent="0.2">
       <c r="H90" s="45" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="91" spans="8:22" x14ac:dyDescent="0.2">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="91" spans="8:17" x14ac:dyDescent="0.2">
+      <c r="H91" t="s">
+        <v>91</v>
+      </c>
       <c r="M91"/>
     </row>
-    <row r="95" spans="8:22" x14ac:dyDescent="0.2">
+    <row r="92" spans="8:17" x14ac:dyDescent="0.2">
+      <c r="H92" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="93" spans="8:17" x14ac:dyDescent="0.2">
+      <c r="H93" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="94" spans="8:17" x14ac:dyDescent="0.2">
+      <c r="H94" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="95" spans="8:17" x14ac:dyDescent="0.2">
+      <c r="H95" t="s">
+        <v>95</v>
+      </c>
       <c r="M95"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update pin usage map for SPI devices
</commit_message>
<xml_diff>
--- a/Electronic Design/Core 64 Pin Usage Mapping.xlsx
+++ b/Electronic Design/Core 64 Pin Usage Mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ageppert/Dropbox/Electronics/Core 64 Interactive Badge/Core-64-Interactive-Core-Memory-Badge/Electronic Design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE583DC6-064D-F942-9471-BD708E65E7BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6723F40D-08F4-FC48-97FE-5BBA8887CF97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="46660" windowHeight="26460" activeTab="1" xr2:uid="{A4752792-CA31-B046-B883-84F8D68A57EC}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="210">
   <si>
     <t>Custom</t>
   </si>
@@ -643,6 +643,27 @@
   </si>
   <si>
     <t>Unused</t>
+  </si>
+  <si>
+    <t>TOUCH_CS</t>
+  </si>
+  <si>
+    <t>TFT 3.2"</t>
+  </si>
+  <si>
+    <t>SPI DEVICE READINESS:</t>
+  </si>
+  <si>
+    <t>OLED TeensyView</t>
+  </si>
+  <si>
+    <t>SD Card</t>
+  </si>
+  <si>
+    <t>Touch Screen Controller</t>
+  </si>
+  <si>
+    <t>OLED Generic</t>
   </si>
 </sst>
 </file>
@@ -751,7 +772,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -809,6 +830,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -943,7 +970,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1081,13 +1108,27 @@
     <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2361,8 +2402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CBC2977-27CE-C64F-BE79-A69FB2535F84}">
   <dimension ref="A1:AD95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="117" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E83" sqref="E83"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="117" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A78" sqref="A78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3139,13 +3180,13 @@
       <c r="Q31" s="36" t="s">
         <v>105</v>
       </c>
-      <c r="W31" s="57"/>
-      <c r="X31" s="57"/>
-      <c r="Y31" s="57"/>
-      <c r="Z31" s="57"/>
-      <c r="AA31" s="57"/>
-      <c r="AB31" s="57"/>
-      <c r="AC31" s="57"/>
+      <c r="W31" s="59"/>
+      <c r="X31" s="59"/>
+      <c r="Y31" s="59"/>
+      <c r="Z31" s="59"/>
+      <c r="AA31" s="59"/>
+      <c r="AB31" s="59"/>
+      <c r="AC31" s="59"/>
       <c r="AD31" s="9"/>
     </row>
     <row r="32" spans="1:30" x14ac:dyDescent="0.2">
@@ -3991,11 +4032,11 @@
         <v>96</v>
       </c>
       <c r="B54" s="22"/>
-      <c r="H54" s="58"/>
-      <c r="I54" s="59" t="s">
+      <c r="H54" s="57"/>
+      <c r="I54" s="58" t="s">
         <v>60</v>
       </c>
-      <c r="J54" s="58"/>
+      <c r="J54" s="57"/>
     </row>
     <row r="55" spans="1:30" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
@@ -4227,6 +4268,9 @@
       <c r="A61" s="8" t="s">
         <v>173</v>
       </c>
+      <c r="B61" s="60" t="s">
+        <v>203</v>
+      </c>
       <c r="D61" s="14" t="s">
         <v>2</v>
       </c>
@@ -4757,7 +4801,9 @@
       <c r="N76" s="39"/>
       <c r="O76" s="39"/>
       <c r="P76" s="39"/>
-      <c r="Q76" s="8"/>
+      <c r="Q76" s="8" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="77" spans="1:20" x14ac:dyDescent="0.2">
       <c r="J77" s="48" t="s">
@@ -4771,9 +4817,14 @@
       <c r="N77" s="39"/>
       <c r="O77" s="39"/>
       <c r="P77" s="39"/>
-      <c r="Q77" s="8"/>
+      <c r="Q77" s="8" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="78" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A78" s="65" t="s">
+        <v>205</v>
+      </c>
       <c r="J78" s="49" t="s">
         <v>4</v>
       </c>
@@ -4788,12 +4839,18 @@
       </c>
     </row>
     <row r="79" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A79" s="64" t="s">
+        <v>204</v>
+      </c>
       <c r="J79" s="41" t="s">
         <v>6</v>
       </c>
       <c r="Q79" s="15"/>
     </row>
     <row r="80" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A80" s="61" t="s">
+        <v>206</v>
+      </c>
       <c r="J80" s="48">
         <v>24</v>
       </c>
@@ -4809,7 +4866,10 @@
         <v>88</v>
       </c>
     </row>
-    <row r="81" spans="8:17" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A81" s="61" t="s">
+        <v>209</v>
+      </c>
       <c r="J81" s="48">
         <v>25</v>
       </c>
@@ -4829,7 +4889,10 @@
         <v>177</v>
       </c>
     </row>
-    <row r="82" spans="8:17" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A82" s="63" t="s">
+        <v>207</v>
+      </c>
       <c r="J82" s="48">
         <v>26</v>
       </c>
@@ -4847,7 +4910,10 @@
         <v>87</v>
       </c>
     </row>
-    <row r="83" spans="8:17" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A83" s="62" t="s">
+        <v>208</v>
+      </c>
       <c r="J83" s="48">
         <v>27</v>
       </c>
@@ -4865,7 +4931,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="84" spans="8:17" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.2">
       <c r="J84" s="48">
         <v>28</v>
       </c>
@@ -4883,7 +4949,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="85" spans="8:17" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:17" x14ac:dyDescent="0.2">
       <c r="J85" s="48">
         <v>29</v>
       </c>
@@ -4901,7 +4967,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="86" spans="8:17" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.2">
       <c r="J86" s="48">
         <v>30</v>
       </c>
@@ -4919,7 +4985,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="87" spans="8:17" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:17" x14ac:dyDescent="0.2">
       <c r="J87" s="48">
         <v>31</v>
       </c>
@@ -4937,7 +5003,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="88" spans="8:17" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:17" x14ac:dyDescent="0.2">
       <c r="J88" s="48">
         <v>32</v>
       </c>
@@ -4957,7 +5023,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="89" spans="8:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="J89" s="50">
         <v>33</v>
       </c>
@@ -4975,33 +5041,33 @@
         <v>181</v>
       </c>
     </row>
-    <row r="90" spans="8:17" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:17" x14ac:dyDescent="0.2">
       <c r="H90" s="45" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="91" spans="8:17" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:17" x14ac:dyDescent="0.2">
       <c r="H91" t="s">
         <v>91</v>
       </c>
       <c r="M91"/>
     </row>
-    <row r="92" spans="8:17" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:17" x14ac:dyDescent="0.2">
       <c r="H92" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="93" spans="8:17" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:17" x14ac:dyDescent="0.2">
       <c r="H93" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="94" spans="8:17" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:17" x14ac:dyDescent="0.2">
       <c r="H94" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="95" spans="8:17" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:17" x14ac:dyDescent="0.2">
       <c r="H95" t="s">
         <v>95</v>
       </c>

</xml_diff>

<commit_message>
Pin mapping and MCU spec updates planning for V0.4
</commit_message>
<xml_diff>
--- a/Electronic Design/Core 64 Pin Usage Mapping.xlsx
+++ b/Electronic Design/Core 64 Pin Usage Mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ageppert/Dropbox/Electronics/Core 64 Interactive Badge/Core-64-Interactive-Core-Memory-Badge/Electronic Design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6723F40D-08F4-FC48-97FE-5BBA8887CF97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFF74E56-2CFD-B941-88B0-632164F9E92E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="46660" windowHeight="26460" activeTab="1" xr2:uid="{A4752792-CA31-B046-B883-84F8D68A57EC}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27940" windowHeight="26460" activeTab="1" xr2:uid="{A4752792-CA31-B046-B883-84F8D68A57EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Reference Pinouts" sheetId="3" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="211">
   <si>
     <t>Custom</t>
   </si>
@@ -303,27 +303,12 @@
     <t>Matrix Drive 20 Q10N</t>
   </si>
   <si>
-    <t>Teensy-LC delivers an impressive collection of capabilities to make modern electronic projects simpler. It features an ARM Cortex-M0+ processor at 48 MHz, 62K Flash, 8K RAM, 12 bit analog input &amp; output, hardware Serial, SPI &amp; I2C, USB, and a total of 27 I/O pins.</t>
-  </si>
-  <si>
     <t>Upgrade path is Teensy 3.1 or 3.2</t>
   </si>
   <si>
-    <t>Version 3.2 features a 32 bit ARM processor.</t>
-  </si>
-  <si>
     <t>Teensy 3.2 adds a more powerful 3.3 volt regulator, with the ability to directly power ESP8266 Wifi, WIZ820io Ethernet and other power-hungry 3.3V add-on boards.</t>
   </si>
   <si>
-    <t>The RAM has quadrupled since 3.0, from 16K to 64K.</t>
-  </si>
-  <si>
-    <t>Flash memory has also doubled, to 256K</t>
-  </si>
-  <si>
-    <t>All digital pins are 5 volt tolerant on Teensy 3.2 &amp; 3.1. However, the analog-only pins (A10-A14), AREF, Program and Reset are 3.3V only.</t>
-  </si>
-  <si>
     <t>https://www.pjrc.com/teensy/teensy31.html</t>
   </si>
   <si>
@@ -450,9 +435,6 @@
     <t>Interrupt capable: Teensy LC 2 - 12, 14, 15, 20 - 23</t>
   </si>
   <si>
-    <t>Interrupt capable: Teensy 3.2 all digital pins.</t>
-  </si>
-  <si>
     <t>SDCARD CLK</t>
   </si>
   <si>
@@ -507,9 +489,6 @@
     <t>Bring out the DAC for expansion!</t>
   </si>
   <si>
-    <t>HALL 1</t>
-  </si>
-  <si>
     <t>SPARE ANALOG (or pseudo digital input)</t>
   </si>
   <si>
@@ -664,6 +643,30 @@
   </si>
   <si>
     <t>OLED Generic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Teensy-LC delivers an impressive collection of capabilities to make modern electronic projects simpler. </t>
+  </si>
+  <si>
+    <t>It features an ARM Cortex-M0+ processor at 48 MHz, 62K Flash, 8K RAM, 12 bit analog input &amp; output, hardware Serial, SPI &amp; I2C, USB, and a total of 27 I/O pins.</t>
+  </si>
+  <si>
+    <t>MUST CUT USB-VUSB JUMPER</t>
+  </si>
+  <si>
+    <t>Interrupt capable: Teensy 3.2 all digital pins. All digital pins are 5 volt tolerant on Teensy 3.2 &amp; 3.1. However, the analog-only pins (A10-A14), AREF, Program and Reset are 3.3V only.</t>
+  </si>
+  <si>
+    <t>Program Flash memory 256K</t>
+  </si>
+  <si>
+    <t>RAM  64K.</t>
+  </si>
+  <si>
+    <t>SPARE DIGITAL  &amp; PWM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Version 3.2 features a 32 bit ARM processor. Freescale MK20DX256VLH7 Cortex M4 w/DSP @72MHz, 256K Program Flash and FlexMemory, -40 to 105°C, </t>
   </si>
 </sst>
 </file>
@@ -970,7 +973,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1129,6 +1132,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1158,13 +1164,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>66222</xdr:colOff>
-      <xdr:row>54</xdr:row>
+      <xdr:row>58</xdr:row>
       <xdr:rowOff>117928</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>1569357</xdr:colOff>
-      <xdr:row>69</xdr:row>
+      <xdr:row>73</xdr:row>
       <xdr:rowOff>9074</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1219,13 +1225,13 @@
     <xdr:from>
       <xdr:col>21</xdr:col>
       <xdr:colOff>32659</xdr:colOff>
-      <xdr:row>53</xdr:row>
+      <xdr:row>57</xdr:row>
       <xdr:rowOff>322952</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>28</xdr:col>
       <xdr:colOff>57902</xdr:colOff>
-      <xdr:row>78</xdr:row>
+      <xdr:row>82</xdr:row>
       <xdr:rowOff>57183</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1280,14 +1286,14 @@
     <xdr:from>
       <xdr:col>28</xdr:col>
       <xdr:colOff>259226</xdr:colOff>
-      <xdr:row>53</xdr:row>
+      <xdr:row>57</xdr:row>
       <xdr:rowOff>317002</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>35</xdr:col>
       <xdr:colOff>302206</xdr:colOff>
-      <xdr:row>77</xdr:row>
-      <xdr:rowOff>181273</xdr:rowOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>181272</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1341,13 +1347,13 @@
     <xdr:from>
       <xdr:col>35</xdr:col>
       <xdr:colOff>626780</xdr:colOff>
-      <xdr:row>53</xdr:row>
+      <xdr:row>57</xdr:row>
       <xdr:rowOff>233918</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>43</xdr:col>
       <xdr:colOff>448981</xdr:colOff>
-      <xdr:row>83</xdr:row>
+      <xdr:row>87</xdr:row>
       <xdr:rowOff>152123</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1402,13 +1408,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>1203035</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>94188</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>1578429</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>21777</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1463,14 +1469,14 @@
     <xdr:from>
       <xdr:col>20</xdr:col>
       <xdr:colOff>1282700</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
       <xdr:colOff>716410</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>16102</xdr:rowOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>16103</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1524,14 +1530,14 @@
     <xdr:from>
       <xdr:col>28</xdr:col>
       <xdr:colOff>609599</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>34</xdr:col>
       <xdr:colOff>776279</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>50801</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1568,13 +1574,13 @@
     <xdr:from>
       <xdr:col>35</xdr:col>
       <xdr:colOff>292099</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>43</xdr:col>
       <xdr:colOff>90260</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>186350</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1629,13 +1635,13 @@
     <xdr:from>
       <xdr:col>37</xdr:col>
       <xdr:colOff>235469</xdr:colOff>
-      <xdr:row>53</xdr:row>
+      <xdr:row>57</xdr:row>
       <xdr:rowOff>157718</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>37</xdr:col>
       <xdr:colOff>525212</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:row>59</xdr:row>
       <xdr:rowOff>11134</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1684,13 +1690,13 @@
     <xdr:from>
       <xdr:col>36</xdr:col>
       <xdr:colOff>290285</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>36</xdr:col>
       <xdr:colOff>580571</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>186872</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1847,15 +1853,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>32564</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>162820</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>814102</xdr:colOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>21709</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>156127</xdr:rowOff>
+      <xdr:rowOff>112708</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1885,7 +1891,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm rot="5400000">
-          <a:off x="21495654" y="-318133"/>
+          <a:off x="25370782" y="-361552"/>
           <a:ext cx="4715102" cy="5763846"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2375,17 +2381,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="22" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="22" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -2400,10 +2406,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CBC2977-27CE-C64F-BE79-A69FB2535F84}">
-  <dimension ref="A1:AD95"/>
+  <dimension ref="A1:AD99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="117" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A78" sqref="A78"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="117" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="I99" sqref="I99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2432,12 +2438,12 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="22" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B2" s="22"/>
       <c r="I2" s="18" t="s">
@@ -3026,7 +3032,7 @@
     </row>
     <row r="22" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="G22" s="14" t="s">
         <v>51</v>
@@ -3061,180 +3067,147 @@
         <v>51</v>
       </c>
     </row>
+    <row r="24" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="H24" s="45" t="s">
+        <v>132</v>
+      </c>
+    </row>
     <row r="25" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="V25" t="s">
+      <c r="H25" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="26" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="H26" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="27" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="H27" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="V26" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>117</v>
-      </c>
-    </row>
     <row r="29" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A29" s="22" t="s">
+      <c r="A29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="30" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A30" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="B30" s="22"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="J30" s="8"/>
+    </row>
+    <row r="31" spans="1:30" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>0</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D31" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E31" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="F31" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="G31" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="H31" t="s">
+        <v>5</v>
+      </c>
+      <c r="J31" t="s">
+        <v>5</v>
+      </c>
+      <c r="K31" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="L31" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="M31" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="N31" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="O31" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="P31" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q31" t="s">
         <v>97</v>
       </c>
-      <c r="B29" s="22"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="J29" s="8"/>
-    </row>
-    <row r="30" spans="1:30" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>0</v>
-      </c>
-      <c r="C30" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="D30" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="E30" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="F30" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="G30" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="H30" t="s">
-        <v>5</v>
-      </c>
-      <c r="J30" t="s">
-        <v>5</v>
-      </c>
-      <c r="K30" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="L30" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="M30" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="N30" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="O30" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="P30" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q30" t="s">
-        <v>102</v>
-      </c>
-      <c r="R30" s="14" t="s">
+      <c r="R31" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="S31" t="s">
         <v>103</v>
       </c>
-      <c r="S30" t="s">
-        <v>108</v>
-      </c>
-      <c r="T30" s="14" t="s">
-        <v>109</v>
-      </c>
-      <c r="U30" t="s">
-        <v>110</v>
-      </c>
-      <c r="W30" s="26"/>
-      <c r="X30" s="26"/>
-      <c r="Y30" s="9"/>
-      <c r="Z30" s="9"/>
-      <c r="AA30" s="9"/>
-      <c r="AB30" s="9"/>
-      <c r="AC30" s="9"/>
-      <c r="AD30" s="9"/>
-    </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A31" s="29" t="s">
+      <c r="T31" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="B31" s="29"/>
-      <c r="C31" s="32"/>
-      <c r="D31" s="32"/>
-      <c r="E31" s="32"/>
-      <c r="F31" s="32"/>
-      <c r="G31" s="32"/>
-      <c r="H31" s="30" t="s">
+      <c r="U31" t="s">
+        <v>105</v>
+      </c>
+      <c r="W31" s="26"/>
+      <c r="X31" s="26"/>
+      <c r="Y31" s="9"/>
+      <c r="Z31" s="9"/>
+      <c r="AA31" s="9"/>
+      <c r="AB31" s="9"/>
+      <c r="AC31" s="9"/>
+      <c r="AD31" s="9"/>
+    </row>
+    <row r="32" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A32" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="B32" s="29"/>
+      <c r="C32" s="32"/>
+      <c r="D32" s="32"/>
+      <c r="E32" s="32"/>
+      <c r="F32" s="32"/>
+      <c r="G32" s="32"/>
+      <c r="H32" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="I31" s="11"/>
-      <c r="J31" s="34" t="s">
+      <c r="I32" s="11"/>
+      <c r="J32" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="K31" s="35"/>
-      <c r="L31" s="25"/>
-      <c r="M31" s="25"/>
-      <c r="N31" s="25"/>
-      <c r="O31" s="25"/>
-      <c r="P31" s="25"/>
-      <c r="Q31" s="36" t="s">
-        <v>105</v>
-      </c>
-      <c r="W31" s="59"/>
-      <c r="X31" s="59"/>
-      <c r="Y31" s="59"/>
-      <c r="Z31" s="59"/>
-      <c r="AA31" s="59"/>
-      <c r="AB31" s="59"/>
-      <c r="AC31" s="59"/>
-      <c r="AD31" s="9"/>
-    </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A32" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="B32" s="8"/>
-      <c r="C32" s="39" t="s">
-        <v>26</v>
-      </c>
-      <c r="D32" s="39"/>
-      <c r="E32" s="39" t="s">
-        <v>19</v>
-      </c>
-      <c r="F32" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="G32" s="39">
-        <v>0</v>
-      </c>
-      <c r="H32" s="3">
-        <v>0</v>
-      </c>
-      <c r="I32" s="7"/>
-      <c r="J32" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="K32" s="33"/>
-      <c r="L32" s="32"/>
-      <c r="M32" s="32"/>
-      <c r="N32" s="32"/>
-      <c r="O32" s="32"/>
-      <c r="P32" s="32"/>
-      <c r="Q32" s="29" t="s">
-        <v>104</v>
-      </c>
-      <c r="W32" s="26"/>
-      <c r="X32" s="26"/>
-      <c r="Y32" s="9"/>
-      <c r="Z32" s="9"/>
-      <c r="AA32" s="9"/>
-      <c r="AB32" s="9"/>
-      <c r="AC32" s="9"/>
+      <c r="K32" s="35"/>
+      <c r="L32" s="25"/>
+      <c r="M32" s="25"/>
+      <c r="N32" s="25"/>
+      <c r="O32" s="25"/>
+      <c r="P32" s="25"/>
+      <c r="Q32" s="36" t="s">
+        <v>100</v>
+      </c>
+      <c r="W32" s="66"/>
+      <c r="X32" s="66"/>
+      <c r="Y32" s="66"/>
+      <c r="Z32" s="66"/>
+      <c r="AA32" s="66"/>
+      <c r="AB32" s="66"/>
+      <c r="AC32" s="66"/>
       <c r="AD32" s="9"/>
     </row>
     <row r="33" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A33" s="8" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B33" s="8"/>
       <c r="C33" s="39" t="s">
@@ -3242,29 +3215,29 @@
       </c>
       <c r="D33" s="39"/>
       <c r="E33" s="39" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F33" s="39" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G33" s="39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H33" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I33" s="7"/>
-      <c r="J33" s="40" t="s">
-        <v>49</v>
-      </c>
-      <c r="K33" s="35"/>
-      <c r="L33" s="25"/>
-      <c r="M33" s="25"/>
-      <c r="N33" s="25"/>
-      <c r="O33" s="25"/>
-      <c r="P33" s="25"/>
-      <c r="Q33" s="24" t="s">
-        <v>145</v>
+      <c r="J33" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="K33" s="33"/>
+      <c r="L33" s="32"/>
+      <c r="M33" s="32"/>
+      <c r="N33" s="32"/>
+      <c r="O33" s="32"/>
+      <c r="P33" s="32"/>
+      <c r="Q33" s="29" t="s">
+        <v>99</v>
       </c>
       <c r="W33" s="26"/>
       <c r="X33" s="26"/>
@@ -3277,40 +3250,37 @@
     </row>
     <row r="34" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A34" s="8" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="B34" s="8"/>
-      <c r="C34" s="39"/>
+      <c r="C34" s="39" t="s">
+        <v>26</v>
+      </c>
       <c r="D34" s="39"/>
-      <c r="E34" s="39"/>
-      <c r="F34" s="39"/>
+      <c r="E34" s="39" t="s">
+        <v>20</v>
+      </c>
+      <c r="F34" s="39" t="s">
+        <v>13</v>
+      </c>
       <c r="G34" s="39">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H34" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I34" s="7"/>
-      <c r="J34" s="4">
-        <v>23</v>
-      </c>
-      <c r="K34" s="7">
-        <v>23</v>
-      </c>
-      <c r="L34" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="M34" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="O34" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="P34" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q34" s="19" t="s">
-        <v>165</v>
+      <c r="J34" s="40" t="s">
+        <v>49</v>
+      </c>
+      <c r="K34" s="35"/>
+      <c r="L34" s="25"/>
+      <c r="M34" s="25"/>
+      <c r="N34" s="25"/>
+      <c r="O34" s="25"/>
+      <c r="P34" s="25"/>
+      <c r="Q34" s="24" t="s">
+        <v>139</v>
       </c>
       <c r="W34" s="26"/>
       <c r="X34" s="26"/>
@@ -3323,35 +3293,31 @@
     </row>
     <row r="35" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A35" s="8" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="B35" s="8"/>
-      <c r="C35" s="39" t="s">
-        <v>26</v>
-      </c>
-      <c r="D35" s="39" t="s">
-        <v>2</v>
-      </c>
+      <c r="C35" s="39"/>
+      <c r="D35" s="39"/>
       <c r="E35" s="39"/>
       <c r="F35" s="39"/>
       <c r="G35" s="39">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H35" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I35" s="7"/>
       <c r="J35" s="4">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K35" s="7">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L35" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M35" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O35" s="14" t="s">
         <v>2</v>
@@ -3359,7 +3325,9 @@
       <c r="P35" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="Q35" s="19"/>
+      <c r="Q35" s="19" t="s">
+        <v>158</v>
+      </c>
       <c r="W35" s="26"/>
       <c r="X35" s="26"/>
       <c r="Y35" s="9"/>
@@ -3371,7 +3339,7 @@
     </row>
     <row r="36" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A36" s="8" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="B36" s="8"/>
       <c r="C36" s="39" t="s">
@@ -3383,30 +3351,31 @@
       <c r="E36" s="39"/>
       <c r="F36" s="39"/>
       <c r="G36" s="39">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H36" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I36" s="7"/>
-      <c r="J36" s="37">
-        <v>21</v>
-      </c>
-      <c r="K36" s="38">
-        <v>21</v>
-      </c>
-      <c r="L36" s="39" t="s">
-        <v>29</v>
-      </c>
-      <c r="M36" s="39"/>
-      <c r="N36" s="39" t="s">
-        <v>19</v>
-      </c>
-      <c r="O36" s="39"/>
-      <c r="P36" s="39"/>
-      <c r="Q36" s="8" t="s">
-        <v>124</v>
-      </c>
+      <c r="J36" s="4">
+        <v>22</v>
+      </c>
+      <c r="K36" s="7">
+        <v>22</v>
+      </c>
+      <c r="L36" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="M36" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="O36" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="P36" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q36" s="19"/>
       <c r="W36" s="26"/>
       <c r="X36" s="26"/>
       <c r="Y36" s="9"/>
@@ -3418,36 +3387,42 @@
     </row>
     <row r="37" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A37" s="8" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B37" s="8"/>
-      <c r="C37" s="39"/>
-      <c r="D37" s="39"/>
+      <c r="C37" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="D37" s="39" t="s">
+        <v>2</v>
+      </c>
       <c r="E37" s="39"/>
       <c r="F37" s="39"/>
       <c r="G37" s="39">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H37" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I37" s="7"/>
-      <c r="J37" s="4">
-        <v>20</v>
-      </c>
-      <c r="K37" s="7">
-        <v>20</v>
-      </c>
-      <c r="L37" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="N37" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="O37" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q37" s="15"/>
+      <c r="J37" s="37">
+        <v>21</v>
+      </c>
+      <c r="K37" s="38">
+        <v>21</v>
+      </c>
+      <c r="L37" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="M37" s="39"/>
+      <c r="N37" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="O37" s="39"/>
+      <c r="P37" s="39"/>
+      <c r="Q37" s="8" t="s">
+        <v>119</v>
+      </c>
       <c r="W37" s="26"/>
       <c r="X37" s="26"/>
       <c r="Y37" s="9"/>
@@ -3458,51 +3433,37 @@
       <c r="AD37" s="9"/>
     </row>
     <row r="38" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A38" s="15"/>
-      <c r="B38" s="15"/>
-      <c r="D38" s="14" t="s">
+      <c r="A38" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="B38" s="8"/>
+      <c r="C38" s="39"/>
+      <c r="D38" s="39"/>
+      <c r="E38" s="39"/>
+      <c r="F38" s="39"/>
+      <c r="G38" s="39">
+        <v>5</v>
+      </c>
+      <c r="H38" s="3">
+        <v>5</v>
+      </c>
+      <c r="I38" s="7"/>
+      <c r="J38" s="4">
+        <v>20</v>
+      </c>
+      <c r="K38" s="7">
+        <v>20</v>
+      </c>
+      <c r="L38" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="N38" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="O38" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E38" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="G38" s="14">
-        <v>6</v>
-      </c>
-      <c r="H38" s="3">
-        <v>6</v>
-      </c>
-      <c r="I38" s="7"/>
-      <c r="J38" s="37">
-        <v>19</v>
-      </c>
-      <c r="K38" s="38">
-        <v>19</v>
-      </c>
-      <c r="L38" s="39" t="s">
-        <v>31</v>
-      </c>
-      <c r="M38" s="39" t="s">
-        <v>45</v>
-      </c>
-      <c r="N38" s="39"/>
-      <c r="O38" s="39"/>
-      <c r="P38" s="39" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q38" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="R38" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="S38" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="T38" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="U38" s="8"/>
+      <c r="Q38" s="15"/>
       <c r="W38" s="26"/>
       <c r="X38" s="26"/>
       <c r="Y38" s="9"/>
@@ -3515,27 +3476,30 @@
     <row r="39" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A39" s="15"/>
       <c r="B39" s="15"/>
-      <c r="F39" s="14" t="s">
-        <v>17</v>
+      <c r="D39" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E39" s="14" t="s">
+        <v>21</v>
       </c>
       <c r="G39" s="14">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H39" s="3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I39" s="7"/>
       <c r="J39" s="37">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K39" s="38">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L39" s="39" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M39" s="39" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="N39" s="39"/>
       <c r="O39" s="39"/>
@@ -3543,16 +3507,16 @@
         <v>26</v>
       </c>
       <c r="Q39" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="R39" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="S39" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="T39" s="8" t="s">
         <v>107</v>
-      </c>
-      <c r="R39" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="S39" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="T39" s="8" t="s">
-        <v>112</v>
       </c>
       <c r="U39" s="8"/>
       <c r="W39" s="26"/>
@@ -3565,46 +3529,48 @@
       <c r="AD39" s="9"/>
     </row>
     <row r="40" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A40" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="B40" s="8"/>
-      <c r="C40" s="39"/>
-      <c r="D40" s="39"/>
-      <c r="E40" s="39"/>
-      <c r="F40" s="39" t="s">
-        <v>16</v>
-      </c>
-      <c r="G40" s="39">
-        <v>8</v>
+      <c r="A40" s="15"/>
+      <c r="B40" s="15"/>
+      <c r="F40" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G40" s="14">
+        <v>7</v>
       </c>
       <c r="H40" s="3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I40" s="7"/>
       <c r="J40" s="37">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K40" s="38">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L40" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="M40" s="39"/>
+        <v>32</v>
+      </c>
+      <c r="M40" s="39" t="s">
+        <v>44</v>
+      </c>
       <c r="N40" s="39"/>
-      <c r="O40" s="39" t="s">
-        <v>2</v>
-      </c>
+      <c r="O40" s="39"/>
       <c r="P40" s="39" t="s">
         <v>26</v>
       </c>
       <c r="Q40" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="R40" s="39" t="s">
-        <v>148</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="R40" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="S40" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="T40" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="U40" s="8"/>
       <c r="W40" s="26"/>
       <c r="X40" s="26"/>
       <c r="Y40" s="9"/>
@@ -3616,42 +3582,44 @@
     </row>
     <row r="41" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A41" s="8" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="B41" s="8"/>
       <c r="C41" s="39"/>
-      <c r="D41" s="39" t="s">
-        <v>2</v>
-      </c>
+      <c r="D41" s="39"/>
       <c r="E41" s="39"/>
       <c r="F41" s="39" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G41" s="39">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H41" s="3">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I41" s="7"/>
-      <c r="J41" s="4">
-        <v>16</v>
-      </c>
-      <c r="K41" s="7">
-        <v>16</v>
-      </c>
-      <c r="L41" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="O41" s="14" t="s">
+      <c r="J41" s="37">
+        <v>17</v>
+      </c>
+      <c r="K41" s="38">
+        <v>17</v>
+      </c>
+      <c r="L41" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="M41" s="39"/>
+      <c r="N41" s="39"/>
+      <c r="O41" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="P41" s="14" t="s">
+      <c r="P41" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="Q41" s="8"/>
+      <c r="Q41" s="8" t="s">
+        <v>110</v>
+      </c>
       <c r="R41" s="39" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="W41" s="26"/>
       <c r="X41" s="26"/>
@@ -3664,47 +3632,46 @@
     </row>
     <row r="42" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A42" s="8" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="39"/>
       <c r="D42" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="E42" s="39" t="s">
-        <v>22</v>
-      </c>
+      <c r="E42" s="39"/>
       <c r="F42" s="39" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G42" s="39">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H42" s="3">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I42" s="7"/>
-      <c r="J42" s="37">
-        <v>15</v>
-      </c>
-      <c r="K42" s="38">
-        <v>15</v>
-      </c>
-      <c r="L42" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="M42" s="39"/>
-      <c r="N42" s="39"/>
-      <c r="O42" s="39"/>
-      <c r="P42" s="39" t="s">
+      <c r="J42" s="4">
+        <v>16</v>
+      </c>
+      <c r="K42" s="7">
+        <v>16</v>
+      </c>
+      <c r="L42" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="O42" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="P42" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="Q42" s="8" t="s">
-        <v>160</v>
+      <c r="Q42" s="8"/>
+      <c r="R42" s="39" t="s">
+        <v>143</v>
       </c>
       <c r="W42" s="26"/>
       <c r="X42" s="26"/>
-      <c r="Y42" s="27"/>
+      <c r="Y42" s="9"/>
       <c r="Z42" s="9"/>
       <c r="AA42" s="9"/>
       <c r="AB42" s="9"/>
@@ -3713,41 +3680,47 @@
     </row>
     <row r="43" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A43" s="8" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="B43" s="8"/>
       <c r="C43" s="39"/>
-      <c r="D43" s="39"/>
+      <c r="D43" s="39" t="s">
+        <v>2</v>
+      </c>
       <c r="E43" s="39" t="s">
-        <v>23</v>
-      </c>
-      <c r="F43" s="39"/>
+        <v>22</v>
+      </c>
+      <c r="F43" s="39" t="s">
+        <v>14</v>
+      </c>
       <c r="G43" s="39">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H43" s="3">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I43" s="7"/>
       <c r="J43" s="37">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K43" s="38">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="L43" s="39" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M43" s="39"/>
       <c r="N43" s="39"/>
       <c r="O43" s="39"/>
-      <c r="P43" s="39"/>
+      <c r="P43" s="39" t="s">
+        <v>26</v>
+      </c>
       <c r="Q43" s="8" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="W43" s="26"/>
       <c r="X43" s="26"/>
-      <c r="Y43" s="9"/>
+      <c r="Y43" s="27"/>
       <c r="Z43" s="9"/>
       <c r="AA43" s="9"/>
       <c r="AB43" s="9"/>
@@ -3756,40 +3729,37 @@
     </row>
     <row r="44" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A44" s="8" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B44" s="8"/>
       <c r="C44" s="39"/>
       <c r="D44" s="39"/>
       <c r="E44" s="39" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F44" s="39"/>
       <c r="G44" s="39">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H44" s="3">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I44" s="7"/>
-      <c r="J44" s="37" t="s">
-        <v>37</v>
+      <c r="J44" s="37">
+        <v>14</v>
       </c>
       <c r="K44" s="38">
-        <v>13</v>
-      </c>
-      <c r="L44" s="39"/>
+        <v>14</v>
+      </c>
+      <c r="L44" s="39" t="s">
+        <v>36</v>
+      </c>
       <c r="M44" s="39"/>
-      <c r="N44" s="39" t="s">
-        <v>122</v>
-      </c>
+      <c r="N44" s="39"/>
       <c r="O44" s="39"/>
       <c r="P44" s="39"/>
       <c r="Q44" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="R44" s="8" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="W44" s="26"/>
       <c r="X44" s="26"/>
@@ -3801,19 +3771,41 @@
       <c r="AD44" s="9"/>
     </row>
     <row r="45" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>51</v>
-      </c>
-      <c r="H45" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="I45" s="12"/>
-      <c r="J45" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="K45" s="7"/>
-      <c r="Q45" t="s">
-        <v>51</v>
+      <c r="A45" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="B45" s="8"/>
+      <c r="C45" s="39"/>
+      <c r="D45" s="39"/>
+      <c r="E45" s="39" t="s">
+        <v>24</v>
+      </c>
+      <c r="F45" s="39"/>
+      <c r="G45" s="39">
+        <v>12</v>
+      </c>
+      <c r="H45" s="3">
+        <v>12</v>
+      </c>
+      <c r="I45" s="7"/>
+      <c r="J45" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="K45" s="38">
+        <v>13</v>
+      </c>
+      <c r="L45" s="39"/>
+      <c r="M45" s="39"/>
+      <c r="N45" s="39" t="s">
+        <v>117</v>
+      </c>
+      <c r="O45" s="39"/>
+      <c r="P45" s="39"/>
+      <c r="Q45" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="R45" s="8" t="s">
+        <v>133</v>
       </c>
       <c r="W45" s="26"/>
       <c r="X45" s="26"/>
@@ -3825,29 +3817,19 @@
       <c r="AD45" s="9"/>
     </row>
     <row r="46" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A46" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="B46" s="15"/>
-      <c r="G46" s="14">
-        <v>17</v>
-      </c>
-      <c r="H46" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="J46" s="37" t="s">
-        <v>10</v>
-      </c>
-      <c r="K46" s="38" t="s">
+      <c r="A46" t="s">
         <v>51</v>
       </c>
-      <c r="L46" s="39"/>
-      <c r="M46" s="39"/>
-      <c r="N46" s="39"/>
-      <c r="O46" s="39"/>
-      <c r="P46" s="39"/>
-      <c r="Q46" s="8" t="s">
-        <v>123</v>
+      <c r="H46" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="I46" s="12"/>
+      <c r="J46" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="K46" s="7"/>
+      <c r="Q46" t="s">
+        <v>51</v>
       </c>
       <c r="W46" s="26"/>
       <c r="X46" s="26"/>
@@ -3860,32 +3842,29 @@
     </row>
     <row r="47" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A47" s="15" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B47" s="15"/>
-      <c r="G47" s="14" t="s">
+      <c r="G47" s="14">
+        <v>17</v>
+      </c>
+      <c r="H47" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J47" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="K47" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="H47" s="44" t="s">
-        <v>6</v>
-      </c>
-      <c r="I47" s="43" t="s">
-        <v>129</v>
-      </c>
-      <c r="J47" s="42">
-        <v>24</v>
-      </c>
-      <c r="K47" s="43">
-        <v>24</v>
-      </c>
-      <c r="L47" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="M47" s="26"/>
-      <c r="N47" s="26"/>
-      <c r="O47" s="26"/>
-      <c r="P47" s="26"/>
-      <c r="Q47" s="15"/>
+      <c r="L47" s="39"/>
+      <c r="M47" s="39"/>
+      <c r="N47" s="39"/>
+      <c r="O47" s="39"/>
+      <c r="P47" s="39"/>
+      <c r="Q47" s="8" t="s">
+        <v>118</v>
+      </c>
       <c r="W47" s="26"/>
       <c r="X47" s="26"/>
       <c r="Y47" s="9"/>
@@ -3897,26 +3876,26 @@
     </row>
     <row r="48" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A48" s="15" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="B48" s="15"/>
       <c r="G48" s="14" t="s">
         <v>51</v>
       </c>
       <c r="H48" s="44" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I48" s="43" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="J48" s="42">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K48" s="43">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L48" s="26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M48" s="26"/>
       <c r="N48" s="26"/>
@@ -3933,29 +3912,33 @@
       <c r="AD48" s="9"/>
     </row>
     <row r="49" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A49" s="15"/>
+      <c r="A49" s="15" t="s">
+        <v>129</v>
+      </c>
       <c r="B49" s="15"/>
       <c r="G49" s="14" t="s">
         <v>51</v>
       </c>
       <c r="H49" s="44" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="I49" s="43" t="s">
-        <v>131</v>
-      </c>
-      <c r="J49" s="40" t="s">
-        <v>66</v>
-      </c>
-      <c r="K49" s="35"/>
-      <c r="L49" s="25"/>
-      <c r="M49" s="25"/>
-      <c r="N49" s="25"/>
-      <c r="O49" s="25"/>
-      <c r="P49" s="25"/>
-      <c r="Q49" s="24" t="s">
-        <v>146</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="J49" s="42">
+        <v>25</v>
+      </c>
+      <c r="K49" s="43">
+        <v>25</v>
+      </c>
+      <c r="L49" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="M49" s="26"/>
+      <c r="N49" s="26"/>
+      <c r="O49" s="26"/>
+      <c r="P49" s="26"/>
+      <c r="Q49" s="15"/>
       <c r="W49" s="26"/>
       <c r="X49" s="26"/>
       <c r="Y49" s="9"/>
@@ -3965,23 +3948,32 @@
       <c r="AC49" s="9"/>
       <c r="AD49" s="9"/>
     </row>
-    <row r="50" spans="1:30" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A50" s="15"/>
       <c r="B50" s="15"/>
-      <c r="G50" s="14">
-        <v>26</v>
-      </c>
-      <c r="H50" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="I50" s="13"/>
-      <c r="J50" s="6"/>
-      <c r="K50" s="7"/>
-      <c r="Q50" t="s">
+      <c r="G50" s="14" t="s">
         <v>51</v>
       </c>
+      <c r="H50" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="I50" s="43" t="s">
+        <v>126</v>
+      </c>
+      <c r="J50" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="K50" s="35"/>
+      <c r="L50" s="25"/>
+      <c r="M50" s="25"/>
+      <c r="N50" s="25"/>
+      <c r="O50" s="25"/>
+      <c r="P50" s="25"/>
+      <c r="Q50" s="24" t="s">
+        <v>140</v>
+      </c>
       <c r="W50" s="26"/>
-      <c r="X50" s="28"/>
+      <c r="X50" s="26"/>
       <c r="Y50" s="9"/>
       <c r="Z50" s="9"/>
       <c r="AA50" s="9"/>
@@ -3989,13 +3981,23 @@
       <c r="AC50" s="9"/>
       <c r="AD50" s="9"/>
     </row>
-    <row r="51" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="G51" s="7"/>
-      <c r="H51" s="45" t="s">
-        <v>137</v>
+    <row r="51" spans="1:30" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="15"/>
+      <c r="B51" s="15"/>
+      <c r="G51" s="14">
+        <v>26</v>
+      </c>
+      <c r="H51" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I51" s="13"/>
+      <c r="J51" s="6"/>
+      <c r="K51" s="7"/>
+      <c r="Q51" t="s">
+        <v>51</v>
       </c>
       <c r="W51" s="26"/>
-      <c r="X51" s="26"/>
+      <c r="X51" s="28"/>
       <c r="Y51" s="9"/>
       <c r="Z51" s="9"/>
       <c r="AA51" s="9"/>
@@ -4004,7 +4006,10 @@
       <c r="AD51" s="9"/>
     </row>
     <row r="52" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="I52" s="10"/>
+      <c r="G52" s="7"/>
+      <c r="H52" s="45" t="s">
+        <v>132</v>
+      </c>
       <c r="W52" s="26"/>
       <c r="X52" s="26"/>
       <c r="Y52" s="9"/>
@@ -4015,9 +4020,10 @@
       <c r="AD52" s="9"/>
     </row>
     <row r="53" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>144</v>
-      </c>
+      <c r="H53" t="s">
+        <v>203</v>
+      </c>
+      <c r="I53" s="10"/>
       <c r="W53" s="26"/>
       <c r="X53" s="26"/>
       <c r="Y53" s="9"/>
@@ -4027,1060 +4033,1109 @@
       <c r="AC53" s="9"/>
       <c r="AD53" s="9"/>
     </row>
-    <row r="54" spans="1:30" ht="26" x14ac:dyDescent="0.3">
-      <c r="A54" s="22" t="s">
-        <v>96</v>
-      </c>
-      <c r="B54" s="22"/>
-      <c r="H54" s="57"/>
-      <c r="I54" s="58" t="s">
-        <v>60</v>
-      </c>
-      <c r="J54" s="57"/>
-    </row>
-    <row r="55" spans="1:30" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>102</v>
-      </c>
-      <c r="B55" s="14" t="s">
+    <row r="54" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="H54" t="s">
+        <v>204</v>
+      </c>
+      <c r="I54" s="10"/>
+      <c r="W54" s="59"/>
+      <c r="X54" s="59"/>
+      <c r="Y54" s="9"/>
+      <c r="Z54" s="9"/>
+      <c r="AA54" s="9"/>
+      <c r="AB54" s="9"/>
+      <c r="AC54" s="9"/>
+      <c r="AD54" s="9"/>
+    </row>
+    <row r="55" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="H55" t="s">
+        <v>89</v>
+      </c>
+      <c r="I55" s="10"/>
+      <c r="W55" s="59"/>
+      <c r="X55" s="59"/>
+      <c r="Y55" s="9"/>
+      <c r="Z55" s="9"/>
+      <c r="AA55" s="9"/>
+      <c r="AB55" s="9"/>
+      <c r="AC55" s="9"/>
+      <c r="AD55" s="9"/>
+    </row>
+    <row r="56" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="I56" s="10"/>
+      <c r="W56" s="59"/>
+      <c r="X56" s="59"/>
+      <c r="Y56" s="9"/>
+      <c r="Z56" s="9"/>
+      <c r="AA56" s="9"/>
+      <c r="AB56" s="9"/>
+      <c r="AC56" s="9"/>
+      <c r="AD56" s="9"/>
+    </row>
+    <row r="57" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>138</v>
+      </c>
+      <c r="W57" s="26"/>
+      <c r="X57" s="26"/>
+      <c r="Y57" s="9"/>
+      <c r="Z57" s="9"/>
+      <c r="AA57" s="9"/>
+      <c r="AB57" s="9"/>
+      <c r="AC57" s="9"/>
+      <c r="AD57" s="9"/>
+    </row>
+    <row r="58" spans="1:30" ht="26" x14ac:dyDescent="0.3">
+      <c r="A58" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="B58" s="22"/>
+      <c r="H58" s="57"/>
+      <c r="I58" s="58" t="s">
+        <v>205</v>
+      </c>
+      <c r="J58" s="57"/>
+    </row>
+    <row r="59" spans="1:30" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>97</v>
+      </c>
+      <c r="B59" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="C59" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="C55" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="D55" s="14" t="s">
+      <c r="D59" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E55" s="14" t="s">
+      <c r="E59" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="F55" s="14" t="s">
+      <c r="F59" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="G55" s="14" t="s">
+      <c r="G59" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="H55" t="s">
+      <c r="H59" t="s">
         <v>5</v>
       </c>
-      <c r="J55" t="s">
+      <c r="J59" t="s">
         <v>5</v>
       </c>
-      <c r="K55" s="14" t="s">
+      <c r="K59" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="L55" s="14" t="s">
+      <c r="L59" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="M55" s="14" t="s">
+      <c r="M59" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="N55" s="14" t="s">
+      <c r="N59" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="O55" s="14" t="s">
+      <c r="O59" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="P55" s="14" t="s">
+      <c r="P59" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="Q55" t="s">
-        <v>102</v>
-      </c>
-      <c r="R55" s="14" t="s">
+      <c r="Q59" t="s">
+        <v>97</v>
+      </c>
+      <c r="R59" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="S59" t="s">
         <v>103</v>
       </c>
-      <c r="S55" t="s">
-        <v>108</v>
-      </c>
-      <c r="T55" s="14" t="s">
-        <v>109</v>
-      </c>
-      <c r="U55" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="56" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A56" s="29" t="s">
+      <c r="T59" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="B56" s="29"/>
-      <c r="C56" s="32"/>
-      <c r="D56" s="32"/>
-      <c r="E56" s="32"/>
-      <c r="F56" s="32"/>
-      <c r="G56" s="32"/>
-      <c r="H56" s="30" t="s">
+      <c r="U59" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="60" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A60" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="B60" s="29"/>
+      <c r="C60" s="32"/>
+      <c r="D60" s="32"/>
+      <c r="E60" s="32"/>
+      <c r="F60" s="32"/>
+      <c r="G60" s="32"/>
+      <c r="H60" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="J56" s="34" t="s">
-        <v>147</v>
-      </c>
-      <c r="K56" s="35"/>
-      <c r="L56" s="25"/>
-      <c r="M56" s="25"/>
-      <c r="N56" s="25"/>
-      <c r="O56" s="25"/>
-      <c r="P56" s="25"/>
-      <c r="Q56" s="36" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="57" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A57" s="8" t="s">
-        <v>162</v>
-      </c>
-      <c r="B57" s="8"/>
-      <c r="C57" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="F57" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="G57" s="14">
-        <v>0</v>
-      </c>
-      <c r="H57" s="3">
-        <v>0</v>
-      </c>
-      <c r="I57" s="7"/>
-      <c r="J57" s="31" t="s">
-        <v>128</v>
-      </c>
-      <c r="K57" s="33"/>
-      <c r="L57" s="32"/>
-      <c r="M57" s="32"/>
-      <c r="N57" s="32"/>
-      <c r="O57" s="32"/>
-      <c r="P57" s="32"/>
-      <c r="Q57" s="29" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="58" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A58" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="B58" s="8"/>
-      <c r="C58" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="F58" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="G58" s="14">
-        <v>1</v>
-      </c>
-      <c r="H58" s="3">
-        <v>1</v>
-      </c>
-      <c r="I58" s="7"/>
-      <c r="J58" s="40" t="s">
-        <v>125</v>
-      </c>
-      <c r="K58" s="35"/>
-      <c r="L58" s="25"/>
-      <c r="M58" s="25"/>
-      <c r="N58" s="25"/>
-      <c r="O58" s="25"/>
-      <c r="P58" s="25"/>
-      <c r="Q58" s="24" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="59" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A59" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="B59" s="56" t="s">
-        <v>187</v>
-      </c>
-      <c r="G59" s="14">
-        <v>2</v>
-      </c>
-      <c r="H59" s="3">
-        <v>2</v>
-      </c>
-      <c r="I59" s="7"/>
-      <c r="J59" s="37">
-        <v>23</v>
-      </c>
-      <c r="K59" s="38">
-        <v>23</v>
-      </c>
-      <c r="L59" s="39" t="s">
-        <v>27</v>
-      </c>
-      <c r="M59" s="39"/>
-      <c r="N59" s="39"/>
-      <c r="O59" s="39" t="s">
-        <v>2</v>
-      </c>
-      <c r="P59" s="39" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q59" s="8" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="60" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A60" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="B60" s="56" t="s">
-        <v>188</v>
-      </c>
-      <c r="D60" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="F60" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="G60" s="14">
-        <v>3</v>
-      </c>
-      <c r="H60" s="3">
-        <v>3</v>
-      </c>
-      <c r="I60" s="7"/>
-      <c r="J60" s="37">
-        <v>22</v>
-      </c>
-      <c r="K60" s="38">
-        <v>22</v>
-      </c>
-      <c r="L60" s="39" t="s">
-        <v>28</v>
-      </c>
-      <c r="M60" s="39"/>
-      <c r="N60" s="39"/>
-      <c r="O60" s="39" t="s">
-        <v>2</v>
-      </c>
-      <c r="P60" s="39" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q60" s="8" t="s">
-        <v>61</v>
+      <c r="J60" s="34" t="s">
+        <v>141</v>
+      </c>
+      <c r="K60" s="35"/>
+      <c r="L60" s="25"/>
+      <c r="M60" s="25"/>
+      <c r="N60" s="25"/>
+      <c r="O60" s="25"/>
+      <c r="P60" s="25"/>
+      <c r="Q60" s="36" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="61" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A61" s="8" t="s">
-        <v>173</v>
-      </c>
-      <c r="B61" s="60" t="s">
-        <v>203</v>
-      </c>
-      <c r="D61" s="14" t="s">
-        <v>2</v>
+        <v>155</v>
+      </c>
+      <c r="B61" s="8"/>
+      <c r="C61" s="14" t="s">
+        <v>26</v>
       </c>
       <c r="F61" s="14" t="s">
-        <v>121</v>
+        <v>12</v>
       </c>
       <c r="G61" s="14">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H61" s="3">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I61" s="7"/>
-      <c r="J61" s="37">
-        <v>21</v>
-      </c>
-      <c r="K61" s="38">
-        <v>21</v>
-      </c>
-      <c r="L61" s="39" t="s">
-        <v>29</v>
-      </c>
-      <c r="M61" s="39"/>
-      <c r="N61" s="39" t="s">
-        <v>120</v>
-      </c>
-      <c r="O61" s="39" t="s">
-        <v>2</v>
-      </c>
-      <c r="P61" s="39"/>
-      <c r="Q61" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="R61" s="39" t="s">
-        <v>189</v>
+      <c r="J61" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="K61" s="33"/>
+      <c r="L61" s="32"/>
+      <c r="M61" s="32"/>
+      <c r="N61" s="32"/>
+      <c r="O61" s="32"/>
+      <c r="P61" s="32"/>
+      <c r="Q61" s="29" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="62" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A62" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="B62" s="56" t="s">
+        <v>156</v>
+      </c>
+      <c r="B62" s="8"/>
+      <c r="C62" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F62" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G62" s="14">
+        <v>1</v>
+      </c>
+      <c r="H62" s="3">
+        <v>1</v>
+      </c>
+      <c r="I62" s="7"/>
+      <c r="J62" s="40" t="s">
+        <v>120</v>
+      </c>
+      <c r="K62" s="35"/>
+      <c r="L62" s="25"/>
+      <c r="M62" s="25"/>
+      <c r="N62" s="25"/>
+      <c r="O62" s="25"/>
+      <c r="P62" s="25"/>
+      <c r="Q62" s="24" t="s">
         <v>191</v>
-      </c>
-      <c r="C62" s="14" t="s">
-        <v>194</v>
-      </c>
-      <c r="D62" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="G62" s="14">
-        <v>5</v>
-      </c>
-      <c r="H62" s="3">
-        <v>5</v>
-      </c>
-      <c r="I62" s="7"/>
-      <c r="J62" s="37">
-        <v>20</v>
-      </c>
-      <c r="K62" s="38">
-        <v>20</v>
-      </c>
-      <c r="L62" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="M62" s="39"/>
-      <c r="N62" s="39" t="s">
-        <v>120</v>
-      </c>
-      <c r="O62" s="39" t="s">
-        <v>2</v>
-      </c>
-      <c r="P62" s="39"/>
-      <c r="Q62" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="R62" s="39" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="63" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A63" s="8" t="s">
-        <v>174</v>
-      </c>
-      <c r="B63" s="53" t="s">
-        <v>161</v>
-      </c>
-      <c r="D63" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="B63" s="56" t="s">
+        <v>180</v>
+      </c>
+      <c r="G63" s="14">
         <v>2</v>
       </c>
-      <c r="G63" s="14">
-        <v>6</v>
-      </c>
       <c r="H63" s="3">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I63" s="7"/>
       <c r="J63" s="37">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="K63" s="38">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="L63" s="39" t="s">
-        <v>31</v>
-      </c>
-      <c r="M63" s="39" t="s">
-        <v>45</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="M63" s="39"/>
       <c r="N63" s="39"/>
-      <c r="O63" s="39"/>
+      <c r="O63" s="39" t="s">
+        <v>2</v>
+      </c>
       <c r="P63" s="39" t="s">
         <v>26</v>
       </c>
       <c r="Q63" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="R63" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="S63" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="T63" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="U63" s="8"/>
+        <v>53</v>
+      </c>
     </row>
     <row r="64" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A64" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="B64" s="8"/>
-      <c r="F64" s="14" t="s">
-        <v>17</v>
+        <v>70</v>
+      </c>
+      <c r="B64" s="56" t="s">
+        <v>181</v>
+      </c>
+      <c r="D64" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="F64" s="39" t="s">
+        <v>116</v>
       </c>
       <c r="G64" s="14">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="H64" s="3">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="I64" s="7"/>
       <c r="J64" s="37">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="K64" s="38">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="L64" s="39" t="s">
-        <v>32</v>
-      </c>
-      <c r="M64" s="39" t="s">
-        <v>44</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="M64" s="39"/>
       <c r="N64" s="39"/>
-      <c r="O64" s="39"/>
+      <c r="O64" s="39" t="s">
+        <v>2</v>
+      </c>
       <c r="P64" s="39" t="s">
         <v>26</v>
       </c>
       <c r="Q64" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="R64" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="S64" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="T64" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="U64" s="8"/>
-    </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="65" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A65" s="8" t="s">
-        <v>175</v>
-      </c>
-      <c r="B65" s="55" t="s">
-        <v>185</v>
-      </c>
-      <c r="F65" s="14" t="s">
-        <v>16</v>
+        <v>166</v>
+      </c>
+      <c r="B65" s="60" t="s">
+        <v>196</v>
+      </c>
+      <c r="D65" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="F65" s="39" t="s">
+        <v>116</v>
       </c>
       <c r="G65" s="14">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="H65" s="3">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="I65" s="7"/>
       <c r="J65" s="37">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="K65" s="38">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="L65" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="M65" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="N65" s="39"/>
+        <v>29</v>
+      </c>
+      <c r="M65" s="39"/>
+      <c r="N65" s="39" t="s">
+        <v>115</v>
+      </c>
       <c r="O65" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="P65" s="39" t="s">
-        <v>26</v>
-      </c>
+      <c r="P65" s="39"/>
       <c r="Q65" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="R65" s="52" t="s">
-        <v>183</v>
-      </c>
-      <c r="S65" s="51"/>
-      <c r="T65" s="51"/>
-    </row>
-    <row r="66" spans="1:20" x14ac:dyDescent="0.2">
+        <v>169</v>
+      </c>
+      <c r="R65" s="39" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="66" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A66" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="B66" s="55" t="s">
-        <v>186</v>
+        <v>72</v>
+      </c>
+      <c r="B66" s="56" t="s">
+        <v>184</v>
+      </c>
+      <c r="C66" s="14" t="s">
+        <v>187</v>
       </c>
       <c r="D66" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="F66" s="14" t="s">
-        <v>15</v>
-      </c>
       <c r="G66" s="14">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="H66" s="3">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="I66" s="7"/>
       <c r="J66" s="37">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="K66" s="38">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="L66" s="39" t="s">
-        <v>34</v>
-      </c>
-      <c r="M66" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="N66" s="39"/>
+        <v>30</v>
+      </c>
+      <c r="M66" s="39"/>
+      <c r="N66" s="39" t="s">
+        <v>115</v>
+      </c>
       <c r="O66" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="P66" s="39" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q66" s="8"/>
-      <c r="R66" s="55" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="P66" s="39"/>
+      <c r="Q66" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="R66" s="39" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="67" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A67" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="B67" s="56" t="s">
-        <v>192</v>
+        <v>167</v>
+      </c>
+      <c r="B67" s="53" t="s">
+        <v>154</v>
       </c>
       <c r="D67" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E67" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="F67" s="14" t="s">
-        <v>14</v>
-      </c>
       <c r="G67" s="14">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="H67" s="3">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="I67" s="7"/>
       <c r="J67" s="37">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="K67" s="38">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="L67" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="M67" s="39"/>
+        <v>31</v>
+      </c>
+      <c r="M67" s="39" t="s">
+        <v>45</v>
+      </c>
       <c r="N67" s="39"/>
       <c r="O67" s="39"/>
       <c r="P67" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="Q67" s="56" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A68" s="51" t="s">
-        <v>196</v>
-      </c>
-      <c r="E68" s="14" t="s">
-        <v>118</v>
+      <c r="Q67" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="R67" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="S67" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="T67" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="U67" s="8"/>
+    </row>
+    <row r="68" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A68" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B68" s="8"/>
+      <c r="F68" s="14" t="s">
+        <v>17</v>
       </c>
       <c r="G68" s="14">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="H68" s="3">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="I68" s="7"/>
       <c r="J68" s="37">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="K68" s="38">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L68" s="39" t="s">
-        <v>36</v>
-      </c>
-      <c r="M68" s="39"/>
+        <v>32</v>
+      </c>
+      <c r="M68" s="39" t="s">
+        <v>44</v>
+      </c>
       <c r="N68" s="39"/>
       <c r="O68" s="39"/>
-      <c r="P68" s="39"/>
-      <c r="Q68" s="54" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A69" s="51" t="s">
-        <v>197</v>
-      </c>
-      <c r="B69" s="14"/>
-      <c r="E69" s="14" t="s">
-        <v>119</v>
+      <c r="P68" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q68" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="R68" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="S68" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="T68" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="U68" s="8"/>
+    </row>
+    <row r="69" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A69" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="B69" s="55" t="s">
+        <v>178</v>
+      </c>
+      <c r="F69" s="14" t="s">
+        <v>16</v>
       </c>
       <c r="G69" s="14">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="H69" s="3">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I69" s="7"/>
-      <c r="J69" s="37" t="s">
-        <v>37</v>
+      <c r="J69" s="37">
+        <v>17</v>
       </c>
       <c r="K69" s="38">
-        <v>13</v>
-      </c>
-      <c r="L69" s="39"/>
-      <c r="M69" s="39"/>
-      <c r="N69" s="39" t="s">
-        <v>122</v>
-      </c>
-      <c r="O69" s="39"/>
-      <c r="P69" s="39"/>
-      <c r="Q69" s="51" t="s">
-        <v>195</v>
-      </c>
-      <c r="R69" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="S69" s="9"/>
-    </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
-        <v>51</v>
-      </c>
-      <c r="H70" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="L69" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="M69" s="46" t="s">
+        <v>39</v>
+      </c>
+      <c r="N69" s="39"/>
+      <c r="O69" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="P69" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q69" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="R69" s="52" t="s">
+        <v>176</v>
+      </c>
+      <c r="S69" s="51"/>
+      <c r="T69" s="51"/>
+    </row>
+    <row r="70" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A70" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B70" s="55" t="s">
+        <v>179</v>
+      </c>
+      <c r="D70" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="F70" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="G70" s="14">
         <v>9</v>
       </c>
-      <c r="I70" s="12"/>
-      <c r="J70" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="K70" s="7"/>
-      <c r="Q70" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A71" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="B71" s="15"/>
-      <c r="G71" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="H71" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="J71" s="37" t="s">
+      <c r="H70" s="3">
+        <v>9</v>
+      </c>
+      <c r="I70" s="7"/>
+      <c r="J70" s="37">
+        <v>16</v>
+      </c>
+      <c r="K70" s="38">
+        <v>16</v>
+      </c>
+      <c r="L70" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="M70" s="46" t="s">
+        <v>40</v>
+      </c>
+      <c r="N70" s="39"/>
+      <c r="O70" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="P70" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q70" s="8"/>
+      <c r="R70" s="55" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="71" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A71" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="B71" s="56" t="s">
+        <v>185</v>
+      </c>
+      <c r="D71" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E71" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="F71" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G71" s="14">
         <v>10</v>
       </c>
-      <c r="K71" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="L71" s="39"/>
+      <c r="H71" s="3">
+        <v>10</v>
+      </c>
+      <c r="I71" s="7"/>
+      <c r="J71" s="37">
+        <v>15</v>
+      </c>
+      <c r="K71" s="38">
+        <v>15</v>
+      </c>
+      <c r="L71" s="39" t="s">
+        <v>35</v>
+      </c>
       <c r="M71" s="39"/>
       <c r="N71" s="39"/>
       <c r="O71" s="39"/>
-      <c r="P71" s="39"/>
-      <c r="Q71" s="8" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A72" s="15" t="s">
-        <v>133</v>
-      </c>
-      <c r="B72" s="15"/>
-      <c r="G72" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="H72" s="44" t="s">
-        <v>6</v>
-      </c>
-      <c r="I72" s="43" t="s">
-        <v>129</v>
-      </c>
-      <c r="J72" s="37" t="s">
-        <v>42</v>
-      </c>
-      <c r="K72" s="38"/>
+      <c r="P71" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q71" s="56" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="72" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A72" s="51" t="s">
+        <v>189</v>
+      </c>
+      <c r="E72" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="G72" s="14">
+        <v>11</v>
+      </c>
+      <c r="H72" s="3">
+        <v>11</v>
+      </c>
+      <c r="I72" s="7"/>
+      <c r="J72" s="37">
+        <v>14</v>
+      </c>
+      <c r="K72" s="38">
+        <v>14</v>
+      </c>
       <c r="L72" s="39" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="M72" s="39"/>
       <c r="N72" s="39"/>
       <c r="O72" s="39"/>
       <c r="P72" s="39"/>
-      <c r="Q72" s="8" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="73" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A73" s="15" t="s">
-        <v>134</v>
-      </c>
-      <c r="B73" s="15"/>
-      <c r="G73" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="H73" s="44" t="s">
-        <v>4</v>
-      </c>
-      <c r="I73" s="43" t="s">
-        <v>130</v>
-      </c>
+      <c r="Q72" s="54" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="73" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A73" s="51" t="s">
+        <v>190</v>
+      </c>
+      <c r="B73" s="14"/>
+      <c r="E73" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="G73" s="14">
+        <v>12</v>
+      </c>
+      <c r="H73" s="3">
+        <v>12</v>
+      </c>
+      <c r="I73" s="7"/>
       <c r="J73" s="37" t="s">
-        <v>43</v>
-      </c>
-      <c r="K73" s="38"/>
-      <c r="L73" s="39" t="s">
-        <v>43</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="K73" s="38">
+        <v>13</v>
+      </c>
+      <c r="L73" s="39"/>
       <c r="M73" s="39"/>
-      <c r="N73" s="39"/>
+      <c r="N73" s="39" t="s">
+        <v>117</v>
+      </c>
       <c r="O73" s="39"/>
       <c r="P73" s="39"/>
-      <c r="Q73" s="8" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="74" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A74" s="15" t="s">
-        <v>202</v>
-      </c>
-      <c r="B74" s="15"/>
-      <c r="G74" s="14" t="s">
+      <c r="Q73" s="51" t="s">
+        <v>188</v>
+      </c>
+      <c r="R73" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="S73" s="9"/>
+    </row>
+    <row r="74" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
         <v>51</v>
       </c>
-      <c r="H74" s="44" t="s">
-        <v>7</v>
-      </c>
-      <c r="I74" s="43" t="s">
-        <v>131</v>
-      </c>
-      <c r="J74" s="40" t="s">
-        <v>66</v>
-      </c>
-      <c r="K74" s="35"/>
-      <c r="L74" s="25"/>
-      <c r="M74" s="25"/>
-      <c r="N74" s="25"/>
-      <c r="O74" s="25"/>
-      <c r="P74" s="25"/>
-      <c r="Q74" s="24" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="75" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="B75" s="8"/>
+      <c r="H74" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="I74" s="12"/>
+      <c r="J74" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="K74" s="7"/>
+      <c r="Q74" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="75" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A75" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="B75" s="15"/>
       <c r="G75" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="H75" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="I75" s="13"/>
-      <c r="J75" s="6"/>
-      <c r="K75" s="7"/>
-      <c r="Q75" t="s">
+      <c r="H75" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="J75" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="K75" s="38" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="76" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="J76" s="47" t="s">
-        <v>126</v>
-      </c>
-      <c r="K76" s="39"/>
+      <c r="L75" s="39"/>
+      <c r="M75" s="39"/>
+      <c r="N75" s="39"/>
+      <c r="O75" s="39"/>
+      <c r="P75" s="39"/>
+      <c r="Q75" s="8" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="76" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A76" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="B76" s="15"/>
+      <c r="G76" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="H76" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="I76" s="43" t="s">
+        <v>124</v>
+      </c>
+      <c r="J76" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="K76" s="38"/>
       <c r="L76" s="39" t="s">
-        <v>126</v>
+        <v>42</v>
       </c>
       <c r="M76" s="39"/>
       <c r="N76" s="39"/>
       <c r="O76" s="39"/>
       <c r="P76" s="39"/>
       <c r="Q76" s="8" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="77" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="J77" s="48" t="s">
-        <v>127</v>
-      </c>
-      <c r="K77" s="39"/>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="77" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A77" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="B77" s="15"/>
+      <c r="G77" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="H77" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="I77" s="43" t="s">
+        <v>125</v>
+      </c>
+      <c r="J77" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="K77" s="38"/>
       <c r="L77" s="39" t="s">
-        <v>127</v>
+        <v>43</v>
       </c>
       <c r="M77" s="39"/>
       <c r="N77" s="39"/>
       <c r="O77" s="39"/>
       <c r="P77" s="39"/>
       <c r="Q77" s="8" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="78" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A78" s="65" t="s">
-        <v>205</v>
-      </c>
-      <c r="J78" s="49" t="s">
-        <v>4</v>
-      </c>
-      <c r="K78" s="32"/>
-      <c r="L78" s="32"/>
-      <c r="M78" s="32"/>
-      <c r="N78" s="32"/>
-      <c r="O78" s="32"/>
-      <c r="P78" s="32"/>
-      <c r="Q78" s="29" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="79" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A79" s="64" t="s">
-        <v>204</v>
-      </c>
-      <c r="J79" s="41" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q79" s="15"/>
-    </row>
-    <row r="80" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A80" s="61" t="s">
-        <v>206</v>
-      </c>
-      <c r="J80" s="48">
-        <v>24</v>
-      </c>
-      <c r="K80" s="39">
-        <v>24</v>
-      </c>
-      <c r="L80" s="39"/>
+        <v>151</v>
+      </c>
+    </row>
+    <row r="78" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A78" s="15" t="s">
+        <v>195</v>
+      </c>
+      <c r="B78" s="15"/>
+      <c r="G78" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="H78" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="I78" s="43" t="s">
+        <v>126</v>
+      </c>
+      <c r="J78" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="K78" s="35"/>
+      <c r="L78" s="25"/>
+      <c r="M78" s="25"/>
+      <c r="N78" s="25"/>
+      <c r="O78" s="25"/>
+      <c r="P78" s="25"/>
+      <c r="Q78" s="24" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="79" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="B79" s="8"/>
+      <c r="G79" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="H79" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="I79" s="13"/>
+      <c r="J79" s="6"/>
+      <c r="K79" s="7"/>
+      <c r="Q79" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="80" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="J80" s="47" t="s">
+        <v>121</v>
+      </c>
+      <c r="K80" s="39"/>
+      <c r="L80" s="39" t="s">
+        <v>121</v>
+      </c>
       <c r="M80" s="39"/>
       <c r="N80" s="39"/>
       <c r="O80" s="39"/>
       <c r="P80" s="39"/>
       <c r="Q80" s="8" t="s">
-        <v>88</v>
+        <v>151</v>
       </c>
     </row>
     <row r="81" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A81" s="61" t="s">
-        <v>209</v>
-      </c>
-      <c r="J81" s="48">
-        <v>25</v>
-      </c>
-      <c r="K81" s="39">
-        <v>25</v>
-      </c>
-      <c r="L81" s="39"/>
+      <c r="J81" s="48" t="s">
+        <v>122</v>
+      </c>
+      <c r="K81" s="39"/>
+      <c r="L81" s="39" t="s">
+        <v>122</v>
+      </c>
       <c r="M81" s="39"/>
       <c r="N81" s="39"/>
-      <c r="O81" s="39" t="s">
-        <v>2</v>
-      </c>
-      <c r="P81" s="39" t="s">
-        <v>26</v>
-      </c>
+      <c r="O81" s="39"/>
+      <c r="P81" s="39"/>
       <c r="Q81" s="8" t="s">
-        <v>177</v>
+        <v>151</v>
       </c>
     </row>
     <row r="82" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A82" s="63" t="s">
-        <v>207</v>
-      </c>
-      <c r="J82" s="48">
-        <v>26</v>
-      </c>
-      <c r="K82" s="39">
-        <v>26</v>
-      </c>
-      <c r="L82" s="39" t="s">
-        <v>166</v>
-      </c>
-      <c r="M82" s="39"/>
-      <c r="N82" s="39"/>
-      <c r="O82" s="39"/>
-      <c r="P82" s="39"/>
-      <c r="Q82" s="8" t="s">
-        <v>87</v>
+      <c r="A82" s="65" t="s">
+        <v>198</v>
+      </c>
+      <c r="J82" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="K82" s="32"/>
+      <c r="L82" s="32"/>
+      <c r="M82" s="32"/>
+      <c r="N82" s="32"/>
+      <c r="O82" s="32"/>
+      <c r="P82" s="32"/>
+      <c r="Q82" s="29" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="83" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A83" s="62" t="s">
-        <v>208</v>
-      </c>
-      <c r="J83" s="48">
-        <v>27</v>
-      </c>
-      <c r="K83" s="39">
-        <v>27</v>
-      </c>
-      <c r="L83" s="39" t="s">
-        <v>167</v>
-      </c>
-      <c r="M83" s="39"/>
-      <c r="N83" s="39"/>
-      <c r="O83" s="39"/>
-      <c r="P83" s="39"/>
-      <c r="Q83" s="8" t="s">
-        <v>178</v>
-      </c>
+      <c r="A83" s="64" t="s">
+        <v>197</v>
+      </c>
+      <c r="J83" s="41" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q83" s="15"/>
     </row>
     <row r="84" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A84" s="61" t="s">
+        <v>199</v>
+      </c>
       <c r="J84" s="48">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="K84" s="39">
-        <v>28</v>
-      </c>
-      <c r="L84" s="39" t="s">
-        <v>168</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="L84" s="39"/>
       <c r="M84" s="39"/>
       <c r="N84" s="39"/>
       <c r="O84" s="39"/>
       <c r="P84" s="39"/>
       <c r="Q84" s="8" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="85" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A85" s="61" t="s">
+        <v>202</v>
+      </c>
       <c r="J85" s="48">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="K85" s="39">
-        <v>29</v>
-      </c>
-      <c r="L85" s="39" t="s">
-        <v>169</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="L85" s="39"/>
       <c r="M85" s="39"/>
       <c r="N85" s="39"/>
-      <c r="O85" s="39"/>
-      <c r="P85" s="39"/>
+      <c r="O85" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="P85" s="39" t="s">
+        <v>26</v>
+      </c>
       <c r="Q85" s="8" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
     </row>
     <row r="86" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A86" s="63" t="s">
+        <v>200</v>
+      </c>
       <c r="J86" s="48">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="K86" s="39">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="L86" s="39" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="M86" s="39"/>
       <c r="N86" s="39"/>
       <c r="O86" s="39"/>
       <c r="P86" s="39"/>
       <c r="Q86" s="8" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="87" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A87" s="62" t="s">
+        <v>201</v>
+      </c>
       <c r="J87" s="48">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="K87" s="39">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="L87" s="39" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="M87" s="39"/>
       <c r="N87" s="39"/>
       <c r="O87" s="39"/>
       <c r="P87" s="39"/>
       <c r="Q87" s="8" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
     </row>
     <row r="88" spans="1:17" x14ac:dyDescent="0.2">
       <c r="J88" s="48">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="K88" s="39">
-        <v>32</v>
-      </c>
-      <c r="L88" s="39"/>
+        <v>28</v>
+      </c>
+      <c r="L88" s="39" t="s">
+        <v>161</v>
+      </c>
       <c r="M88" s="39"/>
       <c r="N88" s="39"/>
-      <c r="O88" s="39" t="s">
-        <v>2</v>
-      </c>
-      <c r="P88" s="39" t="s">
-        <v>26</v>
-      </c>
+      <c r="O88" s="39"/>
+      <c r="P88" s="39"/>
       <c r="Q88" s="8" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="89" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J89" s="50">
-        <v>33</v>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="89" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="J89" s="48">
+        <v>29</v>
       </c>
       <c r="K89" s="39">
-        <v>33</v>
-      </c>
-      <c r="L89" s="39"/>
+        <v>29</v>
+      </c>
+      <c r="L89" s="39" t="s">
+        <v>162</v>
+      </c>
       <c r="M89" s="39"/>
       <c r="N89" s="39"/>
       <c r="O89" s="39"/>
-      <c r="P89" s="39" t="s">
+      <c r="P89" s="39"/>
+      <c r="Q89" s="8" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="90" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="J90" s="48">
+        <v>30</v>
+      </c>
+      <c r="K90" s="39">
+        <v>30</v>
+      </c>
+      <c r="L90" s="39" t="s">
+        <v>163</v>
+      </c>
+      <c r="M90" s="39"/>
+      <c r="N90" s="39"/>
+      <c r="O90" s="39"/>
+      <c r="P90" s="39"/>
+      <c r="Q90" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="91" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="J91" s="48">
+        <v>31</v>
+      </c>
+      <c r="K91" s="39">
+        <v>31</v>
+      </c>
+      <c r="L91" s="39" t="s">
+        <v>164</v>
+      </c>
+      <c r="M91" s="39"/>
+      <c r="N91" s="39"/>
+      <c r="O91" s="39"/>
+      <c r="P91" s="39"/>
+      <c r="Q91" s="8" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="92" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="J92" s="48">
+        <v>32</v>
+      </c>
+      <c r="K92" s="39">
+        <v>32</v>
+      </c>
+      <c r="L92" s="39"/>
+      <c r="M92" s="39"/>
+      <c r="N92" s="39"/>
+      <c r="O92" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="P92" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="Q89" s="8" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="H90" s="45" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="H91" t="s">
-        <v>91</v>
-      </c>
-      <c r="M91"/>
-    </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="H92" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="H93" t="s">
-        <v>93</v>
+      <c r="Q92" s="8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="93" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="J93" s="50">
+        <v>33</v>
+      </c>
+      <c r="K93" s="39">
+        <v>33</v>
+      </c>
+      <c r="L93" s="39"/>
+      <c r="M93" s="39"/>
+      <c r="N93" s="39"/>
+      <c r="O93" s="39"/>
+      <c r="P93" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q93" s="8" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="94" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="H94" t="s">
-        <v>94</v>
+      <c r="H94" s="45" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="95" spans="1:17" x14ac:dyDescent="0.2">
       <c r="H95" t="s">
-        <v>95</v>
+        <v>210</v>
       </c>
       <c r="M95"/>
+    </row>
+    <row r="96" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="H96" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="97" spans="8:13" x14ac:dyDescent="0.2">
+      <c r="H97" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="98" spans="8:13" x14ac:dyDescent="0.2">
+      <c r="H98" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="99" spans="8:13" x14ac:dyDescent="0.2">
+      <c r="M99"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="W31:AC31"/>
+    <mergeCell ref="W32:AC32"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="A54" r:id="rId1" xr:uid="{CF74EE04-8972-D048-A403-865EBF5C5826}"/>
-    <hyperlink ref="A29" r:id="rId2" xr:uid="{5F2D9B69-2151-9947-A08D-C8EC4C5057AC}"/>
+    <hyperlink ref="A58" r:id="rId1" xr:uid="{CF74EE04-8972-D048-A403-865EBF5C5826}"/>
+    <hyperlink ref="A30" r:id="rId2" xr:uid="{5F2D9B69-2151-9947-A08D-C8EC4C5057AC}"/>
     <hyperlink ref="A2" r:id="rId3" xr:uid="{29D2941F-3028-724F-8C27-63EF821FDE70}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Log time, battery, brightness every minute to SD Card
</commit_message>
<xml_diff>
--- a/Electronic Design/Core 64 Pin Usage Mapping.xlsx
+++ b/Electronic Design/Core 64 Pin Usage Mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ageppert/Dropbox/Electronics/Core 64 Interactive Badge/Core-64-Interactive-Core-Memory-Badge/Electronic Design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFF74E56-2CFD-B941-88B0-632164F9E92E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{397ACE9E-D115-104A-9D14-C39419A0D205}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="27940" windowHeight="26460" activeTab="1" xr2:uid="{A4752792-CA31-B046-B883-84F8D68A57EC}"/>
   </bookViews>
@@ -2408,7 +2408,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CBC2977-27CE-C64F-BE79-A69FB2535F84}">
   <dimension ref="A1:AD99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="117" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B26" zoomScale="117" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="I99" sqref="I99"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update pin usage plan
</commit_message>
<xml_diff>
--- a/Electronic Design/Core 64 Pin Usage Mapping.xlsx
+++ b/Electronic Design/Core 64 Pin Usage Mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ageppert/Dropbox/Electronics/Core 64 Interactive Badge/Core-64-Interactive-Core-Memory-Badge/Electronic Design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{397ACE9E-D115-104A-9D14-C39419A0D205}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53A47DA4-0A94-2643-917C-AFF10E5880A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27940" windowHeight="26460" activeTab="1" xr2:uid="{A4752792-CA31-B046-B883-84F8D68A57EC}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="27480" activeTab="1" xr2:uid="{A4752792-CA31-B046-B883-84F8D68A57EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Reference Pinouts" sheetId="3" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="216">
   <si>
     <t>Custom</t>
   </si>
@@ -561,12 +561,6 @@
     <t>Matrix Drive 11 - Q6P (normally high)</t>
   </si>
   <si>
-    <t>TFT Reset (cannot be shared pin)</t>
-  </si>
-  <si>
-    <t>TFT BACKLIGHT LED BRIGHTNESS</t>
-  </si>
-  <si>
     <t>LED - Built-in (heart beat)</t>
   </si>
   <si>
@@ -594,9 +588,6 @@
     <t>Teensy View CS (default)</t>
   </si>
   <si>
-    <t>Teensy View Reset (cannot be shared pin) (default)</t>
-  </si>
-  <si>
     <t>IR MODULATOR</t>
   </si>
   <si>
@@ -667,6 +658,30 @@
   </si>
   <si>
     <t xml:space="preserve">Version 3.2 features a 32 bit ARM processor. Freescale MK20DX256VLH7 Cortex M4 w/DSP @72MHz, 256K Program Flash and FlexMemory, -40 to 105°C, </t>
+  </si>
+  <si>
+    <t>TFT BACKLIGHT</t>
+  </si>
+  <si>
+    <t>TFT Reset (cannot share)</t>
+  </si>
+  <si>
+    <t>Teensy View Reset (cannot share) (default)</t>
+  </si>
+  <si>
+    <t>SPARE GPIO 4</t>
+  </si>
+  <si>
+    <t>SPARE GPIO 5</t>
+  </si>
+  <si>
+    <t>SPARE GPIO 1 (3-to-8 decoder)</t>
+  </si>
+  <si>
+    <t>SPARE GPIO 2 (3-to-8 decoder)</t>
+  </si>
+  <si>
+    <t>SPARE GPIO 3 (3-to-8 decoder)</t>
   </si>
 </sst>
 </file>
@@ -2408,8 +2423,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CBC2977-27CE-C64F-BE79-A69FB2535F84}">
   <dimension ref="A1:AD99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B26" zoomScale="117" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="I99" sqref="I99"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="117" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="H80" sqref="H80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3074,12 +3089,12 @@
     </row>
     <row r="25" spans="1:30" x14ac:dyDescent="0.2">
       <c r="H25" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="26" spans="1:30" x14ac:dyDescent="0.2">
       <c r="H26" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="27" spans="1:30" x14ac:dyDescent="0.2">
@@ -4021,7 +4036,7 @@
     </row>
     <row r="53" spans="1:30" x14ac:dyDescent="0.2">
       <c r="H53" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="I53" s="10"/>
       <c r="W53" s="26"/>
@@ -4035,7 +4050,7 @@
     </row>
     <row r="54" spans="1:30" x14ac:dyDescent="0.2">
       <c r="H54" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="I54" s="10"/>
       <c r="W54" s="59"/>
@@ -4092,7 +4107,7 @@
       <c r="B58" s="22"/>
       <c r="H58" s="57"/>
       <c r="I58" s="58" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="J58" s="57"/>
     </row>
@@ -4181,14 +4196,16 @@
       <c r="O60" s="25"/>
       <c r="P60" s="25"/>
       <c r="Q60" s="36" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="61" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A61" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="B61" s="8"/>
+      <c r="B61" s="8" t="s">
+        <v>214</v>
+      </c>
       <c r="C61" s="14" t="s">
         <v>26</v>
       </c>
@@ -4219,7 +4236,9 @@
       <c r="A62" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="B62" s="8"/>
+      <c r="B62" s="8" t="s">
+        <v>213</v>
+      </c>
       <c r="C62" s="14" t="s">
         <v>26</v>
       </c>
@@ -4243,7 +4262,7 @@
       <c r="O62" s="25"/>
       <c r="P62" s="25"/>
       <c r="Q62" s="24" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="63" spans="1:30" x14ac:dyDescent="0.2">
@@ -4251,7 +4270,7 @@
         <v>165</v>
       </c>
       <c r="B63" s="56" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="G63" s="14">
         <v>2</v>
@@ -4286,7 +4305,7 @@
         <v>70</v>
       </c>
       <c r="B64" s="56" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D64" s="14" t="s">
         <v>2</v>
@@ -4327,7 +4346,7 @@
         <v>166</v>
       </c>
       <c r="B65" s="60" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="D65" s="14" t="s">
         <v>2</v>
@@ -4363,7 +4382,7 @@
         <v>169</v>
       </c>
       <c r="R65" s="39" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="66" spans="1:21" x14ac:dyDescent="0.2">
@@ -4371,10 +4390,10 @@
         <v>72</v>
       </c>
       <c r="B66" s="56" t="s">
+        <v>182</v>
+      </c>
+      <c r="C66" s="14" t="s">
         <v>184</v>
-      </c>
-      <c r="C66" s="14" t="s">
-        <v>187</v>
       </c>
       <c r="D66" s="14" t="s">
         <v>2</v>
@@ -4407,7 +4426,7 @@
         <v>78</v>
       </c>
       <c r="R66" s="39" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="67" spans="1:21" x14ac:dyDescent="0.2">
@@ -4509,7 +4528,7 @@
         <v>168</v>
       </c>
       <c r="B69" s="55" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F69" s="14" t="s">
         <v>16</v>
@@ -4544,17 +4563,15 @@
         <v>110</v>
       </c>
       <c r="R69" s="52" t="s">
-        <v>176</v>
-      </c>
-      <c r="S69" s="51"/>
-      <c r="T69" s="51"/>
+        <v>208</v>
+      </c>
     </row>
     <row r="70" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A70" s="8" t="s">
         <v>76</v>
       </c>
       <c r="B70" s="55" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D70" s="14" t="s">
         <v>2</v>
@@ -4588,17 +4605,19 @@
       <c r="P70" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="Q70" s="8"/>
+      <c r="Q70" s="8" t="s">
+        <v>212</v>
+      </c>
       <c r="R70" s="55" t="s">
-        <v>175</v>
+        <v>209</v>
       </c>
     </row>
     <row r="71" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A71" s="8" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B71" s="56" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D71" s="14" t="s">
         <v>2</v>
@@ -4631,13 +4650,16 @@
       <c r="P71" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="Q71" s="56" t="s">
-        <v>186</v>
+      <c r="Q71" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="R71" s="56" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="72" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A72" s="51" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="E72" s="14" t="s">
         <v>113</v>
@@ -4662,13 +4684,13 @@
       <c r="N72" s="39"/>
       <c r="O72" s="39"/>
       <c r="P72" s="39"/>
-      <c r="Q72" s="54" t="s">
-        <v>153</v>
+      <c r="Q72" s="8" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="73" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A73" s="51" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B73" s="14"/>
       <c r="E73" s="14" t="s">
@@ -4695,10 +4717,10 @@
       <c r="O73" s="39"/>
       <c r="P73" s="39"/>
       <c r="Q73" s="51" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="R73" s="8" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="S73" s="9"/>
     </row>
@@ -4741,7 +4763,7 @@
       <c r="O75" s="39"/>
       <c r="P75" s="39"/>
       <c r="Q75" s="8" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="76" spans="1:21" x14ac:dyDescent="0.2">
@@ -4798,13 +4820,13 @@
       <c r="N77" s="39"/>
       <c r="O77" s="39"/>
       <c r="P77" s="39"/>
-      <c r="Q77" s="8" t="s">
-        <v>151</v>
+      <c r="Q77" s="54" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="78" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A78" s="15" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B78" s="15"/>
       <c r="G78" s="14" t="s">
@@ -4826,7 +4848,7 @@
       <c r="O78" s="25"/>
       <c r="P78" s="25"/>
       <c r="Q78" s="24" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="79" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -4881,7 +4903,7 @@
     </row>
     <row r="82" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A82" s="65" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="J82" s="49" t="s">
         <v>4</v>
@@ -4898,7 +4920,7 @@
     </row>
     <row r="83" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A83" s="64" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="J83" s="41" t="s">
         <v>6</v>
@@ -4907,7 +4929,7 @@
     </row>
     <row r="84" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A84" s="61" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="J84" s="48">
         <v>24</v>
@@ -4926,7 +4948,7 @@
     </row>
     <row r="85" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A85" s="61" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="J85" s="48">
         <v>25</v>
@@ -4949,7 +4971,7 @@
     </row>
     <row r="86" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A86" s="63" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="J86" s="48">
         <v>26</v>
@@ -4970,7 +4992,7 @@
     </row>
     <row r="87" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A87" s="62" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="J87" s="48">
         <v>27</v>
@@ -5101,12 +5123,12 @@
     </row>
     <row r="94" spans="1:17" x14ac:dyDescent="0.2">
       <c r="H94" s="45" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="95" spans="1:17" x14ac:dyDescent="0.2">
       <c r="H95" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="M95"/>
     </row>
@@ -5117,12 +5139,12 @@
     </row>
     <row r="97" spans="8:13" x14ac:dyDescent="0.2">
       <c r="H97" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="98" spans="8:13" x14ac:dyDescent="0.2">
       <c r="H98" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="99" spans="8:13" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Update BOM V0.4, move assembly photos out of github
</commit_message>
<xml_diff>
--- a/Electronic Design/Core 64 Pin Usage Mapping.xlsx
+++ b/Electronic Design/Core 64 Pin Usage Mapping.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ageppert/Dropbox/Electronics/Core 64 Interactive Badge/Core-64-Interactive-Core-Memory-Badge/Electronic Design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53A47DA4-0A94-2643-917C-AFF10E5880A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CE75675-B927-5C4B-85D2-051FB01E5325}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="27480" activeTab="1" xr2:uid="{A4752792-CA31-B046-B883-84F8D68A57EC}"/>
   </bookViews>
@@ -2423,8 +2423,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CBC2977-27CE-C64F-BE79-A69FB2535F84}">
   <dimension ref="A1:AD99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="117" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="H80" sqref="H80"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="117" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B96" sqref="B96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Complete LB power schematic, add 3-to-8 decoder
</commit_message>
<xml_diff>
--- a/Electronic Design/Core 64 Pin Usage Mapping.xlsx
+++ b/Electronic Design/Core 64 Pin Usage Mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ageppert/Dropbox/Electronics/Core 64 Interactive Badge/Core-64-Interactive-Core-Memory-Badge/Electronic Design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CE75675-B927-5C4B-85D2-051FB01E5325}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51359086-F483-494A-9527-AFDEC7C60827}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="27480" activeTab="1" xr2:uid="{A4752792-CA31-B046-B883-84F8D68A57EC}"/>
+    <workbookView xWindow="16200" yWindow="460" windowWidth="35000" windowHeight="27480" activeTab="1" xr2:uid="{A4752792-CA31-B046-B883-84F8D68A57EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Reference Pinouts" sheetId="3" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="218">
   <si>
     <t>Custom</t>
   </si>
@@ -654,9 +654,6 @@
     <t>RAM  64K.</t>
   </si>
   <si>
-    <t>SPARE DIGITAL  &amp; PWM</t>
-  </si>
-  <si>
     <t xml:space="preserve">Version 3.2 features a 32 bit ARM processor. Freescale MK20DX256VLH7 Cortex M4 w/DSP @72MHz, 256K Program Flash and FlexMemory, -40 to 105°C, </t>
   </si>
   <si>
@@ -682,6 +679,15 @@
   </si>
   <si>
     <t>SPARE GPIO 3 (3-to-8 decoder)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Battery Voltage monitor </t>
+  </si>
+  <si>
+    <t>SPARE 6 DIGITAL  &amp; PWM</t>
+  </si>
+  <si>
+    <t>SENSE_RESET</t>
   </si>
 </sst>
 </file>
@@ -2423,8 +2429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CBC2977-27CE-C64F-BE79-A69FB2535F84}">
   <dimension ref="A1:AD99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="117" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B96" sqref="B96"/>
+    <sheetView tabSelected="1" topLeftCell="B55" zoomScale="117" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="R72" sqref="R72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4204,7 +4210,7 @@
         <v>155</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C61" s="14" t="s">
         <v>26</v>
@@ -4237,7 +4243,7 @@
         <v>156</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C62" s="14" t="s">
         <v>26</v>
@@ -4563,7 +4569,7 @@
         <v>110</v>
       </c>
       <c r="R69" s="52" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="70" spans="1:21" x14ac:dyDescent="0.2">
@@ -4606,15 +4612,15 @@
         <v>26</v>
       </c>
       <c r="Q70" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="R70" s="55" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="71" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A71" s="8" t="s">
-        <v>206</v>
+        <v>216</v>
       </c>
       <c r="B71" s="56" t="s">
         <v>183</v>
@@ -4651,10 +4657,10 @@
         <v>26</v>
       </c>
       <c r="Q71" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="R71" s="56" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="72" spans="1:21" x14ac:dyDescent="0.2">
@@ -4685,7 +4691,10 @@
       <c r="O72" s="39"/>
       <c r="P72" s="39"/>
       <c r="Q72" s="8" t="s">
-        <v>215</v>
+        <v>214</v>
+      </c>
+      <c r="R72" s="8" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="73" spans="1:21" x14ac:dyDescent="0.2">
@@ -4792,7 +4801,7 @@
       <c r="O76" s="39"/>
       <c r="P76" s="39"/>
       <c r="Q76" s="8" t="s">
-        <v>119</v>
+        <v>215</v>
       </c>
     </row>
     <row r="77" spans="1:21" x14ac:dyDescent="0.2">
@@ -5128,7 +5137,7 @@
     </row>
     <row r="95" spans="1:17" x14ac:dyDescent="0.2">
       <c r="H95" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="M95"/>
     </row>

</xml_diff>

<commit_message>
Add 3-to-8 and begin other expansion on schematic
</commit_message>
<xml_diff>
--- a/Electronic Design/Core 64 Pin Usage Mapping.xlsx
+++ b/Electronic Design/Core 64 Pin Usage Mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ageppert/Dropbox/Electronics/Core 64 Interactive Badge/Core-64-Interactive-Core-Memory-Badge/Electronic Design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51359086-F483-494A-9527-AFDEC7C60827}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0EA9C86-4F42-FF48-AD96-86E6C95FEB98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16200" yWindow="460" windowWidth="35000" windowHeight="27480" activeTab="1" xr2:uid="{A4752792-CA31-B046-B883-84F8D68A57EC}"/>
   </bookViews>
@@ -501,12 +501,6 @@
     <t>SDCARD_CS</t>
   </si>
   <si>
-    <t>SAO Port 1&amp;2, GPIO 2 (RX)</t>
-  </si>
-  <si>
-    <t>SAO Port 1&amp;2, GPIO 1 (TX)</t>
-  </si>
-  <si>
     <t>SAO 1&amp;2</t>
   </si>
   <si>
@@ -688,6 +682,12 @@
   </si>
   <si>
     <t>SENSE_RESET</t>
+  </si>
+  <si>
+    <t>SAO Port, GPIO 1</t>
+  </si>
+  <si>
+    <t>SAO Port, GPIO 2</t>
   </si>
 </sst>
 </file>
@@ -796,7 +796,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -860,6 +860,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -994,7 +1000,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1156,6 +1162,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2429,8 +2436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CBC2977-27CE-C64F-BE79-A69FB2535F84}">
   <dimension ref="A1:AD99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B55" zoomScale="117" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="R72" sqref="R72"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="117" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="I81" sqref="I81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3095,12 +3102,12 @@
     </row>
     <row r="25" spans="1:30" x14ac:dyDescent="0.2">
       <c r="H25" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="26" spans="1:30" x14ac:dyDescent="0.2">
       <c r="H26" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="27" spans="1:30" x14ac:dyDescent="0.2">
@@ -3347,7 +3354,7 @@
         <v>26</v>
       </c>
       <c r="Q35" s="19" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="W35" s="26"/>
       <c r="X35" s="26"/>
@@ -4042,7 +4049,7 @@
     </row>
     <row r="53" spans="1:30" x14ac:dyDescent="0.2">
       <c r="H53" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="I53" s="10"/>
       <c r="W53" s="26"/>
@@ -4056,7 +4063,7 @@
     </row>
     <row r="54" spans="1:30" x14ac:dyDescent="0.2">
       <c r="H54" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="I54" s="10"/>
       <c r="W54" s="59"/>
@@ -4113,7 +4120,7 @@
       <c r="B58" s="22"/>
       <c r="H58" s="57"/>
       <c r="I58" s="58" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="J58" s="57"/>
     </row>
@@ -4202,15 +4209,15 @@
       <c r="O60" s="25"/>
       <c r="P60" s="25"/>
       <c r="Q60" s="36" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="61" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A61" s="8" t="s">
-        <v>155</v>
+        <v>216</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C61" s="14" t="s">
         <v>26</v>
@@ -4240,10 +4247,10 @@
     </row>
     <row r="62" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A62" s="8" t="s">
-        <v>156</v>
+        <v>217</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C62" s="14" t="s">
         <v>26</v>
@@ -4268,15 +4275,15 @@
       <c r="O62" s="25"/>
       <c r="P62" s="25"/>
       <c r="Q62" s="24" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="63" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A63" s="8" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B63" s="56" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G63" s="14">
         <v>2</v>
@@ -4311,7 +4318,7 @@
         <v>70</v>
       </c>
       <c r="B64" s="56" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D64" s="14" t="s">
         <v>2</v>
@@ -4349,10 +4356,10 @@
     </row>
     <row r="65" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A65" s="8" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B65" s="60" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D65" s="14" t="s">
         <v>2</v>
@@ -4385,10 +4392,10 @@
       </c>
       <c r="P65" s="39"/>
       <c r="Q65" s="8" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="R65" s="39" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="66" spans="1:21" x14ac:dyDescent="0.2">
@@ -4396,10 +4403,10 @@
         <v>72</v>
       </c>
       <c r="B66" s="56" t="s">
+        <v>180</v>
+      </c>
+      <c r="C66" s="14" t="s">
         <v>182</v>
-      </c>
-      <c r="C66" s="14" t="s">
-        <v>184</v>
       </c>
       <c r="D66" s="14" t="s">
         <v>2</v>
@@ -4432,12 +4439,12 @@
         <v>78</v>
       </c>
       <c r="R66" s="39" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="67" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A67" s="8" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B67" s="53" t="s">
         <v>154</v>
@@ -4479,7 +4486,7 @@
         <v>106</v>
       </c>
       <c r="T67" s="8" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="U67" s="8"/>
     </row>
@@ -4525,16 +4532,16 @@
         <v>106</v>
       </c>
       <c r="T68" s="8" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="U68" s="8"/>
     </row>
     <row r="69" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A69" s="8" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B69" s="55" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F69" s="14" t="s">
         <v>16</v>
@@ -4569,7 +4576,7 @@
         <v>110</v>
       </c>
       <c r="R69" s="52" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="70" spans="1:21" x14ac:dyDescent="0.2">
@@ -4577,7 +4584,7 @@
         <v>76</v>
       </c>
       <c r="B70" s="55" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D70" s="14" t="s">
         <v>2</v>
@@ -4612,18 +4619,18 @@
         <v>26</v>
       </c>
       <c r="Q70" s="8" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="R70" s="55" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="71" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A71" s="8" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B71" s="56" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D71" s="14" t="s">
         <v>2</v>
@@ -4657,15 +4664,15 @@
         <v>26</v>
       </c>
       <c r="Q71" s="8" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="R71" s="56" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="72" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A72" s="51" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E72" s="14" t="s">
         <v>113</v>
@@ -4691,15 +4698,12 @@
       <c r="O72" s="39"/>
       <c r="P72" s="39"/>
       <c r="Q72" s="8" t="s">
-        <v>214</v>
-      </c>
-      <c r="R72" s="8" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
     </row>
     <row r="73" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A73" s="51" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B73" s="14"/>
       <c r="E73" s="14" t="s">
@@ -4724,12 +4728,14 @@
         <v>117</v>
       </c>
       <c r="O73" s="39"/>
-      <c r="P73" s="39"/>
+      <c r="P73" s="67" t="s">
+        <v>215</v>
+      </c>
       <c r="Q73" s="51" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="R73" s="8" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="S73" s="9"/>
     </row>
@@ -4772,7 +4778,7 @@
       <c r="O75" s="39"/>
       <c r="P75" s="39"/>
       <c r="Q75" s="8" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="76" spans="1:21" x14ac:dyDescent="0.2">
@@ -4801,7 +4807,7 @@
       <c r="O76" s="39"/>
       <c r="P76" s="39"/>
       <c r="Q76" s="8" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="77" spans="1:21" x14ac:dyDescent="0.2">
@@ -4835,7 +4841,7 @@
     </row>
     <row r="78" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A78" s="15" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B78" s="15"/>
       <c r="G78" s="14" t="s">
@@ -4857,7 +4863,7 @@
       <c r="O78" s="25"/>
       <c r="P78" s="25"/>
       <c r="Q78" s="24" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="79" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -4912,7 +4918,7 @@
     </row>
     <row r="82" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A82" s="65" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="J82" s="49" t="s">
         <v>4</v>
@@ -4929,7 +4935,7 @@
     </row>
     <row r="83" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A83" s="64" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="J83" s="41" t="s">
         <v>6</v>
@@ -4938,7 +4944,7 @@
     </row>
     <row r="84" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A84" s="61" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="J84" s="48">
         <v>24</v>
@@ -4957,7 +4963,7 @@
     </row>
     <row r="85" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A85" s="61" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="J85" s="48">
         <v>25</v>
@@ -4975,12 +4981,12 @@
         <v>26</v>
       </c>
       <c r="Q85" s="8" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="86" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A86" s="63" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="J86" s="48">
         <v>26</v>
@@ -4989,7 +4995,7 @@
         <v>26</v>
       </c>
       <c r="L86" s="39" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="M86" s="39"/>
       <c r="N86" s="39"/>
@@ -5001,7 +5007,7 @@
     </row>
     <row r="87" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A87" s="62" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J87" s="48">
         <v>27</v>
@@ -5010,14 +5016,14 @@
         <v>27</v>
       </c>
       <c r="L87" s="39" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="M87" s="39"/>
       <c r="N87" s="39"/>
       <c r="O87" s="39"/>
       <c r="P87" s="39"/>
       <c r="Q87" s="8" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="88" spans="1:17" x14ac:dyDescent="0.2">
@@ -5028,7 +5034,7 @@
         <v>28</v>
       </c>
       <c r="L88" s="39" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="M88" s="39"/>
       <c r="N88" s="39"/>
@@ -5046,14 +5052,14 @@
         <v>29</v>
       </c>
       <c r="L89" s="39" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="M89" s="39"/>
       <c r="N89" s="39"/>
       <c r="O89" s="39"/>
       <c r="P89" s="39"/>
       <c r="Q89" s="8" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="90" spans="1:17" x14ac:dyDescent="0.2">
@@ -5064,7 +5070,7 @@
         <v>30</v>
       </c>
       <c r="L90" s="39" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="M90" s="39"/>
       <c r="N90" s="39"/>
@@ -5082,14 +5088,14 @@
         <v>31</v>
       </c>
       <c r="L91" s="39" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="M91" s="39"/>
       <c r="N91" s="39"/>
       <c r="O91" s="39"/>
       <c r="P91" s="39"/>
       <c r="Q91" s="8" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="92" spans="1:17" x14ac:dyDescent="0.2">
@@ -5127,17 +5133,17 @@
         <v>26</v>
       </c>
       <c r="Q93" s="8" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="94" spans="1:17" x14ac:dyDescent="0.2">
       <c r="H94" s="45" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="95" spans="1:17" x14ac:dyDescent="0.2">
       <c r="H95" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="M95"/>
     </row>
@@ -5148,12 +5154,12 @@
     </row>
     <row r="97" spans="8:13" x14ac:dyDescent="0.2">
       <c r="H97" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="98" spans="8:13" x14ac:dyDescent="0.2">
       <c r="H98" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="99" spans="8:13" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Update schematic and XLS pin usage
</commit_message>
<xml_diff>
--- a/Electronic Design/Core 64 Pin Usage Mapping.xlsx
+++ b/Electronic Design/Core 64 Pin Usage Mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ageppert/Dropbox/Electronics/Core 64 Interactive Badge/Core-64-Interactive-Core-Memory-Badge/Electronic Design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0EA9C86-4F42-FF48-AD96-86E6C95FEB98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{446F0AF5-F205-1E43-98A7-9582B3F0C7A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16200" yWindow="460" windowWidth="35000" windowHeight="27480" activeTab="1" xr2:uid="{A4752792-CA31-B046-B883-84F8D68A57EC}"/>
+    <workbookView xWindow="16500" yWindow="460" windowWidth="34700" windowHeight="27480" activeTab="1" xr2:uid="{A4752792-CA31-B046-B883-84F8D68A57EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Reference Pinouts" sheetId="3" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="219">
   <si>
     <t>Custom</t>
   </si>
@@ -489,9 +489,6 @@
     <t>Bring out the DAC for expansion!</t>
   </si>
   <si>
-    <t>SPARE ANALOG (or pseudo digital input)</t>
-  </si>
-  <si>
     <t>A14/DAC</t>
   </si>
   <si>
@@ -588,12 +585,6 @@
     <t>SPI SCK (default)</t>
   </si>
   <si>
-    <t>SPI SDI (MOSI) default</t>
-  </si>
-  <si>
-    <t>SPI SDO (MISO) default</t>
-  </si>
-  <si>
     <t>TEENSY_3V3_AREF</t>
   </si>
   <si>
@@ -657,30 +648,12 @@
     <t>TFT Reset (cannot share)</t>
   </si>
   <si>
-    <t>Teensy View Reset (cannot share) (default)</t>
-  </si>
-  <si>
-    <t>SPARE GPIO 4</t>
-  </si>
-  <si>
     <t>SPARE GPIO 5</t>
   </si>
   <si>
-    <t>SPARE GPIO 1 (3-to-8 decoder)</t>
-  </si>
-  <si>
-    <t>SPARE GPIO 2 (3-to-8 decoder)</t>
-  </si>
-  <si>
-    <t>SPARE GPIO 3 (3-to-8 decoder)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Battery Voltage monitor </t>
   </si>
   <si>
-    <t>SPARE 6 DIGITAL  &amp; PWM</t>
-  </si>
-  <si>
     <t>SENSE_RESET</t>
   </si>
   <si>
@@ -688,6 +661,36 @@
   </si>
   <si>
     <t>SAO Port, GPIO 2</t>
+  </si>
+  <si>
+    <t>Primary Use</t>
+  </si>
+  <si>
+    <t>SPI SDO (MOSI) default</t>
+  </si>
+  <si>
+    <t>SPI SDI (MISO) default</t>
+  </si>
+  <si>
+    <t>DO NOT USE Teensy View Reset (cannot share) (default)</t>
+  </si>
+  <si>
+    <t>SPARE 6 ANALOG (or pseudo digital input)</t>
+  </si>
+  <si>
+    <t>SPARE 7 ANALOG (or pseudo digital input)</t>
+  </si>
+  <si>
+    <t>SPARE 4 DIGITAL  &amp; PWM</t>
+  </si>
+  <si>
+    <t>SPARE GPIO 3 (ADDR2 3-to-8 decoder)</t>
+  </si>
+  <si>
+    <t>SPARE 1 GPIO 1 (ADDR 0 3-to-8 decoder)</t>
+  </si>
+  <si>
+    <t>SPARE 2 GPIO 2 (ADDR 1 3-to-8 decoder)</t>
   </si>
 </sst>
 </file>
@@ -1159,10 +1162,10 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2436,8 +2439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CBC2977-27CE-C64F-BE79-A69FB2535F84}">
   <dimension ref="A1:AD99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="117" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="I81" sqref="I81"/>
+    <sheetView tabSelected="1" topLeftCell="B48" zoomScale="117" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="F61" sqref="F61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3102,12 +3105,12 @@
     </row>
     <row r="25" spans="1:30" x14ac:dyDescent="0.2">
       <c r="H25" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="26" spans="1:30" x14ac:dyDescent="0.2">
       <c r="H26" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="27" spans="1:30" x14ac:dyDescent="0.2">
@@ -3224,13 +3227,13 @@
       <c r="Q32" s="36" t="s">
         <v>100</v>
       </c>
-      <c r="W32" s="66"/>
-      <c r="X32" s="66"/>
-      <c r="Y32" s="66"/>
-      <c r="Z32" s="66"/>
-      <c r="AA32" s="66"/>
-      <c r="AB32" s="66"/>
-      <c r="AC32" s="66"/>
+      <c r="W32" s="67"/>
+      <c r="X32" s="67"/>
+      <c r="Y32" s="67"/>
+      <c r="Z32" s="67"/>
+      <c r="AA32" s="67"/>
+      <c r="AB32" s="67"/>
+      <c r="AC32" s="67"/>
       <c r="AD32" s="9"/>
     </row>
     <row r="33" spans="1:30" x14ac:dyDescent="0.2">
@@ -3354,7 +3357,7 @@
         <v>26</v>
       </c>
       <c r="Q35" s="19" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="W35" s="26"/>
       <c r="X35" s="26"/>
@@ -3744,7 +3747,7 @@
         <v>26</v>
       </c>
       <c r="Q43" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="W43" s="26"/>
       <c r="X43" s="26"/>
@@ -4049,7 +4052,7 @@
     </row>
     <row r="53" spans="1:30" x14ac:dyDescent="0.2">
       <c r="H53" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="I53" s="10"/>
       <c r="W53" s="26"/>
@@ -4063,7 +4066,7 @@
     </row>
     <row r="54" spans="1:30" x14ac:dyDescent="0.2">
       <c r="H54" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="I54" s="10"/>
       <c r="W54" s="59"/>
@@ -4120,13 +4123,13 @@
       <c r="B58" s="22"/>
       <c r="H58" s="57"/>
       <c r="I58" s="58" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="J58" s="57"/>
     </row>
     <row r="59" spans="1:30" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>97</v>
+        <v>209</v>
       </c>
       <c r="B59" s="14" t="s">
         <v>98</v>
@@ -4209,15 +4212,15 @@
       <c r="O60" s="25"/>
       <c r="P60" s="25"/>
       <c r="Q60" s="36" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="61" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A61" s="8" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>210</v>
+        <v>217</v>
       </c>
       <c r="C61" s="14" t="s">
         <v>26</v>
@@ -4247,10 +4250,10 @@
     </row>
     <row r="62" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A62" s="8" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="C62" s="14" t="s">
         <v>26</v>
@@ -4275,15 +4278,15 @@
       <c r="O62" s="25"/>
       <c r="P62" s="25"/>
       <c r="Q62" s="24" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="63" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A63" s="8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B63" s="56" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G63" s="14">
         <v>2</v>
@@ -4318,7 +4321,7 @@
         <v>70</v>
       </c>
       <c r="B64" s="56" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D64" s="14" t="s">
         <v>2</v>
@@ -4356,10 +4359,10 @@
     </row>
     <row r="65" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A65" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B65" s="60" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="D65" s="14" t="s">
         <v>2</v>
@@ -4392,7 +4395,7 @@
       </c>
       <c r="P65" s="39"/>
       <c r="Q65" s="8" t="s">
-        <v>167</v>
+        <v>78</v>
       </c>
       <c r="R65" s="39" t="s">
         <v>178</v>
@@ -4403,10 +4406,10 @@
         <v>72</v>
       </c>
       <c r="B66" s="56" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C66" s="14" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D66" s="14" t="s">
         <v>2</v>
@@ -4436,18 +4439,18 @@
       </c>
       <c r="P66" s="39"/>
       <c r="Q66" s="8" t="s">
-        <v>78</v>
+        <v>166</v>
       </c>
       <c r="R66" s="39" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="67" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A67" s="8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B67" s="53" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D67" s="14" t="s">
         <v>2</v>
@@ -4486,7 +4489,7 @@
         <v>106</v>
       </c>
       <c r="T67" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="U67" s="8"/>
     </row>
@@ -4532,16 +4535,16 @@
         <v>106</v>
       </c>
       <c r="T68" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="U68" s="8"/>
     </row>
     <row r="69" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A69" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B69" s="55" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F69" s="14" t="s">
         <v>16</v>
@@ -4576,7 +4579,7 @@
         <v>110</v>
       </c>
       <c r="R69" s="52" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="70" spans="1:21" x14ac:dyDescent="0.2">
@@ -4584,7 +4587,7 @@
         <v>76</v>
       </c>
       <c r="B70" s="55" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D70" s="14" t="s">
         <v>2</v>
@@ -4619,18 +4622,18 @@
         <v>26</v>
       </c>
       <c r="Q70" s="8" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="R70" s="55" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="71" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A71" s="8" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B71" s="56" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D71" s="14" t="s">
         <v>2</v>
@@ -4663,16 +4666,16 @@
       <c r="P71" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="Q71" s="8" t="s">
-        <v>208</v>
+      <c r="Q71" s="66" t="s">
+        <v>206</v>
       </c>
       <c r="R71" s="56" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
     </row>
     <row r="72" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A72" s="51" t="s">
-        <v>184</v>
+        <v>210</v>
       </c>
       <c r="E72" s="14" t="s">
         <v>113</v>
@@ -4698,12 +4701,12 @@
       <c r="O72" s="39"/>
       <c r="P72" s="39"/>
       <c r="Q72" s="8" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
     </row>
     <row r="73" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A73" s="51" t="s">
-        <v>185</v>
+        <v>211</v>
       </c>
       <c r="B73" s="14"/>
       <c r="E73" s="14" t="s">
@@ -4728,14 +4731,12 @@
         <v>117</v>
       </c>
       <c r="O73" s="39"/>
-      <c r="P73" s="67" t="s">
-        <v>215</v>
-      </c>
+      <c r="P73" s="39"/>
       <c r="Q73" s="51" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="R73" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="S73" s="9"/>
     </row>
@@ -4778,7 +4779,7 @@
       <c r="O75" s="39"/>
       <c r="P75" s="39"/>
       <c r="Q75" s="8" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="76" spans="1:21" x14ac:dyDescent="0.2">
@@ -4807,7 +4808,7 @@
       <c r="O76" s="39"/>
       <c r="P76" s="39"/>
       <c r="Q76" s="8" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
     </row>
     <row r="77" spans="1:21" x14ac:dyDescent="0.2">
@@ -4836,12 +4837,12 @@
       <c r="O77" s="39"/>
       <c r="P77" s="39"/>
       <c r="Q77" s="54" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="78" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A78" s="15" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B78" s="15"/>
       <c r="G78" s="14" t="s">
@@ -4863,7 +4864,7 @@
       <c r="O78" s="25"/>
       <c r="P78" s="25"/>
       <c r="Q78" s="24" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="79" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -4875,7 +4876,7 @@
         <v>51</v>
       </c>
       <c r="H79" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I79" s="13"/>
       <c r="J79" s="6"/>
@@ -4897,7 +4898,7 @@
       <c r="O80" s="39"/>
       <c r="P80" s="39"/>
       <c r="Q80" s="8" t="s">
-        <v>151</v>
+        <v>213</v>
       </c>
     </row>
     <row r="81" spans="1:17" x14ac:dyDescent="0.2">
@@ -4913,12 +4914,12 @@
       <c r="O81" s="39"/>
       <c r="P81" s="39"/>
       <c r="Q81" s="8" t="s">
-        <v>151</v>
+        <v>214</v>
       </c>
     </row>
     <row r="82" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A82" s="65" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="J82" s="49" t="s">
         <v>4</v>
@@ -4935,7 +4936,7 @@
     </row>
     <row r="83" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A83" s="64" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="J83" s="41" t="s">
         <v>6</v>
@@ -4944,7 +4945,7 @@
     </row>
     <row r="84" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A84" s="61" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="J84" s="48">
         <v>24</v>
@@ -4958,12 +4959,12 @@
       <c r="O84" s="39"/>
       <c r="P84" s="39"/>
       <c r="Q84" s="8" t="s">
-        <v>88</v>
+        <v>171</v>
       </c>
     </row>
     <row r="85" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A85" s="61" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="J85" s="48">
         <v>25</v>
@@ -4981,12 +4982,12 @@
         <v>26</v>
       </c>
       <c r="Q85" s="8" t="s">
-        <v>168</v>
+        <v>80</v>
       </c>
     </row>
     <row r="86" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A86" s="63" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="J86" s="48">
         <v>26</v>
@@ -4995,19 +4996,19 @@
         <v>26</v>
       </c>
       <c r="L86" s="39" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="M86" s="39"/>
       <c r="N86" s="39"/>
       <c r="O86" s="39"/>
       <c r="P86" s="39"/>
       <c r="Q86" s="8" t="s">
-        <v>87</v>
+        <v>170</v>
       </c>
     </row>
     <row r="87" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A87" s="62" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J87" s="48">
         <v>27</v>
@@ -5016,14 +5017,14 @@
         <v>27</v>
       </c>
       <c r="L87" s="39" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="M87" s="39"/>
       <c r="N87" s="39"/>
       <c r="O87" s="39"/>
       <c r="P87" s="39"/>
       <c r="Q87" s="8" t="s">
-        <v>169</v>
+        <v>85</v>
       </c>
     </row>
     <row r="88" spans="1:17" x14ac:dyDescent="0.2">
@@ -5034,14 +5035,14 @@
         <v>28</v>
       </c>
       <c r="L88" s="39" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M88" s="39"/>
       <c r="N88" s="39"/>
       <c r="O88" s="39"/>
       <c r="P88" s="39"/>
       <c r="Q88" s="8" t="s">
-        <v>86</v>
+        <v>169</v>
       </c>
     </row>
     <row r="89" spans="1:17" x14ac:dyDescent="0.2">
@@ -5052,14 +5053,14 @@
         <v>29</v>
       </c>
       <c r="L89" s="39" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="M89" s="39"/>
       <c r="N89" s="39"/>
       <c r="O89" s="39"/>
       <c r="P89" s="39"/>
       <c r="Q89" s="8" t="s">
-        <v>170</v>
+        <v>86</v>
       </c>
     </row>
     <row r="90" spans="1:17" x14ac:dyDescent="0.2">
@@ -5070,14 +5071,14 @@
         <v>30</v>
       </c>
       <c r="L90" s="39" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="M90" s="39"/>
       <c r="N90" s="39"/>
       <c r="O90" s="39"/>
       <c r="P90" s="39"/>
       <c r="Q90" s="8" t="s">
-        <v>85</v>
+        <v>168</v>
       </c>
     </row>
     <row r="91" spans="1:17" x14ac:dyDescent="0.2">
@@ -5088,14 +5089,14 @@
         <v>31</v>
       </c>
       <c r="L91" s="39" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="M91" s="39"/>
       <c r="N91" s="39"/>
       <c r="O91" s="39"/>
       <c r="P91" s="39"/>
       <c r="Q91" s="8" t="s">
-        <v>171</v>
+        <v>87</v>
       </c>
     </row>
     <row r="92" spans="1:17" x14ac:dyDescent="0.2">
@@ -5115,7 +5116,7 @@
         <v>26</v>
       </c>
       <c r="Q92" s="8" t="s">
-        <v>80</v>
+        <v>167</v>
       </c>
     </row>
     <row r="93" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -5133,17 +5134,17 @@
         <v>26</v>
       </c>
       <c r="Q93" s="8" t="s">
-        <v>172</v>
+        <v>88</v>
       </c>
     </row>
     <row r="94" spans="1:17" x14ac:dyDescent="0.2">
       <c r="H94" s="45" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="95" spans="1:17" x14ac:dyDescent="0.2">
       <c r="H95" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="M95"/>
     </row>
@@ -5154,12 +5155,12 @@
     </row>
     <row r="97" spans="8:13" x14ac:dyDescent="0.2">
       <c r="H97" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="98" spans="8:13" x14ac:dyDescent="0.2">
       <c r="H98" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="99" spans="8:13" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Update footprint mounting holes TFT, LED array, battery packs, lipo charger, arrange components to fit on the board
</commit_message>
<xml_diff>
--- a/Electronic Design/Core 64 Pin Usage Mapping.xlsx
+++ b/Electronic Design/Core 64 Pin Usage Mapping.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ageppert/Dropbox/Electronics/Core 64 Interactive Badge/Core-64-Interactive-Core-Memory-Badge/Electronic Design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F9624A3-5A94-E340-BCD8-DAFA5D10E093}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67204BDF-80EB-6548-9880-85FD848AEED0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16500" yWindow="460" windowWidth="34700" windowHeight="27480" activeTab="1" xr2:uid="{A4752792-CA31-B046-B883-84F8D68A57EC}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="219">
   <si>
     <t>Custom</t>
   </si>
@@ -579,9 +579,6 @@
     <t>Teensy View CS (default)</t>
   </si>
   <si>
-    <t>IR MODULATOR</t>
-  </si>
-  <si>
     <t>SPI SCK (default)</t>
   </si>
   <si>
@@ -688,6 +685,12 @@
   </si>
   <si>
     <t>TFT RESET, Teensy View Reset</t>
+  </si>
+  <si>
+    <t>IR MODULATOR OUT</t>
+  </si>
+  <si>
+    <t>IR MODULATOR IN</t>
   </si>
 </sst>
 </file>
@@ -2429,8 +2432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CBC2977-27CE-C64F-BE79-A69FB2535F84}">
   <dimension ref="A1:AD99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C38" zoomScale="117" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D55" sqref="D55"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="117" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E63" sqref="E63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3095,12 +3098,12 @@
     </row>
     <row r="25" spans="1:30" x14ac:dyDescent="0.2">
       <c r="H25" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="26" spans="1:30" x14ac:dyDescent="0.2">
       <c r="H26" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="27" spans="1:30" x14ac:dyDescent="0.2">
@@ -4042,7 +4045,7 @@
     </row>
     <row r="53" spans="1:30" x14ac:dyDescent="0.2">
       <c r="H53" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I53" s="10"/>
       <c r="W53" s="26"/>
@@ -4056,7 +4059,7 @@
     </row>
     <row r="54" spans="1:30" x14ac:dyDescent="0.2">
       <c r="H54" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I54" s="10"/>
       <c r="W54" s="59"/>
@@ -4113,13 +4116,13 @@
       <c r="B58" s="22"/>
       <c r="H58" s="57"/>
       <c r="I58" s="58" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J58" s="57"/>
     </row>
     <row r="59" spans="1:30" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B59" s="14" t="s">
         <v>98</v>
@@ -4202,15 +4205,15 @@
       <c r="O60" s="25"/>
       <c r="P60" s="25"/>
       <c r="Q60" s="36" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="61" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A61" s="8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C61" s="14" t="s">
         <v>26</v>
@@ -4240,10 +4243,10 @@
     </row>
     <row r="62" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A62" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C62" s="14" t="s">
         <v>26</v>
@@ -4268,7 +4271,7 @@
       <c r="O62" s="25"/>
       <c r="P62" s="25"/>
       <c r="Q62" s="24" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="63" spans="1:30" x14ac:dyDescent="0.2">
@@ -4352,7 +4355,7 @@
         <v>163</v>
       </c>
       <c r="B65" s="60" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D65" s="14" t="s">
         <v>2</v>
@@ -4399,7 +4402,7 @@
         <v>179</v>
       </c>
       <c r="C66" s="14" t="s">
-        <v>181</v>
+        <v>217</v>
       </c>
       <c r="D66" s="14" t="s">
         <v>2</v>
@@ -4569,7 +4572,7 @@
         <v>110</v>
       </c>
       <c r="R69" s="52" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="70" spans="1:21" x14ac:dyDescent="0.2">
@@ -4612,15 +4615,18 @@
         <v>26</v>
       </c>
       <c r="Q70" s="8" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="71" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A71" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B71" s="56" t="s">
         <v>180</v>
+      </c>
+      <c r="C71" s="14" t="s">
+        <v>218</v>
       </c>
       <c r="D71" s="14" t="s">
         <v>2</v>
@@ -4654,15 +4660,15 @@
         <v>26</v>
       </c>
       <c r="Q71" s="8" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="R71" s="56" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="72" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A72" s="51" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E72" s="14" t="s">
         <v>113</v>
@@ -4688,12 +4694,12 @@
       <c r="O72" s="39"/>
       <c r="P72" s="39"/>
       <c r="Q72" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="73" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A73" s="51" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B73" s="14"/>
       <c r="E73" s="14" t="s">
@@ -4720,7 +4726,7 @@
       <c r="O73" s="39"/>
       <c r="P73" s="39"/>
       <c r="Q73" s="51" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="R73" s="8" t="s">
         <v>172</v>
@@ -4766,7 +4772,7 @@
       <c r="O75" s="39"/>
       <c r="P75" s="39"/>
       <c r="Q75" s="8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="76" spans="1:21" x14ac:dyDescent="0.2">
@@ -4795,7 +4801,7 @@
       <c r="O76" s="39"/>
       <c r="P76" s="39"/>
       <c r="Q76" s="8" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="77" spans="1:21" x14ac:dyDescent="0.2">
@@ -4829,7 +4835,7 @@
     </row>
     <row r="78" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A78" s="15" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B78" s="15"/>
       <c r="G78" s="14" t="s">
@@ -4851,7 +4857,7 @@
       <c r="O78" s="25"/>
       <c r="P78" s="25"/>
       <c r="Q78" s="24" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="79" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -4885,7 +4891,7 @@
       <c r="O80" s="39"/>
       <c r="P80" s="39"/>
       <c r="Q80" s="8" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="81" spans="1:17" x14ac:dyDescent="0.2">
@@ -4901,12 +4907,12 @@
       <c r="O81" s="39"/>
       <c r="P81" s="39"/>
       <c r="Q81" s="8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="82" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A82" s="65" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J82" s="49" t="s">
         <v>4</v>
@@ -4923,7 +4929,7 @@
     </row>
     <row r="83" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A83" s="64" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J83" s="41" t="s">
         <v>6</v>
@@ -4932,7 +4938,7 @@
     </row>
     <row r="84" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A84" s="61" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J84" s="48">
         <v>24</v>
@@ -4951,7 +4957,7 @@
     </row>
     <row r="85" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A85" s="61" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J85" s="48">
         <v>25</v>
@@ -4974,7 +4980,7 @@
     </row>
     <row r="86" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A86" s="63" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J86" s="48">
         <v>26</v>
@@ -4995,7 +5001,7 @@
     </row>
     <row r="87" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A87" s="62" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="J87" s="48">
         <v>27</v>
@@ -5126,12 +5132,12 @@
     </row>
     <row r="94" spans="1:17" x14ac:dyDescent="0.2">
       <c r="H94" s="45" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="95" spans="1:17" x14ac:dyDescent="0.2">
       <c r="H95" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M95"/>
     </row>
@@ -5142,12 +5148,12 @@
     </row>
     <row r="97" spans="8:13" x14ac:dyDescent="0.2">
       <c r="H97" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="98" spans="8:13" x14ac:dyDescent="0.2">
       <c r="H98" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="99" spans="8:13" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Review and tweak Logic Board (LB) schematic, pin usage
</commit_message>
<xml_diff>
--- a/Electronic Design/Core 64 Pin Usage Mapping.xlsx
+++ b/Electronic Design/Core 64 Pin Usage Mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ageppert/Dropbox/Electronics/Core 64 Interactive Badge/Core-64-Interactive-Core-Memory-Badge/Electronic Design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67204BDF-80EB-6548-9880-85FD848AEED0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{193C3B5F-2F9F-8649-928C-FE3277251463}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16500" yWindow="460" windowWidth="34700" windowHeight="27480" activeTab="1" xr2:uid="{A4752792-CA31-B046-B883-84F8D68A57EC}"/>
+    <workbookView xWindow="3700" yWindow="1080" windowWidth="34700" windowHeight="22680" activeTab="1" xr2:uid="{A4752792-CA31-B046-B883-84F8D68A57EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Reference Pinouts" sheetId="3" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="220">
   <si>
     <t>Custom</t>
   </si>
@@ -567,12 +567,6 @@
     <t>OLED Data/control</t>
   </si>
   <si>
-    <t>Spare SPI CS</t>
-  </si>
-  <si>
-    <t>Spare SPI Data/Control</t>
-  </si>
-  <si>
     <t>Teensy View Data/control (default)</t>
   </si>
   <si>
@@ -691,6 +685,15 @@
   </si>
   <si>
     <t>IR MODULATOR IN</t>
+  </si>
+  <si>
+    <t>OLED</t>
+  </si>
+  <si>
+    <t>Board ID</t>
+  </si>
+  <si>
+    <t>SPARE 8 ANALOG (or pseudo digital input)</t>
   </si>
 </sst>
 </file>
@@ -799,7 +802,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -863,6 +866,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -997,7 +1006,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1097,9 +1106,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1157,6 +1163,29 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2432,8 +2461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CBC2977-27CE-C64F-BE79-A69FB2535F84}">
   <dimension ref="A1:AD99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="117" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E63" sqref="E63"/>
+    <sheetView tabSelected="1" topLeftCell="B58" zoomScale="117" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="L91" sqref="L91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3092,18 +3121,18 @@
       </c>
     </row>
     <row r="24" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="H24" s="45" t="s">
+      <c r="H24" s="44" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="25" spans="1:30" x14ac:dyDescent="0.2">
       <c r="H25" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="26" spans="1:30" x14ac:dyDescent="0.2">
       <c r="H26" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="27" spans="1:30" x14ac:dyDescent="0.2">
@@ -3220,13 +3249,13 @@
       <c r="Q32" s="36" t="s">
         <v>100</v>
       </c>
-      <c r="W32" s="66"/>
-      <c r="X32" s="66"/>
-      <c r="Y32" s="66"/>
-      <c r="Z32" s="66"/>
-      <c r="AA32" s="66"/>
-      <c r="AB32" s="66"/>
-      <c r="AC32" s="66"/>
+      <c r="W32" s="65"/>
+      <c r="X32" s="65"/>
+      <c r="Y32" s="65"/>
+      <c r="Z32" s="65"/>
+      <c r="AA32" s="65"/>
+      <c r="AB32" s="65"/>
+      <c r="AC32" s="65"/>
       <c r="AD32" s="9"/>
     </row>
     <row r="33" spans="1:30" x14ac:dyDescent="0.2">
@@ -3906,16 +3935,16 @@
       <c r="G48" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="H48" s="44" t="s">
+      <c r="H48" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="I48" s="43" t="s">
+      <c r="I48" s="42" t="s">
         <v>124</v>
       </c>
-      <c r="J48" s="42">
+      <c r="J48" s="41">
         <v>24</v>
       </c>
-      <c r="K48" s="43">
+      <c r="K48" s="42">
         <v>24</v>
       </c>
       <c r="L48" s="26" t="s">
@@ -3943,16 +3972,16 @@
       <c r="G49" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="H49" s="44" t="s">
+      <c r="H49" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="I49" s="43" t="s">
+      <c r="I49" s="42" t="s">
         <v>125</v>
       </c>
-      <c r="J49" s="42">
+      <c r="J49" s="41">
         <v>25</v>
       </c>
-      <c r="K49" s="43">
+      <c r="K49" s="42">
         <v>25</v>
       </c>
       <c r="L49" s="26" t="s">
@@ -3978,10 +4007,10 @@
       <c r="G50" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="H50" s="44" t="s">
+      <c r="H50" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="I50" s="43" t="s">
+      <c r="I50" s="42" t="s">
         <v>126</v>
       </c>
       <c r="J50" s="40" t="s">
@@ -4031,7 +4060,7 @@
     </row>
     <row r="52" spans="1:30" x14ac:dyDescent="0.2">
       <c r="G52" s="7"/>
-      <c r="H52" s="45" t="s">
+      <c r="H52" s="44" t="s">
         <v>132</v>
       </c>
       <c r="W52" s="26"/>
@@ -4045,7 +4074,7 @@
     </row>
     <row r="53" spans="1:30" x14ac:dyDescent="0.2">
       <c r="H53" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="I53" s="10"/>
       <c r="W53" s="26"/>
@@ -4059,11 +4088,11 @@
     </row>
     <row r="54" spans="1:30" x14ac:dyDescent="0.2">
       <c r="H54" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="I54" s="10"/>
-      <c r="W54" s="59"/>
-      <c r="X54" s="59"/>
+      <c r="W54" s="58"/>
+      <c r="X54" s="58"/>
       <c r="Y54" s="9"/>
       <c r="Z54" s="9"/>
       <c r="AA54" s="9"/>
@@ -4076,8 +4105,8 @@
         <v>89</v>
       </c>
       <c r="I55" s="10"/>
-      <c r="W55" s="59"/>
-      <c r="X55" s="59"/>
+      <c r="W55" s="58"/>
+      <c r="X55" s="58"/>
       <c r="Y55" s="9"/>
       <c r="Z55" s="9"/>
       <c r="AA55" s="9"/>
@@ -4087,8 +4116,8 @@
     </row>
     <row r="56" spans="1:30" x14ac:dyDescent="0.2">
       <c r="I56" s="10"/>
-      <c r="W56" s="59"/>
-      <c r="X56" s="59"/>
+      <c r="W56" s="58"/>
+      <c r="X56" s="58"/>
       <c r="Y56" s="9"/>
       <c r="Z56" s="9"/>
       <c r="AA56" s="9"/>
@@ -4114,15 +4143,15 @@
         <v>91</v>
       </c>
       <c r="B58" s="22"/>
-      <c r="H58" s="57"/>
-      <c r="I58" s="58" t="s">
-        <v>196</v>
-      </c>
-      <c r="J58" s="57"/>
+      <c r="H58" s="56"/>
+      <c r="I58" s="57" t="s">
+        <v>194</v>
+      </c>
+      <c r="J58" s="56"/>
     </row>
     <row r="59" spans="1:30" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B59" s="14" t="s">
         <v>98</v>
@@ -4195,25 +4224,25 @@
       <c r="H60" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="J60" s="34" t="s">
+      <c r="J60" s="66" t="s">
         <v>141</v>
       </c>
-      <c r="K60" s="35"/>
-      <c r="L60" s="25"/>
-      <c r="M60" s="25"/>
-      <c r="N60" s="25"/>
-      <c r="O60" s="25"/>
-      <c r="P60" s="25"/>
-      <c r="Q60" s="36" t="s">
-        <v>184</v>
+      <c r="K60" s="67"/>
+      <c r="L60" s="68"/>
+      <c r="M60" s="68"/>
+      <c r="N60" s="68"/>
+      <c r="O60" s="68"/>
+      <c r="P60" s="68"/>
+      <c r="Q60" s="69" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="61" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A61" s="8" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C61" s="14" t="s">
         <v>26</v>
@@ -4243,10 +4272,10 @@
     </row>
     <row r="62" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A62" s="8" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C62" s="14" t="s">
         <v>26</v>
@@ -4271,14 +4300,14 @@
       <c r="O62" s="25"/>
       <c r="P62" s="25"/>
       <c r="Q62" s="24" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="63" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A63" s="8" t="s">
         <v>162</v>
       </c>
-      <c r="B63" s="56" t="s">
+      <c r="B63" s="55" t="s">
         <v>175</v>
       </c>
       <c r="G63" s="14">
@@ -4313,7 +4342,7 @@
       <c r="A64" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="B64" s="56" t="s">
+      <c r="B64" s="55" t="s">
         <v>176</v>
       </c>
       <c r="D64" s="14" t="s">
@@ -4354,8 +4383,8 @@
       <c r="A65" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="B65" s="60" t="s">
-        <v>187</v>
+      <c r="B65" s="59" t="s">
+        <v>185</v>
       </c>
       <c r="D65" s="14" t="s">
         <v>2</v>
@@ -4388,21 +4417,18 @@
       </c>
       <c r="P65" s="39"/>
       <c r="Q65" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="R65" s="39" t="s">
-        <v>178</v>
+        <v>202</v>
       </c>
     </row>
     <row r="66" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A66" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B66" s="56" t="s">
-        <v>179</v>
+      <c r="B66" s="55" t="s">
+        <v>177</v>
       </c>
       <c r="C66" s="14" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D66" s="14" t="s">
         <v>2</v>
@@ -4432,17 +4458,17 @@
       </c>
       <c r="P66" s="39"/>
       <c r="Q66" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="R66" s="39" t="s">
-        <v>177</v>
+        <v>110</v>
+      </c>
+      <c r="R66" s="51" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="67" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A67" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="B67" s="53" t="s">
+      <c r="B67" s="52" t="s">
         <v>153</v>
       </c>
       <c r="D67" s="14" t="s">
@@ -4476,7 +4502,7 @@
         <v>149</v>
       </c>
       <c r="R67" s="8" t="s">
-        <v>101</v>
+        <v>217</v>
       </c>
       <c r="S67" s="8" t="s">
         <v>106</v>
@@ -4484,7 +4510,9 @@
       <c r="T67" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="U67" s="8"/>
+      <c r="U67" s="8" t="s">
+        <v>218</v>
+      </c>
     </row>
     <row r="68" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A68" s="8" t="s">
@@ -4522,7 +4550,7 @@
         <v>149</v>
       </c>
       <c r="R68" s="8" t="s">
-        <v>101</v>
+        <v>217</v>
       </c>
       <c r="S68" s="8" t="s">
         <v>106</v>
@@ -4530,13 +4558,15 @@
       <c r="T68" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="U68" s="8"/>
+      <c r="U68" s="8" t="s">
+        <v>218</v>
+      </c>
     </row>
     <row r="69" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A69" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="B69" s="55" t="s">
+      <c r="B69" s="54" t="s">
         <v>173</v>
       </c>
       <c r="F69" s="14" t="s">
@@ -4558,7 +4588,7 @@
       <c r="L69" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="M69" s="46" t="s">
+      <c r="M69" s="45" t="s">
         <v>39</v>
       </c>
       <c r="N69" s="39"/>
@@ -4569,17 +4599,14 @@
         <v>26</v>
       </c>
       <c r="Q69" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="R69" s="52" t="s">
-        <v>201</v>
+        <v>78</v>
       </c>
     </row>
     <row r="70" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A70" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="B70" s="55" t="s">
+      <c r="B70" s="54" t="s">
         <v>174</v>
       </c>
       <c r="D70" s="14" t="s">
@@ -4604,7 +4631,7 @@
       <c r="L70" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="M70" s="46" t="s">
+      <c r="M70" s="45" t="s">
         <v>40</v>
       </c>
       <c r="N70" s="39"/>
@@ -4615,18 +4642,18 @@
         <v>26</v>
       </c>
       <c r="Q70" s="8" t="s">
-        <v>204</v>
+        <v>166</v>
       </c>
     </row>
     <row r="71" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A71" s="8" t="s">
-        <v>210</v>
-      </c>
-      <c r="B71" s="56" t="s">
-        <v>180</v>
+        <v>208</v>
+      </c>
+      <c r="B71" s="55" t="s">
+        <v>178</v>
       </c>
       <c r="C71" s="14" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D71" s="14" t="s">
         <v>2</v>
@@ -4660,15 +4687,15 @@
         <v>26</v>
       </c>
       <c r="Q71" s="8" t="s">
-        <v>202</v>
-      </c>
-      <c r="R71" s="56" t="s">
-        <v>216</v>
+        <v>200</v>
+      </c>
+      <c r="R71" s="55" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="72" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A72" s="51" t="s">
-        <v>206</v>
+      <c r="A72" s="50" t="s">
+        <v>204</v>
       </c>
       <c r="E72" s="14" t="s">
         <v>113</v>
@@ -4694,12 +4721,12 @@
       <c r="O72" s="39"/>
       <c r="P72" s="39"/>
       <c r="Q72" s="8" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="73" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A73" s="51" t="s">
-        <v>207</v>
+      <c r="A73" s="50" t="s">
+        <v>205</v>
       </c>
       <c r="B73" s="14"/>
       <c r="E73" s="14" t="s">
@@ -4725,8 +4752,8 @@
       </c>
       <c r="O73" s="39"/>
       <c r="P73" s="39"/>
-      <c r="Q73" s="51" t="s">
-        <v>181</v>
+      <c r="Q73" s="50" t="s">
+        <v>179</v>
       </c>
       <c r="R73" s="8" t="s">
         <v>172</v>
@@ -4772,7 +4799,7 @@
       <c r="O75" s="39"/>
       <c r="P75" s="39"/>
       <c r="Q75" s="8" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="76" spans="1:21" x14ac:dyDescent="0.2">
@@ -4783,10 +4810,10 @@
       <c r="G76" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="H76" s="44" t="s">
+      <c r="H76" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="I76" s="43" t="s">
+      <c r="I76" s="42" t="s">
         <v>124</v>
       </c>
       <c r="J76" s="37" t="s">
@@ -4801,7 +4828,7 @@
       <c r="O76" s="39"/>
       <c r="P76" s="39"/>
       <c r="Q76" s="8" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="77" spans="1:21" x14ac:dyDescent="0.2">
@@ -4812,10 +4839,10 @@
       <c r="G77" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="H77" s="44" t="s">
+      <c r="H77" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="I77" s="43" t="s">
+      <c r="I77" s="42" t="s">
         <v>125</v>
       </c>
       <c r="J77" s="37" t="s">
@@ -4829,35 +4856,38 @@
       <c r="N77" s="39"/>
       <c r="O77" s="39"/>
       <c r="P77" s="39"/>
-      <c r="Q77" s="54" t="s">
+      <c r="Q77" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="R77" s="53" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="78" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A78" s="15" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B78" s="15"/>
       <c r="G78" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="H78" s="44" t="s">
+      <c r="H78" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="I78" s="43" t="s">
+      <c r="I78" s="42" t="s">
         <v>126</v>
       </c>
-      <c r="J78" s="40" t="s">
+      <c r="J78" s="70" t="s">
         <v>66</v>
       </c>
-      <c r="K78" s="35"/>
-      <c r="L78" s="25"/>
-      <c r="M78" s="25"/>
-      <c r="N78" s="25"/>
-      <c r="O78" s="25"/>
-      <c r="P78" s="25"/>
-      <c r="Q78" s="24" t="s">
-        <v>185</v>
+      <c r="K78" s="71"/>
+      <c r="L78" s="72"/>
+      <c r="M78" s="72"/>
+      <c r="N78" s="72"/>
+      <c r="O78" s="72"/>
+      <c r="P78" s="72"/>
+      <c r="Q78" s="73" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="79" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -4879,7 +4909,7 @@
       </c>
     </row>
     <row r="80" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="J80" s="47" t="s">
+      <c r="J80" s="46" t="s">
         <v>121</v>
       </c>
       <c r="K80" s="39"/>
@@ -4891,11 +4921,11 @@
       <c r="O80" s="39"/>
       <c r="P80" s="39"/>
       <c r="Q80" s="8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="81" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="J81" s="48" t="s">
+      <c r="J81" s="47" t="s">
         <v>122</v>
       </c>
       <c r="K81" s="39"/>
@@ -4907,14 +4937,14 @@
       <c r="O81" s="39"/>
       <c r="P81" s="39"/>
       <c r="Q81" s="8" t="s">
-        <v>209</v>
+        <v>219</v>
       </c>
     </row>
     <row r="82" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A82" s="65" t="s">
-        <v>189</v>
-      </c>
-      <c r="J82" s="49" t="s">
+      <c r="A82" s="64" t="s">
+        <v>187</v>
+      </c>
+      <c r="J82" s="48" t="s">
         <v>4</v>
       </c>
       <c r="K82" s="32"/>
@@ -4928,19 +4958,25 @@
       </c>
     </row>
     <row r="83" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A83" s="64" t="s">
+      <c r="A83" s="63" t="s">
+        <v>186</v>
+      </c>
+      <c r="J83" s="74" t="s">
+        <v>6</v>
+      </c>
+      <c r="K83" s="68"/>
+      <c r="L83" s="68"/>
+      <c r="M83" s="68"/>
+      <c r="N83" s="68"/>
+      <c r="O83" s="68"/>
+      <c r="P83" s="68"/>
+      <c r="Q83" s="55"/>
+    </row>
+    <row r="84" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A84" s="60" t="s">
         <v>188</v>
       </c>
-      <c r="J83" s="41" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q83" s="15"/>
-    </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A84" s="61" t="s">
-        <v>190</v>
-      </c>
-      <c r="J84" s="48">
+      <c r="J84" s="47">
         <v>24</v>
       </c>
       <c r="K84" s="39">
@@ -4956,10 +4992,10 @@
       </c>
     </row>
     <row r="85" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A85" s="61" t="s">
-        <v>193</v>
-      </c>
-      <c r="J85" s="48">
+      <c r="A85" s="60" t="s">
+        <v>191</v>
+      </c>
+      <c r="J85" s="47">
         <v>25</v>
       </c>
       <c r="K85" s="39">
@@ -4979,10 +5015,10 @@
       </c>
     </row>
     <row r="86" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A86" s="63" t="s">
-        <v>191</v>
-      </c>
-      <c r="J86" s="48">
+      <c r="A86" s="62" t="s">
+        <v>189</v>
+      </c>
+      <c r="J86" s="47">
         <v>26</v>
       </c>
       <c r="K86" s="39">
@@ -5000,10 +5036,10 @@
       </c>
     </row>
     <row r="87" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A87" s="62" t="s">
-        <v>192</v>
-      </c>
-      <c r="J87" s="48">
+      <c r="A87" s="61" t="s">
+        <v>190</v>
+      </c>
+      <c r="J87" s="47">
         <v>27</v>
       </c>
       <c r="K87" s="39">
@@ -5021,7 +5057,7 @@
       </c>
     </row>
     <row r="88" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="J88" s="48">
+      <c r="J88" s="47">
         <v>28</v>
       </c>
       <c r="K88" s="39">
@@ -5039,7 +5075,7 @@
       </c>
     </row>
     <row r="89" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="J89" s="48">
+      <c r="J89" s="47">
         <v>29</v>
       </c>
       <c r="K89" s="39">
@@ -5057,7 +5093,7 @@
       </c>
     </row>
     <row r="90" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="J90" s="48">
+      <c r="J90" s="47">
         <v>30</v>
       </c>
       <c r="K90" s="39">
@@ -5075,7 +5111,7 @@
       </c>
     </row>
     <row r="91" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="J91" s="48">
+      <c r="J91" s="47">
         <v>31</v>
       </c>
       <c r="K91" s="39">
@@ -5093,7 +5129,7 @@
       </c>
     </row>
     <row r="92" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="J92" s="48">
+      <c r="J92" s="47">
         <v>32</v>
       </c>
       <c r="K92" s="39">
@@ -5113,7 +5149,7 @@
       </c>
     </row>
     <row r="93" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J93" s="50">
+      <c r="J93" s="49">
         <v>33</v>
       </c>
       <c r="K93" s="39">
@@ -5131,13 +5167,13 @@
       </c>
     </row>
     <row r="94" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="H94" s="45" t="s">
-        <v>197</v>
+      <c r="H94" s="44" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="95" spans="1:17" x14ac:dyDescent="0.2">
       <c r="H95" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="M95"/>
     </row>
@@ -5148,12 +5184,12 @@
     </row>
     <row r="97" spans="8:13" x14ac:dyDescent="0.2">
       <c r="H97" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="98" spans="8:13" x14ac:dyDescent="0.2">
       <c r="H98" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="99" spans="8:13" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Review and test SPI pins with Teensy 3.2
Move Q5P/N, BACKLIGHT to PWM, Sense Reset by Sense Pulse and Enable, move SPI CS/DC pins that didn't work with ILI9341_t3n
</commit_message>
<xml_diff>
--- a/Electronic Design/Core 64 Pin Usage Mapping.xlsx
+++ b/Electronic Design/Core 64 Pin Usage Mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ageppert/Dropbox/Electronics/Core 64 Interactive Badge/Core-64-Interactive-Core-Memory-Badge/Electronic Design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{193C3B5F-2F9F-8649-928C-FE3277251463}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBFCB118-1C89-D044-A932-E70EBE9CA181}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3700" yWindow="1080" windowWidth="34700" windowHeight="22680" activeTab="1" xr2:uid="{A4752792-CA31-B046-B883-84F8D68A57EC}"/>
+    <workbookView xWindow="8220" yWindow="3800" windowWidth="40360" windowHeight="22680" activeTab="1" xr2:uid="{A4752792-CA31-B046-B883-84F8D68A57EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Reference Pinouts" sheetId="3" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="221">
   <si>
     <t>Custom</t>
   </si>
@@ -567,9 +567,6 @@
     <t>OLED Data/control</t>
   </si>
   <si>
-    <t>Teensy View Data/control (default)</t>
-  </si>
-  <si>
     <t>Teensy View CS (default)</t>
   </si>
   <si>
@@ -588,9 +585,6 @@
     <t>TEENSY_VUSB supply to Core64 Power Switch SPDT</t>
   </si>
   <si>
-    <t>Unused</t>
-  </si>
-  <si>
     <t>TOUCH_CS</t>
   </si>
   <si>
@@ -694,6 +688,15 @@
   </si>
   <si>
     <t>SPARE 8 ANALOG (or pseudo digital input)</t>
+  </si>
+  <si>
+    <t>CR2032 RTC</t>
+  </si>
+  <si>
+    <t>Program, 10K to 3.3V pull-up</t>
+  </si>
+  <si>
+    <t>Teensy View Data/control (alternate)</t>
   </si>
 </sst>
 </file>
@@ -1162,9 +1165,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1186,6 +1186,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2461,8 +2464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CBC2977-27CE-C64F-BE79-A69FB2535F84}">
   <dimension ref="A1:AD99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B58" zoomScale="117" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="L91" sqref="L91"/>
+    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="117" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B82" sqref="B82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3127,12 +3130,12 @@
     </row>
     <row r="25" spans="1:30" x14ac:dyDescent="0.2">
       <c r="H25" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="26" spans="1:30" x14ac:dyDescent="0.2">
       <c r="H26" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="27" spans="1:30" x14ac:dyDescent="0.2">
@@ -3249,13 +3252,13 @@
       <c r="Q32" s="36" t="s">
         <v>100</v>
       </c>
-      <c r="W32" s="65"/>
-      <c r="X32" s="65"/>
-      <c r="Y32" s="65"/>
-      <c r="Z32" s="65"/>
-      <c r="AA32" s="65"/>
-      <c r="AB32" s="65"/>
-      <c r="AC32" s="65"/>
+      <c r="W32" s="74"/>
+      <c r="X32" s="74"/>
+      <c r="Y32" s="74"/>
+      <c r="Z32" s="74"/>
+      <c r="AA32" s="74"/>
+      <c r="AB32" s="74"/>
+      <c r="AC32" s="74"/>
       <c r="AD32" s="9"/>
     </row>
     <row r="33" spans="1:30" x14ac:dyDescent="0.2">
@@ -4074,7 +4077,7 @@
     </row>
     <row r="53" spans="1:30" x14ac:dyDescent="0.2">
       <c r="H53" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="I53" s="10"/>
       <c r="W53" s="26"/>
@@ -4088,7 +4091,7 @@
     </row>
     <row r="54" spans="1:30" x14ac:dyDescent="0.2">
       <c r="H54" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="I54" s="10"/>
       <c r="W54" s="58"/>
@@ -4145,13 +4148,13 @@
       <c r="B58" s="22"/>
       <c r="H58" s="56"/>
       <c r="I58" s="57" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="J58" s="56"/>
     </row>
     <row r="59" spans="1:30" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B59" s="14" t="s">
         <v>98</v>
@@ -4224,25 +4227,25 @@
       <c r="H60" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="J60" s="66" t="s">
+      <c r="J60" s="65" t="s">
         <v>141</v>
       </c>
-      <c r="K60" s="67"/>
-      <c r="L60" s="68"/>
-      <c r="M60" s="68"/>
-      <c r="N60" s="68"/>
-      <c r="O60" s="68"/>
-      <c r="P60" s="68"/>
-      <c r="Q60" s="69" t="s">
-        <v>182</v>
+      <c r="K60" s="66"/>
+      <c r="L60" s="67"/>
+      <c r="M60" s="67"/>
+      <c r="N60" s="67"/>
+      <c r="O60" s="67"/>
+      <c r="P60" s="67"/>
+      <c r="Q60" s="68" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="61" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A61" s="8" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C61" s="14" t="s">
         <v>26</v>
@@ -4272,10 +4275,10 @@
     </row>
     <row r="62" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A62" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C62" s="14" t="s">
         <v>26</v>
@@ -4300,7 +4303,7 @@
       <c r="O62" s="25"/>
       <c r="P62" s="25"/>
       <c r="Q62" s="24" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="63" spans="1:30" x14ac:dyDescent="0.2">
@@ -4337,13 +4340,13 @@
       <c r="Q63" s="8" t="s">
         <v>53</v>
       </c>
+      <c r="R63" s="55" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="64" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A64" s="8" t="s">
         <v>70</v>
-      </c>
-      <c r="B64" s="55" t="s">
-        <v>176</v>
       </c>
       <c r="D64" s="14" t="s">
         <v>2</v>
@@ -4384,7 +4387,7 @@
         <v>163</v>
       </c>
       <c r="B65" s="59" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D65" s="14" t="s">
         <v>2</v>
@@ -4417,18 +4420,18 @@
       </c>
       <c r="P65" s="39"/>
       <c r="Q65" s="8" t="s">
-        <v>202</v>
+        <v>200</v>
+      </c>
+      <c r="R65" s="55" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="66" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A66" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B66" s="55" t="s">
-        <v>177</v>
-      </c>
       <c r="C66" s="14" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D66" s="14" t="s">
         <v>2</v>
@@ -4461,7 +4464,7 @@
         <v>110</v>
       </c>
       <c r="R66" s="51" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="67" spans="1:21" x14ac:dyDescent="0.2">
@@ -4502,7 +4505,7 @@
         <v>149</v>
       </c>
       <c r="R67" s="8" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="S67" s="8" t="s">
         <v>106</v>
@@ -4511,7 +4514,7 @@
         <v>154</v>
       </c>
       <c r="U67" s="8" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="68" spans="1:21" x14ac:dyDescent="0.2">
@@ -4550,7 +4553,7 @@
         <v>149</v>
       </c>
       <c r="R68" s="8" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="S68" s="8" t="s">
         <v>106</v>
@@ -4559,7 +4562,7 @@
         <v>154</v>
       </c>
       <c r="U68" s="8" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="69" spans="1:21" x14ac:dyDescent="0.2">
@@ -4647,13 +4650,13 @@
     </row>
     <row r="71" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A71" s="8" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B71" s="55" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C71" s="14" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D71" s="14" t="s">
         <v>2</v>
@@ -4687,15 +4690,15 @@
         <v>26</v>
       </c>
       <c r="Q71" s="8" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="R71" s="55" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="72" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A72" s="50" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E72" s="14" t="s">
         <v>113</v>
@@ -4721,12 +4724,12 @@
       <c r="O72" s="39"/>
       <c r="P72" s="39"/>
       <c r="Q72" s="8" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="73" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A73" s="50" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B73" s="14"/>
       <c r="E73" s="14" t="s">
@@ -4753,7 +4756,7 @@
       <c r="O73" s="39"/>
       <c r="P73" s="39"/>
       <c r="Q73" s="50" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="R73" s="8" t="s">
         <v>172</v>
@@ -4778,9 +4781,9 @@
     </row>
     <row r="75" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A75" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="B75" s="15"/>
+        <v>218</v>
+      </c>
+      <c r="B75" s="9"/>
       <c r="G75" s="14" t="s">
         <v>51</v>
       </c>
@@ -4799,14 +4802,14 @@
       <c r="O75" s="39"/>
       <c r="P75" s="39"/>
       <c r="Q75" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="76" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A76" s="15" t="s">
-        <v>128</v>
-      </c>
-      <c r="B76" s="15"/>
+      <c r="A76" s="73" t="s">
+        <v>6</v>
+      </c>
+      <c r="B76" s="9"/>
       <c r="G76" s="14" t="s">
         <v>51</v>
       </c>
@@ -4828,14 +4831,14 @@
       <c r="O76" s="39"/>
       <c r="P76" s="39"/>
       <c r="Q76" s="8" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="77" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A77" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="B77" s="15"/>
+      <c r="A77" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="B77" s="9"/>
       <c r="G77" s="14" t="s">
         <v>51</v>
       </c>
@@ -4857,7 +4860,7 @@
       <c r="O77" s="39"/>
       <c r="P77" s="39"/>
       <c r="Q77" s="8" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="R77" s="53" t="s">
         <v>152</v>
@@ -4865,9 +4868,9 @@
     </row>
     <row r="78" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A78" s="15" t="s">
-        <v>184</v>
-      </c>
-      <c r="B78" s="15"/>
+        <v>219</v>
+      </c>
+      <c r="B78" s="9"/>
       <c r="G78" s="14" t="s">
         <v>51</v>
       </c>
@@ -4877,24 +4880,24 @@
       <c r="I78" s="42" t="s">
         <v>126</v>
       </c>
-      <c r="J78" s="70" t="s">
+      <c r="J78" s="69" t="s">
         <v>66</v>
       </c>
-      <c r="K78" s="71"/>
-      <c r="L78" s="72"/>
-      <c r="M78" s="72"/>
-      <c r="N78" s="72"/>
-      <c r="O78" s="72"/>
-      <c r="P78" s="72"/>
-      <c r="Q78" s="73" t="s">
-        <v>183</v>
+      <c r="K78" s="70"/>
+      <c r="L78" s="71"/>
+      <c r="M78" s="71"/>
+      <c r="N78" s="71"/>
+      <c r="O78" s="71"/>
+      <c r="P78" s="71"/>
+      <c r="Q78" s="72" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="79" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A79" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="B79" s="8"/>
+      <c r="B79" s="9"/>
       <c r="G79" s="14" t="s">
         <v>51</v>
       </c>
@@ -4921,7 +4924,7 @@
       <c r="O80" s="39"/>
       <c r="P80" s="39"/>
       <c r="Q80" s="8" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="81" spans="1:17" x14ac:dyDescent="0.2">
@@ -4937,12 +4940,12 @@
       <c r="O81" s="39"/>
       <c r="P81" s="39"/>
       <c r="Q81" s="8" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="82" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A82" s="64" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="J82" s="48" t="s">
         <v>4</v>
@@ -4959,22 +4962,22 @@
     </row>
     <row r="83" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A83" s="63" t="s">
-        <v>186</v>
-      </c>
-      <c r="J83" s="74" t="s">
+        <v>184</v>
+      </c>
+      <c r="J83" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="K83" s="68"/>
-      <c r="L83" s="68"/>
-      <c r="M83" s="68"/>
-      <c r="N83" s="68"/>
-      <c r="O83" s="68"/>
-      <c r="P83" s="68"/>
+      <c r="K83" s="67"/>
+      <c r="L83" s="67"/>
+      <c r="M83" s="67"/>
+      <c r="N83" s="67"/>
+      <c r="O83" s="67"/>
+      <c r="P83" s="67"/>
       <c r="Q83" s="55"/>
     </row>
     <row r="84" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A84" s="60" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="J84" s="47">
         <v>24</v>
@@ -4993,7 +4996,7 @@
     </row>
     <row r="85" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A85" s="60" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="J85" s="47">
         <v>25</v>
@@ -5016,7 +5019,7 @@
     </row>
     <row r="86" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A86" s="62" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="J86" s="47">
         <v>26</v>
@@ -5037,7 +5040,7 @@
     </row>
     <row r="87" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A87" s="61" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="J87" s="47">
         <v>27</v>
@@ -5168,12 +5171,12 @@
     </row>
     <row r="94" spans="1:17" x14ac:dyDescent="0.2">
       <c r="H94" s="44" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="95" spans="1:17" x14ac:dyDescent="0.2">
       <c r="H95" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="M95"/>
     </row>
@@ -5184,12 +5187,12 @@
     </row>
     <row r="97" spans="8:13" x14ac:dyDescent="0.2">
       <c r="H97" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="98" spans="8:13" x14ac:dyDescent="0.2">
       <c r="H98" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="99" spans="8:13" x14ac:dyDescent="0.2">

</xml_diff>